<commit_message>
feat：update tower excel change and levelEffect
新增表key值+新增升级特效表
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="261">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -76,16 +76,34 @@
     <t xml:space="preserve">guid</t>
   </si>
   <si>
+    <t xml:space="preserve">guid2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guid3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">characterDelayTime</t>
+  </si>
+  <si>
     <t xml:space="preserve">weaponGuid</t>
   </si>
   <si>
+    <t xml:space="preserve">weaponSlot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weaponLocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effectDelayTime</t>
+  </si>
+  <si>
     <t xml:space="preserve">attackEffect</t>
   </si>
   <si>
     <t xml:space="preserve">hitEffect</t>
   </si>
   <si>
-    <t xml:space="preserve">effectDelayTime</t>
+    <t xml:space="preserve">attackEffectDelay</t>
   </si>
   <si>
     <t xml:space="preserve">attackTime</t>
@@ -110,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">attackAnim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attackAnimNew</t>
   </si>
   <si>
     <t xml:space="preserve">AtkAnimDur</t>
@@ -167,7 +188,25 @@
     <t xml:space="preserve">塔每一级buff特效的guid</t>
   </si>
   <si>
+    <t xml:space="preserve">防御塔二级特效guid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">防御塔三级特效guid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">防御塔攻击特效延迟时间</t>
+  </si>
+  <si>
     <t xml:space="preserve">武器guid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">武器挂载插槽</t>
+  </si>
+  <si>
+    <t xml:space="preserve">武器相对于插槽的位置</t>
+  </si>
+  <si>
+    <t xml:space="preserve">武器特效延迟播放时间</t>
   </si>
   <si>
     <t xml:space="preserve">击中特效</t>
@@ -204,6 +243,9 @@
   </si>
   <si>
     <t xml:space="preserve">攻击动画</t>
+  </si>
+  <si>
+    <t xml:space="preserve">攻击动画数组</t>
   </si>
   <si>
     <t xml:space="preserve">攻击动画持续时间</t>
@@ -863,6 +905,9 @@
     <t xml:space="preserve">E8DF061043359EE84F60AEAAB3D3A68A</t>
   </si>
   <si>
+    <t xml:space="preserve">10|5|6</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.48|0.48|0.48</t>
   </si>
   <si>
@@ -885,6 +930,9 @@
   </si>
   <si>
     <t xml:space="preserve">1000|1250|1500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81687|80483</t>
   </si>
   <si>
     <t xml:space="preserve">光龙娘3</t>
@@ -1189,7 +1237,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1242,27 +1290,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1275,10 +1303,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1501,15 +1525,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BA28"/>
+  <dimension ref="A1:BH28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topRight" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="13.35"/>
@@ -1519,35 +1543,40 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="36.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="44.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="53.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="17" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="24" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="27.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="117.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="46.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="96.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="36.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="64.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="36.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="15.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="27.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="31.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="23.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="45" min="44" style="1" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="50" min="47" style="1" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="15.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="31.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="16.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="18.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="55" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="1" width="53.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="23.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="21.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="20" style="1" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="23" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="21.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="32" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="27.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="117.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="46.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="96.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="36.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="64.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="36.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="15.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="2" width="27.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="2" width="31.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="23.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="57" min="54" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="31.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="16.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="18.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1032" min="62" style="1" width="12.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1588,43 +1617,43 @@
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="S1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="X1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>5</v>
@@ -1633,25 +1662,39 @@
         <v>5</v>
       </c>
       <c r="AB1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
+      <c r="AG1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
-      <c r="AL1" s="4"/>
+      <c r="AL1" s="3"/>
       <c r="AM1" s="3"/>
       <c r="AN1" s="3"/>
       <c r="AO1" s="3"/>
       <c r="AP1" s="3"/>
       <c r="AQ1" s="3"/>
       <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
+      <c r="AS1" s="4"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -1660,6 +1703,13 @@
       <c r="AY1" s="3"/>
       <c r="AZ1" s="3"/>
       <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -1746,23 +1796,37 @@
       <c r="AB2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
+      <c r="AC2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
-      <c r="AL2" s="4"/>
+      <c r="AL2" s="3"/>
       <c r="AM2" s="3"/>
       <c r="AN2" s="3"/>
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
       <c r="AQ2" s="3"/>
       <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
+      <c r="AS2" s="4"/>
       <c r="AT2" s="3"/>
       <c r="AU2" s="3"/>
       <c r="AV2" s="3"/>
@@ -1771,109 +1835,130 @@
       <c r="AY2" s="3"/>
       <c r="AZ2" s="3"/>
       <c r="BA2" s="3"/>
+      <c r="BB2" s="3"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
-      <c r="AL3" s="4"/>
+      <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
       <c r="AQ3" s="3"/>
       <c r="AR3" s="3"/>
-      <c r="AS3" s="3"/>
+      <c r="AS3" s="4"/>
       <c r="AT3" s="3"/>
       <c r="AU3" s="3"/>
       <c r="AV3" s="3"/>
@@ -1882,10 +1967,17 @@
       <c r="AY3" s="3"/>
       <c r="AZ3" s="3"/>
       <c r="BA3" s="3"/>
+      <c r="BB3" s="3"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3"/>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,10 +1985,10 @@
         <v>1001</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>300</v>
@@ -1905,87 +1997,87 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>291768</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N5" s="8" t="n">
+        <v>84</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T5" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O5" s="8" t="n">
+      <c r="U5" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P5" s="1" t="n">
+      <c r="V5" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="V5" s="1" t="n">
+      <c r="W5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB5" s="1" t="n">
         <v>281795</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="X5" s="1" t="n">
+      <c r="AC5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD5" s="1" t="n">
         <v>81687</v>
       </c>
-      <c r="Y5" s="1" t="n">
+      <c r="AF5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA5" s="8" t="n">
+      <c r="AG5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH5" s="8" t="n">
         <v>4007</v>
       </c>
-      <c r="AB5" s="8"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="9"/>
-      <c r="AQ5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AS5" s="9"/>
       <c r="AT5" s="8"/>
+      <c r="AU5" s="9"/>
+      <c r="AX5" s="8"/>
+      <c r="BA5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>1002</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>360</v>
@@ -1994,82 +2086,82 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="G6" s="10" t="n">
         <v>291769</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="N6" s="8" t="n">
+        <v>98</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T6" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O6" s="8" t="n">
+      <c r="U6" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P6" s="1" t="n">
+      <c r="V6" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="T6" s="1" t="s">
+      <c r="W6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="X6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="V6" s="1" t="n">
+      <c r="Z6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB6" s="1" t="n">
         <v>281710</v>
       </c>
-      <c r="W6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="X6" s="1" t="n">
+      <c r="AC6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD6" s="1" t="n">
         <v>80483</v>
       </c>
-      <c r="Y6" s="1" t="n">
+      <c r="AF6" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="Z6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-      <c r="AL6" s="9"/>
-      <c r="AN6" s="9"/>
+      <c r="AG6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AS6" s="9"/>
+      <c r="AU6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>1003</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>540</v>
@@ -2084,79 +2176,79 @@
         <v>291776</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T7" s="8" t="n">
+        <v>107535</v>
+      </c>
+      <c r="U7" s="8" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>281710</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD7" s="1" t="n">
+        <v>80483</v>
+      </c>
+      <c r="AF7" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AG7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N7" s="8" t="n">
-        <v>107535</v>
-      </c>
-      <c r="O7" s="8" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="P7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="V7" s="1" t="n">
-        <v>281710</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="X7" s="1" t="n">
-        <v>80483</v>
-      </c>
-      <c r="Y7" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="8"/>
-      <c r="AN7" s="9"/>
-      <c r="AQ7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AS7" s="9"/>
       <c r="AT7" s="8"/>
+      <c r="AU7" s="9"/>
+      <c r="AX7" s="8"/>
+      <c r="BA7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>1004</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>750</v>
@@ -2165,82 +2257,82 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="G8" s="10" t="n">
         <v>291770</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="N8" s="8" t="n">
+        <v>119</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T8" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O8" s="8" t="n">
+      <c r="U8" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P8" s="1" t="n">
+      <c r="V8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="V8" s="1" t="n">
+      <c r="W8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB8" s="1" t="n">
         <v>20227</v>
       </c>
-      <c r="W8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="X8" s="1" t="n">
+      <c r="AC8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD8" s="1" t="n">
         <v>20279</v>
       </c>
-      <c r="Y8" s="1" t="n">
+      <c r="AF8" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AL8" s="9"/>
-      <c r="AN8" s="9"/>
+      <c r="AG8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AS8" s="9"/>
+      <c r="AU8" s="9"/>
     </row>
     <row r="9" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>1005</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>1125</v>
@@ -2249,80 +2341,87 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="G9" s="10" t="n">
         <v>291772</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="N9" s="8" t="n">
+        <v>129</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O9" s="8" t="n">
+      <c r="U9" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P9" s="1" t="n">
+      <c r="V9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="V9" s="1" t="n">
+      <c r="W9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB9" s="1" t="n">
         <v>20273</v>
       </c>
-      <c r="W9" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="X9" s="1" t="n">
+      <c r="AC9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD9" s="1" t="n">
         <v>288430</v>
       </c>
-      <c r="Y9" s="1" t="n">
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
+      <c r="AG9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
     </row>
     <row r="10" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>1006</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>720</v>
@@ -2331,80 +2430,87 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="G10" s="10" t="n">
         <v>291775</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N10" s="8" t="n">
+        <v>140</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O10" s="8" t="n">
+      <c r="U10" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P10" s="1" t="n">
+      <c r="V10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="V10" s="1" t="n">
+      <c r="W10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB10" s="1" t="n">
         <v>281710</v>
       </c>
-      <c r="W10" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="X10" s="1" t="n">
+      <c r="AC10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD10" s="1" t="n">
         <v>80483</v>
       </c>
-      <c r="Y10" s="1" t="n">
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="Z10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
+      <c r="AG10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
     </row>
     <row r="11" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>1007</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>900</v>
@@ -2413,68 +2519,75 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="G11" s="10" t="n">
         <v>291779</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="N11" s="8" t="n">
+        <v>149</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O11" s="8" t="n">
+      <c r="U11" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P11" s="1" t="n">
+      <c r="V11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="V11" s="1" t="n">
+      <c r="W11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB11" s="1" t="n">
         <v>35385</v>
       </c>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1" t="n">
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1" t="n">
         <v>84862</v>
       </c>
-      <c r="Y11" s="1" t="n">
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8" t="n">
+      <c r="AG11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8" t="n">
         <v>200</v>
       </c>
     </row>
@@ -2483,10 +2596,10 @@
         <v>1008</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>1800</v>
@@ -2495,66 +2608,73 @@
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="G12" s="10" t="n">
         <v>291773</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N12" s="8" t="n">
+        <v>159</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O12" s="8" t="n">
+      <c r="U12" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P12" s="1" t="n">
+      <c r="V12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="V12" s="1" t="n">
+      <c r="W12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB12" s="1" t="n">
         <v>180888</v>
       </c>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1" t="n">
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1" t="n">
         <v>86462</v>
       </c>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8" t="n">
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2563,10 +2683,10 @@
         <v>1009</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>675</v>
@@ -2581,74 +2701,81 @@
         <v>291780</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N13" s="8" t="n">
+        <v>164</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O13" s="8" t="n">
+      <c r="U13" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P13" s="1" t="n">
+      <c r="V13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="V13" s="1" t="n">
+      <c r="W13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB13" s="1" t="n">
         <v>281710</v>
       </c>
-      <c r="W13" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="X13" s="1" t="n">
+      <c r="AC13" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD13" s="1" t="n">
         <v>80483</v>
       </c>
-      <c r="Y13" s="1" t="n">
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="Z13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
+      <c r="AG13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH13" s="8"/>
+      <c r="AI13" s="8"/>
     </row>
     <row r="14" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>1010</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>2100</v>
@@ -2657,80 +2784,87 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="G14" s="10" t="n">
         <v>291778</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="N14" s="8" t="n">
+        <v>172</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O14" s="8" t="n">
+      <c r="U14" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P14" s="1" t="n">
+      <c r="V14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="V14" s="1" t="n">
+      <c r="W14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB14" s="1" t="n">
         <v>281710</v>
       </c>
-      <c r="W14" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="X14" s="1" t="n">
+      <c r="AC14" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD14" s="1" t="n">
         <v>281780</v>
       </c>
-      <c r="Y14" s="1" t="n">
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
+      <c r="AG14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>2001</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>100</v>
@@ -2742,70 +2876,70 @@
         <v>291777</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N15" s="8" t="n">
+        <v>184</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T15" s="8" t="n">
         <v>107535</v>
       </c>
-      <c r="O15" s="8" t="n">
+      <c r="U15" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P15" s="1" t="n">
+      <c r="V15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q15" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="V15" s="1" t="n">
+      <c r="W15" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB15" s="1" t="n">
         <v>180888</v>
       </c>
-      <c r="X15" s="1" t="n">
+      <c r="AD15" s="1" t="n">
         <v>97181</v>
       </c>
-      <c r="Z15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="8"/>
-      <c r="AL15" s="9"/>
-      <c r="AN15" s="9"/>
+      <c r="AG15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH15" s="12"/>
+      <c r="AI15" s="8"/>
+      <c r="AS15" s="9"/>
+      <c r="AU15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>3001</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>500</v>
@@ -2817,905 +2951,900 @@
         <v>291764</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8" t="n">
+        <v>193</v>
+      </c>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8" t="n">
         <v>0.8</v>
       </c>
-      <c r="P16" s="1" t="n">
+      <c r="V16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="X16" s="1" t="n">
+      <c r="W16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD16" s="1" t="n">
         <v>97181</v>
       </c>
-      <c r="Z16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA16" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB16" s="8"/>
-      <c r="AL16" s="9"/>
-      <c r="AN16" s="9"/>
+      <c r="AG16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH16" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="AI16" s="8"/>
+      <c r="AS16" s="9"/>
+      <c r="AU16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="n">
+      <c r="A17" s="2" t="n">
         <v>1011</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="D17" s="14" t="n">
+      <c r="B17" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="E17" s="14" t="n">
+      <c r="E17" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="14" t="n">
+      <c r="F17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="10" t="n">
         <v>326244</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="N17" s="18" t="n">
+      <c r="H17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O17" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="S17" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T17" s="8" t="n">
         <v>168944</v>
       </c>
-      <c r="O17" s="18" t="n">
+      <c r="U17" s="8" t="n">
         <v>0.3</v>
       </c>
-      <c r="P17" s="16" t="n">
+      <c r="V17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q17" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="R17" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="S17" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T17" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="U17" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="V17" s="16" t="n">
+      <c r="W17" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB17" s="1" t="n">
         <v>144183</v>
       </c>
-      <c r="W17" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X17" s="16" t="n">
+      <c r="AC17" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD17" s="1" t="n">
         <v>85959</v>
       </c>
-      <c r="Y17" s="16" t="n">
+      <c r="AF17" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="Z17" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="16"/>
-      <c r="AL17" s="9"/>
-      <c r="AM17" s="8"/>
-      <c r="AN17" s="9"/>
-      <c r="AQ17" s="8"/>
+      <c r="AG17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS17" s="9"/>
       <c r="AT17" s="8"/>
+      <c r="AU17" s="9"/>
+      <c r="AX17" s="8"/>
+      <c r="BA17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="n">
+      <c r="A18" s="2" t="n">
         <v>1012</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D18" s="16" t="n">
+      <c r="B18" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="E18" s="16" t="n">
+      <c r="E18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="19" t="n">
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="14" t="n">
         <v>326244</v>
       </c>
-      <c r="H18" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="M18" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="N18" s="16" t="n">
+      <c r="H18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="T18" s="1" t="n">
         <v>153046</v>
       </c>
-      <c r="O18" s="18" t="n">
+      <c r="U18" s="8" t="n">
         <v>1.5</v>
       </c>
-      <c r="P18" s="16" t="n">
+      <c r="V18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q18" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="R18" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="S18" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T18" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="U18" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="V18" s="16" t="n">
+      <c r="W18" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB18" s="1" t="n">
         <v>284848</v>
       </c>
-      <c r="W18" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X18" s="16" t="n">
+      <c r="AC18" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD18" s="1" t="n">
         <v>121794</v>
       </c>
-      <c r="Y18" s="16" t="n">
+      <c r="AE18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF18" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Z18" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AL18" s="9"/>
-      <c r="AN18" s="9"/>
+      <c r="AG18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS18" s="9"/>
+      <c r="AU18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="n">
+      <c r="A19" s="2" t="n">
         <v>1013</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D19" s="14" t="n">
+      <c r="B19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" s="10" t="n">
         <v>550</v>
       </c>
-      <c r="E19" s="14" t="n">
+      <c r="E19" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="22" t="n">
+      <c r="F19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="12" t="n">
         <v>326267</v>
       </c>
-      <c r="H19" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="N19" s="16" t="n">
+      <c r="H19" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="T19" s="1" t="n">
         <v>151551</v>
       </c>
-      <c r="O19" s="16" t="n">
+      <c r="U19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P19" s="16" t="n">
+      <c r="V19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q19" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="R19" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="S19" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T19" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="U19" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="V19" s="16" t="n">
+      <c r="W19" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB19" s="1" t="n">
         <v>144183</v>
       </c>
-      <c r="W19" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X19" s="16" t="n">
+      <c r="AC19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD19" s="1" t="n">
         <v>20275</v>
       </c>
-      <c r="Y19" s="16" t="n">
+      <c r="AF19" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Z19" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA19" s="16"/>
-      <c r="AB19" s="16" t="n">
+      <c r="AG19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI19" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="AL19" s="9"/>
-      <c r="AM19" s="8"/>
-      <c r="AN19" s="9"/>
-      <c r="AQ19" s="8"/>
+      <c r="AS19" s="9"/>
       <c r="AT19" s="8"/>
+      <c r="AU19" s="9"/>
+      <c r="AX19" s="8"/>
+      <c r="BA19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="2" t="n">
         <v>1014</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="D20" s="16" t="n">
+      <c r="B20" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="E20" s="16" t="n">
+      <c r="E20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="22" t="n">
+      <c r="F20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="12" t="n">
         <v>150576</v>
       </c>
-      <c r="H20" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="N20" s="16" t="n">
+      <c r="H20" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="T20" s="1" t="n">
         <v>200133</v>
       </c>
-      <c r="O20" s="16" t="n">
+      <c r="U20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P20" s="16" t="n">
+      <c r="V20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q20" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="R20" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="S20" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T20" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="U20" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="V20" s="16" t="n">
+      <c r="W20" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB20" s="1" t="n">
         <v>144183</v>
       </c>
-      <c r="W20" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X20" s="16" t="n">
+      <c r="AC20" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD20" s="1" t="n">
         <v>20270</v>
       </c>
-      <c r="Y20" s="16" t="n">
+      <c r="AF20" s="1" t="n">
         <v>1.8</v>
       </c>
-      <c r="Z20" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA20" s="16"/>
-      <c r="AB20" s="16"/>
-      <c r="AL20" s="9"/>
-      <c r="AN20" s="9"/>
+      <c r="AG20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS20" s="9"/>
+      <c r="AU20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="n">
+      <c r="A21" s="18" t="n">
         <v>1015</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="D21" s="14" t="n">
+      <c r="B21" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="E21" s="14" t="n">
+      <c r="E21" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="22" t="n">
+      <c r="F21" s="10"/>
+      <c r="G21" s="12" t="n">
         <v>130536</v>
       </c>
-      <c r="H21" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="J21" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="N21" s="16" t="n">
+      <c r="H21" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="T21" s="1" t="n">
         <v>200133</v>
       </c>
-      <c r="O21" s="16" t="n">
+      <c r="U21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P21" s="16" t="n">
+      <c r="V21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="R21" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="S21" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="T21" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="U21" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="V21" s="16" t="n">
+      <c r="W21" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB21" s="1" t="n">
         <v>144183</v>
       </c>
-      <c r="W21" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X21" s="16" t="n">
+      <c r="AC21" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD21" s="1" t="n">
         <v>20270</v>
       </c>
-      <c r="Y21" s="16" t="n">
+      <c r="AF21" s="1" t="n">
         <v>1.8</v>
       </c>
-      <c r="Z21" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA21" s="16"/>
-      <c r="AB21" s="16"/>
-      <c r="AL21" s="9"/>
-      <c r="AM21" s="8"/>
-      <c r="AN21" s="9"/>
-      <c r="AQ21" s="8"/>
+      <c r="AG21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS21" s="9"/>
       <c r="AT21" s="8"/>
+      <c r="AU21" s="9"/>
+      <c r="AX21" s="8"/>
+      <c r="BA21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="n">
+      <c r="A22" s="18" t="n">
         <v>1016</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="D22" s="16" t="n">
+      <c r="B22" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" s="22" t="n">
+      <c r="F22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="12" t="n">
         <v>326241</v>
       </c>
-      <c r="H22" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="K22" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="M22" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="N22" s="16" t="n">
+      <c r="H22" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="T22" s="1" t="n">
         <v>150929</v>
       </c>
-      <c r="O22" s="16" t="n">
+      <c r="U22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P22" s="16" t="n">
+      <c r="V22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="R22" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="S22" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T22" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="U22" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="V22" s="16" t="n">
+      <c r="W22" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB22" s="1" t="n">
         <v>122546</v>
       </c>
-      <c r="W22" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X22" s="16" t="n">
+      <c r="AC22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD22" s="1" t="n">
         <v>135369</v>
       </c>
-      <c r="Y22" s="16" t="n">
+      <c r="AF22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Z22" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA22" s="16"/>
-      <c r="AB22" s="16"/>
-      <c r="AL22" s="9"/>
-      <c r="AN22" s="9"/>
+      <c r="AG22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS22" s="9"/>
+      <c r="AU22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="n">
+      <c r="A23" s="19" t="n">
         <v>1017</v>
       </c>
-      <c r="B23" s="25" t="s">
-        <v>212</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="D23" s="26" t="n">
+      <c r="B23" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D23" s="20" t="n">
         <v>300</v>
       </c>
-      <c r="E23" s="26" t="n">
+      <c r="E23" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27" t="n">
+      <c r="F23" s="20"/>
+      <c r="G23" s="21" t="n">
         <v>326271</v>
       </c>
-      <c r="H23" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="I23" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="K23" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="L23" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16" t="n">
+      <c r="H23" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="L23" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="U23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P23" s="16" t="n">
+      <c r="V23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="R23" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="S23" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="T23" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="U23" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16" t="n">
+      <c r="W23" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD23" s="1" t="n">
         <v>20270</v>
       </c>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA23" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB23" s="16"/>
-      <c r="AL23" s="9"/>
-      <c r="AM23" s="8"/>
-      <c r="AN23" s="9"/>
-      <c r="AQ23" s="8"/>
+      <c r="AG23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH23" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="AS23" s="9"/>
       <c r="AT23" s="8"/>
+      <c r="AU23" s="9"/>
+      <c r="AX23" s="8"/>
+      <c r="BA23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="n">
+      <c r="A24" s="2" t="n">
         <v>1018</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D24" s="16" t="n">
+      <c r="B24" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E24" s="16" t="n">
+      <c r="E24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="22" t="n">
+      <c r="F24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="12" t="n">
         <v>143689</v>
       </c>
-      <c r="H24" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="N24" s="16" t="n">
+      <c r="H24" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="T24" s="1" t="n">
         <v>254300</v>
       </c>
-      <c r="O24" s="16" t="n">
+      <c r="U24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P24" s="16" t="n">
+      <c r="V24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="R24" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="S24" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T24" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="U24" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="V24" s="14" t="n">
+      <c r="W24" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB24" s="10" t="n">
         <v>285370</v>
       </c>
-      <c r="W24" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X24" s="16" t="n">
+      <c r="AC24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD24" s="1" t="n">
         <v>279685</v>
       </c>
-      <c r="Y24" s="16" t="n">
+      <c r="AF24" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z24" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA24" s="16"/>
-      <c r="AB24" s="16"/>
-      <c r="AL24" s="9"/>
-      <c r="AM24" s="8"/>
-      <c r="AN24" s="9"/>
-      <c r="AQ24" s="8"/>
+      <c r="AG24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS24" s="9"/>
       <c r="AT24" s="8"/>
+      <c r="AU24" s="9"/>
+      <c r="AX24" s="8"/>
+      <c r="BA24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="n">
+      <c r="A25" s="2" t="n">
         <v>1019</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="D25" s="14" t="n">
+      <c r="B25" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D25" s="10" t="n">
         <v>160</v>
       </c>
-      <c r="E25" s="14" t="n">
+      <c r="E25" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="14" t="n">
+      <c r="F25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="10" t="n">
         <v>326237</v>
       </c>
-      <c r="H25" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="K25" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="M25" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="N25" s="16" t="n">
+      <c r="H25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="T25" s="1" t="n">
         <v>150927</v>
       </c>
-      <c r="O25" s="16" t="n">
+      <c r="U25" s="1" t="n">
         <v>1.3</v>
       </c>
-      <c r="P25" s="16" t="n">
+      <c r="V25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="R25" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="S25" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T25" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="U25" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="V25" s="16" t="n">
+      <c r="W25" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB25" s="1" t="n">
         <v>146119</v>
       </c>
-      <c r="W25" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X25" s="16" t="n">
+      <c r="AC25" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD25" s="1" t="n">
         <v>279672</v>
       </c>
-      <c r="Y25" s="16" t="n">
+      <c r="AF25" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z25" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA25" s="16"/>
-      <c r="AB25" s="16"/>
-      <c r="AL25" s="9"/>
-      <c r="AM25" s="8"/>
-      <c r="AN25" s="9"/>
-      <c r="AQ25" s="8"/>
+      <c r="AG25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS25" s="9"/>
       <c r="AT25" s="8"/>
+      <c r="AU25" s="9"/>
+      <c r="AX25" s="8"/>
+      <c r="BA25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="n">
+      <c r="A26" s="2" t="n">
         <v>1020</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="D26" s="16" t="n">
+      <c r="B26" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D26" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="E26" s="16" t="n">
+      <c r="E26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" s="16" t="n">
+      <c r="F26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="1" t="n">
         <v>326236</v>
       </c>
-      <c r="H26" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="L26" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="M26" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="N26" s="16" t="n">
+      <c r="H26" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="T26" s="1" t="n">
         <v>181026</v>
       </c>
-      <c r="O26" s="16" t="n">
+      <c r="U26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P26" s="16" t="n">
+      <c r="V26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="R26" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="S26" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T26" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="U26" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="V26" s="14" t="n">
+      <c r="W26" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB26" s="10" t="n">
         <v>144198</v>
       </c>
-      <c r="W26" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="X26" s="16" t="n">
+      <c r="AC26" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD26" s="1" t="n">
         <v>285283</v>
       </c>
-      <c r="Y26" s="16" t="n">
+      <c r="AF26" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="Z26" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="16"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="8"/>
-      <c r="AN26" s="9"/>
-      <c r="AQ26" s="8"/>
+      <c r="AG26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS26" s="9"/>
       <c r="AT26" s="8"/>
+      <c r="AU26" s="9"/>
+      <c r="AX26" s="8"/>
+      <c r="BA26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
@@ -3728,8 +3857,8 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="AL27" s="9"/>
-      <c r="AN27" s="9"/>
+      <c r="AS27" s="9"/>
+      <c r="AU27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
@@ -3737,12 +3866,15 @@
       <c r="C28" s="2"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
-      <c r="V28" s="10"/>
-      <c r="AL28" s="9"/>
-      <c r="AM28" s="8"/>
-      <c r="AN28" s="9"/>
-      <c r="AQ28" s="8"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="AB28" s="10"/>
+      <c r="AS28" s="9"/>
       <c r="AT28" s="8"/>
+      <c r="AU28" s="9"/>
+      <c r="AX28" s="8"/>
+      <c r="BA28" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat：update new tower excel
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="306">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -969,9 +969,6 @@
   </si>
   <si>
     <t xml:space="preserve">E8DF061043359EE84F60AEAAB3D3A68A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10|5|6</t>
   </si>
   <si>
     <t xml:space="preserve">0.48|0.48|0.48</t>
@@ -1835,10 +1832,10 @@
   </sheetPr>
   <dimension ref="A1:BG35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="Y22" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="topRight" activeCell="AF38" activeCellId="0" sqref="AF38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="O4" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topRight" activeCell="R36" activeCellId="0" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2317,6 +2314,9 @@
       <c r="P5" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="Q5" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="T5" s="8" t="n">
         <v>107535</v>
       </c>
@@ -2406,6 +2406,9 @@
       <c r="P6" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="Q6" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="T6" s="8" t="n">
         <v>107535</v>
       </c>
@@ -2489,6 +2492,9 @@
       </c>
       <c r="P7" s="1" t="s">
         <v>107</v>
+      </c>
+      <c r="Q7" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T7" s="8" t="n">
         <v>107535</v>
@@ -2577,6 +2583,9 @@
       <c r="P8" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="Q8" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="T8" s="8" t="n">
         <v>107535</v>
       </c>
@@ -2664,7 +2673,9 @@
       <c r="P9" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Q9" s="1"/>
+      <c r="Q9" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="8" t="n">
@@ -2752,7 +2763,9 @@
       <c r="P10" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Q10" s="1"/>
+      <c r="Q10" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="8" t="n">
@@ -2840,7 +2853,9 @@
       <c r="P11" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="Q11" s="1"/>
+      <c r="Q11" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="8" t="n">
@@ -2928,7 +2943,9 @@
       <c r="P12" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Q12" s="1"/>
+      <c r="Q12" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="8" t="n">
@@ -3014,7 +3031,9 @@
       <c r="P13" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="Q13" s="1"/>
+      <c r="Q13" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="8" t="n">
@@ -3102,7 +3121,9 @@
       <c r="P14" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="Q14" s="1"/>
+      <c r="Q14" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="8" t="n">
@@ -3183,6 +3204,9 @@
       </c>
       <c r="P15" s="1" t="s">
         <v>107</v>
+      </c>
+      <c r="Q15" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T15" s="8" t="n">
         <v>107535</v>
@@ -3257,6 +3281,9 @@
       <c r="L16" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="Q16" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="T16" s="8"/>
       <c r="U16" s="8" t="n">
         <v>0.8</v>
@@ -3337,10 +3364,7 @@
         <v>200</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>201</v>
+        <v>16</v>
       </c>
       <c r="S17" s="1" t="n">
         <v>0.5</v>
@@ -3355,7 +3379,7 @@
         <v>0</v>
       </c>
       <c r="W17" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X17" s="9" t="s">
         <v>85</v>
@@ -3367,7 +3391,7 @@
         <v>85</v>
       </c>
       <c r="AA17" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB17" s="9" t="n">
         <v>144183</v>
@@ -3397,10 +3421,10 @@
         <v>1012</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D18" s="9" t="n">
         <v>600</v>
@@ -3421,16 +3445,19 @@
         <v>79</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L18" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="K18" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="L18" s="9" t="s">
+      <c r="P18" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="P18" s="9" t="s">
-        <v>207</v>
+      <c r="Q18" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T18" s="9" t="n">
         <v>153046</v>
@@ -3442,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="W18" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="X18" s="9" t="s">
         <v>85</v>
@@ -3454,7 +3481,7 @@
         <v>149</v>
       </c>
       <c r="AA18" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB18" s="9" t="n">
         <v>284848</v>
@@ -3481,10 +3508,10 @@
         <v>1013</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D19" s="14" t="n">
         <v>550</v>
@@ -3505,16 +3532,19 @@
         <v>79</v>
       </c>
       <c r="J19" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L19" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="K19" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="L19" s="9" t="s">
+      <c r="P19" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="P19" s="9" t="s">
-        <v>213</v>
+      <c r="Q19" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T19" s="9" t="n">
         <v>151551</v>
@@ -3529,16 +3559,16 @@
         <v>149</v>
       </c>
       <c r="X19" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y19" s="9" t="s">
         <v>86</v>
       </c>
       <c r="Z19" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA19" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="AA19" s="9" t="s">
-        <v>216</v>
       </c>
       <c r="AB19" s="9" t="n">
         <v>144183</v>
@@ -3570,10 +3600,10 @@
         <v>1014</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="D20" s="9" t="n">
         <v>80</v>
@@ -3594,16 +3624,19 @@
         <v>79</v>
       </c>
       <c r="J20" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="L20" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="K20" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="L20" s="9" t="s">
+      <c r="P20" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="P20" s="9" t="s">
-        <v>221</v>
+      <c r="Q20" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T20" s="9" t="n">
         <v>200133</v>
@@ -3615,7 +3648,7 @@
         <v>0</v>
       </c>
       <c r="W20" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X20" s="9" t="s">
         <v>85</v>
@@ -3624,10 +3657,10 @@
         <v>86</v>
       </c>
       <c r="Z20" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA20" s="9" t="s">
         <v>223</v>
-      </c>
-      <c r="AA20" s="9" t="s">
-        <v>224</v>
       </c>
       <c r="AB20" s="9" t="n">
         <v>144183</v>
@@ -3654,10 +3687,10 @@
         <v>1015</v>
       </c>
       <c r="B21" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="D21" s="14" t="n">
         <v>100</v>
@@ -3670,7 +3703,7 @@
         <v>130536</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>179</v>
@@ -3682,10 +3715,13 @@
         <v>181</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
+      </c>
+      <c r="Q21" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T21" s="9" t="n">
         <v>200133</v>
@@ -3739,10 +3775,10 @@
         <v>1016</v>
       </c>
       <c r="B22" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="D22" s="9" t="n">
         <v>200</v>
@@ -3763,16 +3799,19 @@
         <v>79</v>
       </c>
       <c r="J22" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="K22" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="L22" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="P22" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="P22" s="9" t="s">
-        <v>234</v>
+      <c r="Q22" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T22" s="9" t="n">
         <v>150929</v>
@@ -3784,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="W22" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="X22" s="9" t="s">
         <v>85</v>
@@ -3796,7 +3835,7 @@
         <v>149</v>
       </c>
       <c r="AA22" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AB22" s="9" t="n">
         <v>122546</v>
@@ -3823,10 +3862,10 @@
         <v>1017</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D23" s="23" t="n">
         <v>300</v>
@@ -3839,7 +3878,7 @@
         <v>326271</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I23" s="26" t="s">
         <v>189</v>
@@ -3851,12 +3890,15 @@
         <v>190</v>
       </c>
       <c r="L23" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M23" s="29"/>
       <c r="N23" s="29"/>
       <c r="O23" s="29"/>
       <c r="P23" s="9"/>
+      <c r="Q23" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="T23" s="9"/>
       <c r="U23" s="9" t="n">
         <v>1</v>
@@ -3903,10 +3945,10 @@
         <v>1018</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D24" s="9" t="n">
         <v>200</v>
@@ -3927,16 +3969,19 @@
         <v>79</v>
       </c>
       <c r="J24" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="L24" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="K24" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="L24" s="9" t="s">
+      <c r="P24" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="P24" s="9" t="s">
-        <v>242</v>
+      <c r="Q24" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T24" s="9" t="n">
         <v>254300</v>
@@ -3948,7 +3993,7 @@
         <v>0</v>
       </c>
       <c r="W24" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X24" s="9" t="s">
         <v>85</v>
@@ -3957,10 +4002,10 @@
         <v>86</v>
       </c>
       <c r="Z24" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA24" s="9" t="s">
         <v>244</v>
-      </c>
-      <c r="AA24" s="9" t="s">
-        <v>245</v>
       </c>
       <c r="AB24" s="14" t="n">
         <v>285370</v>
@@ -3990,10 +4035,10 @@
         <v>1019</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D25" s="14" t="n">
         <v>160</v>
@@ -4014,16 +4059,19 @@
         <v>79</v>
       </c>
       <c r="J25" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="L25" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="K25" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="L25" s="9" t="s">
+      <c r="P25" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="P25" s="9" t="s">
-        <v>249</v>
+      <c r="Q25" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T25" s="9" t="n">
         <v>150927</v>
@@ -4035,19 +4083,19 @@
         <v>0</v>
       </c>
       <c r="W25" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="X25" s="9" t="s">
         <v>250</v>
-      </c>
-      <c r="X25" s="9" t="s">
-        <v>251</v>
       </c>
       <c r="Y25" s="9" t="s">
         <v>86</v>
       </c>
       <c r="Z25" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA25" s="9" t="s">
         <v>252</v>
-      </c>
-      <c r="AA25" s="9" t="s">
-        <v>253</v>
       </c>
       <c r="AB25" s="9" t="n">
         <v>146119</v>
@@ -4077,10 +4125,10 @@
         <v>1020</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D26" s="9" t="n">
         <v>70</v>
@@ -4101,16 +4149,19 @@
         <v>79</v>
       </c>
       <c r="J26" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="L26" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="K26" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="L26" s="9" t="s">
+      <c r="P26" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="P26" s="9" t="s">
-        <v>257</v>
+      <c r="Q26" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T26" s="9" t="n">
         <v>181026</v>
@@ -4122,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="W26" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="X26" s="9" t="s">
         <v>85</v>
@@ -4131,10 +4182,10 @@
         <v>86</v>
       </c>
       <c r="Z26" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA26" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="AA26" s="9" t="s">
-        <v>260</v>
       </c>
       <c r="AB26" s="14" t="n">
         <v>144198</v>
@@ -4164,10 +4215,10 @@
         <v>1021</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D27" s="14" t="n">
         <v>80</v>
@@ -4188,16 +4239,19 @@
         <v>79</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L27" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="P27" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="P27" s="9" t="s">
-        <v>263</v>
+      <c r="Q27" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T27" s="9" t="n">
         <v>151069</v>
@@ -4209,19 +4263,19 @@
         <v>0</v>
       </c>
       <c r="W27" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="X27" s="9" t="s">
         <v>264</v>
-      </c>
-      <c r="X27" s="9" t="s">
-        <v>265</v>
       </c>
       <c r="Y27" s="9" t="s">
         <v>86</v>
       </c>
       <c r="Z27" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="AA27" s="9" t="s">
         <v>265</v>
-      </c>
-      <c r="AA27" s="9" t="s">
-        <v>266</v>
       </c>
       <c r="AB27" s="9" t="n">
         <v>281886</v>
@@ -4248,10 +4302,10 @@
         <v>1022</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D28" s="14" t="n">
         <v>100</v>
@@ -4266,25 +4320,28 @@
         <v>130536</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>179</v>
       </c>
       <c r="J28" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="L28" s="9" t="s">
         <v>268</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>269</v>
       </c>
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
       <c r="P28" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T28" s="9" t="n">
         <v>200133</v>
@@ -4296,7 +4353,7 @@
         <v>0</v>
       </c>
       <c r="W28" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="X28" s="9" t="s">
         <v>184</v>
@@ -4308,7 +4365,7 @@
         <v>86</v>
       </c>
       <c r="AA28" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AB28" s="9" t="n">
         <v>144183</v>
@@ -4338,10 +4395,10 @@
         <v>1023</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D29" s="9" t="n">
         <v>150</v>
@@ -4354,7 +4411,7 @@
         <v>129508</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>189</v>
@@ -4366,9 +4423,12 @@
         <v>115</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P29" s="9"/>
+      <c r="Q29" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="T29" s="9"/>
       <c r="U29" s="9" t="n">
         <v>1</v>
@@ -4389,7 +4449,7 @@
         <v>114</v>
       </c>
       <c r="AA29" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AB29" s="9"/>
       <c r="AC29" s="9"/>
@@ -4410,10 +4470,10 @@
         <v>1024</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D30" s="9" t="n">
         <v>250</v>
@@ -4426,7 +4486,7 @@
         <v>319126</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>189</v>
@@ -4438,9 +4498,12 @@
         <v>115</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P30" s="9"/>
+      <c r="Q30" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="T30" s="9"/>
       <c r="U30" s="9" t="n">
         <v>1</v>
@@ -4461,7 +4524,7 @@
         <v>114</v>
       </c>
       <c r="AA30" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AB30" s="9"/>
       <c r="AC30" s="9"/>
@@ -4482,10 +4545,10 @@
         <v>1025</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D31" s="9" t="n">
         <v>400</v>
@@ -4506,16 +4569,19 @@
         <v>79</v>
       </c>
       <c r="J31" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="L31" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="K31" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="L31" s="9" t="s">
+      <c r="P31" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="P31" s="9" t="s">
-        <v>281</v>
+      <c r="Q31" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T31" s="9" t="n">
         <v>151576</v>
@@ -4527,7 +4593,7 @@
         <v>0</v>
       </c>
       <c r="W31" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="X31" s="9" t="s">
         <v>130</v>
@@ -4539,7 +4605,7 @@
         <v>149</v>
       </c>
       <c r="AA31" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AB31" s="9" t="n">
         <v>281788</v>
@@ -4564,10 +4630,10 @@
         <v>1026</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D32" s="9" t="n">
         <v>210</v>
@@ -4588,16 +4654,19 @@
         <v>79</v>
       </c>
       <c r="J32" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="L32" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="K32" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="L32" s="9" t="s">
+      <c r="P32" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="P32" s="9" t="s">
-        <v>287</v>
+      <c r="Q32" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T32" s="9" t="n">
         <v>168944</v>
@@ -4609,7 +4678,7 @@
         <v>0</v>
       </c>
       <c r="W32" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X32" s="9" t="s">
         <v>172</v>
@@ -4618,10 +4687,10 @@
         <v>86</v>
       </c>
       <c r="Z32" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AA32" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AB32" s="9" t="n">
         <v>285400</v>
@@ -4646,10 +4715,10 @@
         <v>1027</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D33" s="9" t="n">
         <v>500</v>
@@ -4670,16 +4739,19 @@
         <v>79</v>
       </c>
       <c r="J33" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="L33" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="K33" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="L33" s="9" t="s">
+      <c r="P33" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="P33" s="9" t="s">
-        <v>292</v>
+      <c r="Q33" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T33" s="9" t="n">
         <v>99608</v>
@@ -4691,7 +4763,7 @@
         <v>0</v>
       </c>
       <c r="W33" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="X33" s="9" t="s">
         <v>172</v>
@@ -4703,7 +4775,7 @@
         <v>149</v>
       </c>
       <c r="AA33" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB33" s="9" t="n">
         <v>281710</v>
@@ -4728,10 +4800,10 @@
         <v>1028</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>270</v>
@@ -4752,16 +4824,19 @@
         <v>79</v>
       </c>
       <c r="J34" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="L34" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="K34" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="L34" s="9" t="s">
+      <c r="P34" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="P34" s="1" t="s">
-        <v>298</v>
+      <c r="Q34" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T34" s="1" t="n">
         <v>288335</v>
@@ -4773,19 +4848,19 @@
         <v>0</v>
       </c>
       <c r="W34" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="X34" s="9" t="s">
         <v>299</v>
-      </c>
-      <c r="X34" s="9" t="s">
-        <v>300</v>
       </c>
       <c r="Y34" s="9" t="s">
         <v>86</v>
       </c>
       <c r="Z34" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AA34" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AB34" s="1" t="n">
         <v>299561</v>
@@ -4808,10 +4883,10 @@
         <v>1029</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>550</v>
@@ -4832,16 +4907,19 @@
         <v>79</v>
       </c>
       <c r="J35" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="L35" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="K35" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="L35" s="9" t="s">
+      <c r="P35" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="P35" s="1" t="s">
-        <v>305</v>
+      <c r="Q35" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="T35" s="1" t="n">
         <v>130642</v>
@@ -4865,7 +4943,7 @@
         <v>149</v>
       </c>
       <c r="AA35" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AB35" s="1" t="n">
         <v>285356</v>

</xml_diff>

<commit_message>
feat：update tower delay time
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="325">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -994,6 +994,9 @@
   </si>
   <si>
     <t xml:space="preserve">B06787054CADB7A7F6D7119045051E1E|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000|500</t>
   </si>
   <si>
     <t xml:space="preserve">D4B7264E42074A814EA43BA7906BBEE7</t>
@@ -1597,6 +1600,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1635,10 +1642,6 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1902,10 +1905,10 @@
   </sheetPr>
   <dimension ref="A1:BF38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C13" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="topRight" activeCell="S36" activeCellId="0" sqref="S36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="O7" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="O20" activeCellId="0" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1950,386 +1953,386 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="16.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="18.75"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1030" min="60" style="1" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="3" width="10.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="4"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3"/>
-      <c r="BA1" s="3"/>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3"/>
-      <c r="BD1" s="3"/>
-      <c r="BE1" s="3"/>
-      <c r="BF1" s="3"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
+      <c r="AL1" s="4"/>
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4"/>
+      <c r="AO1" s="4"/>
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="4"/>
+      <c r="AS1" s="4"/>
+      <c r="AT1" s="4"/>
+      <c r="AU1" s="4"/>
+      <c r="AV1" s="4"/>
+      <c r="AW1" s="4"/>
+      <c r="AX1" s="4"/>
+      <c r="AY1" s="4"/>
+      <c r="AZ1" s="4"/>
+      <c r="BA1" s="4"/>
+      <c r="BB1" s="4"/>
+      <c r="BC1" s="4"/>
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="3"/>
-      <c r="AY2" s="3"/>
-      <c r="AZ2" s="3"/>
-      <c r="BA2" s="3"/>
-      <c r="BB2" s="3"/>
-      <c r="BC2" s="3"/>
-      <c r="BD2" s="3"/>
-      <c r="BE2" s="3"/>
-      <c r="BF2" s="3"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="4"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="4"/>
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="4"/>
+      <c r="BB2" s="4"/>
+      <c r="BC2" s="4"/>
+      <c r="BD2" s="4"/>
+      <c r="BE2" s="4"/>
+      <c r="BF2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="Z3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AA3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AB3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AC3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AD3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AE3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="AF3" s="5" t="s">
+      <c r="AF3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="AG3" s="5" t="s">
+      <c r="AG3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="3"/>
-      <c r="AJ3" s="3"/>
-      <c r="AK3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AM3" s="3"/>
-      <c r="AN3" s="3"/>
-      <c r="AO3" s="3"/>
-      <c r="AP3" s="3"/>
-      <c r="AQ3" s="4"/>
-      <c r="AR3" s="3"/>
-      <c r="AS3" s="3"/>
-      <c r="AT3" s="3"/>
-      <c r="AU3" s="3"/>
-      <c r="AV3" s="3"/>
-      <c r="AW3" s="3"/>
-      <c r="AX3" s="3"/>
-      <c r="AY3" s="3"/>
-      <c r="AZ3" s="3"/>
-      <c r="BA3" s="3"/>
-      <c r="BB3" s="3"/>
-      <c r="BC3" s="3"/>
-      <c r="BD3" s="3"/>
-      <c r="BE3" s="3"/>
-      <c r="BF3" s="3"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="4"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
+      <c r="BA3" s="4"/>
+      <c r="BB3" s="4"/>
+      <c r="BC3" s="4"/>
+      <c r="BD3" s="4"/>
+      <c r="BE3" s="4"/>
+      <c r="BF3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
@@ -2340,7 +2343,7 @@
       <c r="A5" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2358,7 +2361,7 @@
       <c r="G5" s="1" t="n">
         <v>291768</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -2379,10 +2382,10 @@
       <c r="Q5" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T5" s="8" t="n">
+      <c r="T5" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U5" s="8" t="n">
+      <c r="U5" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V5" s="1" t="s">
@@ -2409,27 +2412,27 @@
       <c r="AC5" s="1" t="n">
         <v>81687</v>
       </c>
-      <c r="AD5" s="9" t="n">
+      <c r="AD5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AE5" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF5" s="10" t="n">
+      <c r="AF5" s="11" t="n">
         <v>4007</v>
       </c>
-      <c r="AG5" s="10"/>
-      <c r="AQ5" s="11"/>
-      <c r="AR5" s="8"/>
-      <c r="AS5" s="11"/>
-      <c r="AV5" s="8"/>
-      <c r="AY5" s="8"/>
+      <c r="AG5" s="11"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="9"/>
+      <c r="AS5" s="12"/>
+      <c r="AV5" s="9"/>
+      <c r="AY5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>1002</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2438,16 +2441,16 @@
       <c r="D6" s="2" t="n">
         <v>360</v>
       </c>
-      <c r="E6" s="12" t="n">
+      <c r="E6" s="13" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="12" t="n">
+      <c r="G6" s="13" t="n">
         <v>291769</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -2468,10 +2471,10 @@
       <c r="Q6" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T6" s="8" t="n">
+      <c r="T6" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U6" s="8" t="n">
+      <c r="U6" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V6" s="1" t="s">
@@ -2498,22 +2501,22 @@
       <c r="AC6" s="1" t="n">
         <v>80483</v>
       </c>
-      <c r="AD6" s="9" t="n">
+      <c r="AD6" s="10" t="n">
         <v>0.1</v>
       </c>
-      <c r="AE6" s="9" t="s">
+      <c r="AE6" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF6" s="10"/>
-      <c r="AG6" s="10"/>
-      <c r="AQ6" s="11"/>
-      <c r="AS6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AQ6" s="12"/>
+      <c r="AS6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>1003</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2531,7 +2534,7 @@
       <c r="G7" s="1" t="n">
         <v>291776</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -2552,10 +2555,10 @@
       <c r="Q7" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T7" s="8" t="n">
+      <c r="T7" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U7" s="8" t="n">
+      <c r="U7" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V7" s="1" t="s">
@@ -2582,25 +2585,25 @@
       <c r="AC7" s="1" t="n">
         <v>80483</v>
       </c>
-      <c r="AD7" s="9" t="n">
+      <c r="AD7" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="AE7" s="9" t="s">
+      <c r="AE7" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF7" s="10"/>
-      <c r="AG7" s="10"/>
-      <c r="AQ7" s="11"/>
-      <c r="AR7" s="8"/>
-      <c r="AS7" s="11"/>
-      <c r="AV7" s="8"/>
-      <c r="AY7" s="8"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AQ7" s="12"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="12"/>
+      <c r="AV7" s="9"/>
+      <c r="AY7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>1004</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -2609,16 +2612,16 @@
       <c r="D8" s="2" t="n">
         <v>750</v>
       </c>
-      <c r="E8" s="12" t="n">
+      <c r="E8" s="13" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G8" s="12" t="n">
+      <c r="G8" s="13" t="n">
         <v>291770</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -2639,10 +2642,10 @@
       <c r="Q8" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T8" s="8" t="n">
+      <c r="T8" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U8" s="8" t="n">
+      <c r="U8" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V8" s="1" t="s">
@@ -2669,22 +2672,22 @@
       <c r="AC8" s="1" t="n">
         <v>20279</v>
       </c>
-      <c r="AD8" s="9" t="n">
+      <c r="AD8" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="AE8" s="9" t="s">
+      <c r="AE8" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF8" s="10"/>
-      <c r="AG8" s="10"/>
-      <c r="AQ8" s="11"/>
-      <c r="AS8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AQ8" s="12"/>
+      <c r="AS8" s="12"/>
     </row>
     <row r="9" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>1005</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>121</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -2699,10 +2702,10 @@
       <c r="F9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="12" t="n">
+      <c r="G9" s="13" t="n">
         <v>291772</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -2728,10 +2731,10 @@
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="8" t="n">
+      <c r="T9" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U9" s="8" t="n">
+      <c r="U9" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V9" s="1" t="s">
@@ -2758,20 +2761,20 @@
       <c r="AC9" s="1" t="n">
         <v>288430</v>
       </c>
-      <c r="AD9" s="9" t="n">
+      <c r="AD9" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="AE9" s="9" t="s">
+      <c r="AE9" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="11"/>
     </row>
     <row r="10" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>1006</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>132</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -2780,16 +2783,16 @@
       <c r="D10" s="2" t="n">
         <v>720</v>
       </c>
-      <c r="E10" s="12" t="n">
+      <c r="E10" s="13" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="12" t="n">
+      <c r="G10" s="13" t="n">
         <v>291775</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -2815,10 +2818,10 @@
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="8" t="n">
+      <c r="T10" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U10" s="8" t="n">
+      <c r="U10" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V10" s="1" t="s">
@@ -2845,20 +2848,20 @@
       <c r="AC10" s="1" t="n">
         <v>80483</v>
       </c>
-      <c r="AD10" s="9" t="n">
+      <c r="AD10" s="10" t="n">
         <v>0.2</v>
       </c>
-      <c r="AE10" s="9" t="s">
+      <c r="AE10" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
     </row>
     <row r="11" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>1007</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>140</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -2873,10 +2876,10 @@
       <c r="F11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G11" s="12" t="n">
+      <c r="G11" s="13" t="n">
         <v>291779</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="8" t="s">
         <v>142</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -2902,10 +2905,10 @@
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="8" t="n">
+      <c r="T11" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U11" s="8" t="n">
+      <c r="U11" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V11" s="1" t="s">
@@ -2930,14 +2933,14 @@
       <c r="AC11" s="1" t="n">
         <v>84862</v>
       </c>
-      <c r="AD11" s="9" t="n">
+      <c r="AD11" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="AE11" s="9" t="s">
+      <c r="AE11" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF11" s="10"/>
-      <c r="AG11" s="10" t="n">
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11" t="n">
         <v>200</v>
       </c>
     </row>
@@ -2945,7 +2948,7 @@
       <c r="A12" s="2" t="n">
         <v>1008</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -2954,16 +2957,16 @@
       <c r="D12" s="2" t="n">
         <v>1800</v>
       </c>
-      <c r="E12" s="12" t="n">
+      <c r="E12" s="13" t="n">
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G12" s="12" t="n">
+      <c r="G12" s="13" t="n">
         <v>291773</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="8" t="s">
         <v>152</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -2989,10 +2992,10 @@
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="8" t="n">
+      <c r="T12" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U12" s="8" t="n">
+      <c r="U12" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V12" s="1" t="s">
@@ -3017,12 +3020,12 @@
       <c r="AC12" s="1" t="n">
         <v>86462</v>
       </c>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9" t="s">
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF12" s="10"/>
-      <c r="AG12" s="10" t="n">
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3030,7 +3033,7 @@
       <c r="A13" s="2" t="n">
         <v>1009</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>156</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -3045,10 +3048,10 @@
       <c r="F13" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G13" s="12" t="n">
+      <c r="G13" s="13" t="n">
         <v>291780</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -3074,10 +3077,10 @@
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="8" t="n">
+      <c r="T13" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U13" s="8" t="n">
+      <c r="U13" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V13" s="1" t="s">
@@ -3104,20 +3107,20 @@
       <c r="AC13" s="1" t="n">
         <v>80483</v>
       </c>
-      <c r="AD13" s="9" t="n">
+      <c r="AD13" s="10" t="n">
         <v>0.3</v>
       </c>
-      <c r="AE13" s="9" t="s">
+      <c r="AE13" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF13" s="10"/>
-      <c r="AG13" s="10"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11"/>
     </row>
     <row r="14" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>1010</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>164</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -3126,16 +3129,16 @@
       <c r="D14" s="2" t="n">
         <v>2100</v>
       </c>
-      <c r="E14" s="12" t="n">
+      <c r="E14" s="13" t="n">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="12" t="n">
+      <c r="G14" s="13" t="n">
         <v>291778</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -3161,10 +3164,10 @@
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="8" t="n">
+      <c r="T14" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U14" s="8" t="n">
+      <c r="U14" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V14" s="1" t="s">
@@ -3191,20 +3194,20 @@
       <c r="AC14" s="1" t="n">
         <v>281780</v>
       </c>
-      <c r="AD14" s="9" t="n">
+      <c r="AD14" s="10" t="n">
         <v>0.25</v>
       </c>
-      <c r="AE14" s="9" t="s">
+      <c r="AE14" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>2001</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>174</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -3213,13 +3216,13 @@
       <c r="D15" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="E15" s="12" t="n">
+      <c r="E15" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="12" t="n">
+      <c r="G15" s="13" t="n">
         <v>291777</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="8" t="s">
         <v>176</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -3240,10 +3243,10 @@
       <c r="Q15" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T15" s="8" t="n">
+      <c r="T15" s="9" t="n">
         <v>107535</v>
       </c>
-      <c r="U15" s="8" t="n">
+      <c r="U15" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V15" s="1" t="s">
@@ -3267,20 +3270,20 @@
       <c r="AC15" s="1" t="n">
         <v>97181</v>
       </c>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9" t="s">
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF15" s="13"/>
-      <c r="AG15" s="10"/>
-      <c r="AQ15" s="11"/>
-      <c r="AS15" s="11"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="11"/>
+      <c r="AQ15" s="12"/>
+      <c r="AS15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>3001</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>184</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -3289,13 +3292,13 @@
       <c r="D16" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="E16" s="12" t="n">
+      <c r="E16" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="G16" s="12" t="n">
+      <c r="G16" s="13" t="n">
         <v>291764</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="8" t="s">
         <v>186</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -3313,8 +3316,8 @@
       <c r="Q16" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8" t="n">
+      <c r="T16" s="9"/>
+      <c r="U16" s="9" t="n">
         <v>0.8</v>
       </c>
       <c r="V16" s="1" t="s">
@@ -3335,16 +3338,16 @@
       <c r="AC16" s="1" t="n">
         <v>97181</v>
       </c>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9" t="s">
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF16" s="10" t="s">
+      <c r="AF16" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="AG16" s="10"/>
-      <c r="AQ16" s="11"/>
-      <c r="AS16" s="11"/>
+      <c r="AG16" s="11"/>
+      <c r="AQ16" s="12"/>
+      <c r="AS16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -3371,7 +3374,7 @@
       <c r="H17" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="10" t="s">
         <v>77</v>
       </c>
       <c r="J17" s="16" t="s">
@@ -3380,61 +3383,61 @@
       <c r="K17" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="10" t="s">
         <v>197</v>
       </c>
       <c r="O17" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="P17" s="10" t="s">
         <v>198</v>
       </c>
       <c r="Q17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T17" s="10" t="n">
+      <c r="T17" s="11" t="n">
         <v>168944</v>
       </c>
-      <c r="U17" s="10" t="n">
+      <c r="U17" s="11" t="n">
         <v>0.3</v>
       </c>
-      <c r="V17" s="9" t="s">
+      <c r="V17" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="W17" s="9" t="s">
+      <c r="W17" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X17" s="9" t="s">
+      <c r="X17" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y17" s="9" t="s">
+      <c r="Y17" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="Z17" s="9" t="s">
+      <c r="Z17" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="AA17" s="9" t="n">
+      <c r="AA17" s="10" t="n">
         <v>144183</v>
       </c>
-      <c r="AB17" s="9" t="s">
+      <c r="AB17" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC17" s="9" t="n">
+      <c r="AC17" s="10" t="n">
         <v>85959</v>
       </c>
-      <c r="AD17" s="9" t="n">
+      <c r="AD17" s="10" t="n">
         <v>0.3</v>
       </c>
-      <c r="AE17" s="9" t="s">
+      <c r="AE17" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AQ17" s="11"/>
-      <c r="AR17" s="8"/>
-      <c r="AS17" s="11"/>
-      <c r="AV17" s="8"/>
-      <c r="AY17" s="8"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AQ17" s="12"/>
+      <c r="AR17" s="9"/>
+      <c r="AS17" s="12"/>
+      <c r="AV17" s="9"/>
+      <c r="AY17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -3446,13 +3449,13 @@
       <c r="C18" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D18" s="9" t="n">
+      <c r="D18" s="10" t="n">
         <v>600</v>
       </c>
-      <c r="E18" s="9" t="n">
+      <c r="E18" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="10" t="s">
         <v>75</v>
       </c>
       <c r="G18" s="17" t="n">
@@ -3467,58 +3470,58 @@
       <c r="J18" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="L18" s="9" t="s">
+      <c r="L18" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="P18" s="9" t="s">
+      <c r="P18" s="10" t="s">
         <v>204</v>
       </c>
       <c r="Q18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T18" s="9" t="n">
+      <c r="T18" s="10" t="n">
         <v>153046</v>
       </c>
-      <c r="U18" s="10" t="n">
+      <c r="U18" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="V18" s="9" t="s">
+      <c r="V18" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="W18" s="9" t="s">
+      <c r="W18" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X18" s="9" t="s">
+      <c r="X18" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y18" s="9" t="s">
+      <c r="Y18" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="Z18" s="9" t="s">
+      <c r="Z18" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="AA18" s="9" t="n">
+      <c r="AA18" s="10" t="n">
         <v>284848</v>
       </c>
-      <c r="AB18" s="9" t="s">
+      <c r="AB18" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC18" s="9" t="n">
+      <c r="AC18" s="10" t="n">
         <v>121794</v>
       </c>
-      <c r="AD18" s="9" t="n">
+      <c r="AD18" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="AE18" s="9" t="s">
+      <c r="AE18" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="9"/>
-      <c r="AQ18" s="11"/>
-      <c r="AS18" s="11"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="10"/>
+      <c r="AQ18" s="12"/>
+      <c r="AS18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="n">
@@ -3536,10 +3539,10 @@
       <c r="E19" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="13" t="n">
+      <c r="G19" s="3" t="n">
         <v>326267</v>
       </c>
       <c r="H19" s="18" t="s">
@@ -3551,90 +3554,90 @@
       <c r="J19" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="L19" s="9" t="s">
+      <c r="L19" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="O19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P19" s="9" t="s">
+      <c r="O19" s="22" t="s">
         <v>210</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="Q19" s="1" t="n">
         <v>16</v>
       </c>
       <c r="S19" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="T19" s="9" t="n">
+        <v>212</v>
+      </c>
+      <c r="T19" s="10" t="n">
         <v>151551</v>
       </c>
-      <c r="U19" s="9" t="n">
+      <c r="U19" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V19" s="9" t="s">
+      <c r="V19" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="W19" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="X19" s="9" t="s">
+      <c r="W19" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="X19" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y19" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z19" s="9" t="s">
+      <c r="Y19" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="AA19" s="9" t="n">
+      <c r="Z19" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA19" s="10" t="n">
         <v>144183</v>
       </c>
-      <c r="AB19" s="9" t="s">
+      <c r="AB19" s="10" t="s">
         <v>173</v>
       </c>
       <c r="AC19" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD19" s="9" t="n">
+        <v>216</v>
+      </c>
+      <c r="AD19" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="AE19" s="9" t="s">
+      <c r="AE19" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="9" t="n">
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="AQ19" s="11"/>
-      <c r="AR19" s="8"/>
-      <c r="AS19" s="11"/>
-      <c r="AV19" s="8"/>
-      <c r="AY19" s="8"/>
+      <c r="AQ19" s="12"/>
+      <c r="AR19" s="9"/>
+      <c r="AS19" s="12"/>
+      <c r="AV19" s="9"/>
+      <c r="AY19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>1014</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D20" s="9" t="n">
+        <v>218</v>
+      </c>
+      <c r="D20" s="10" t="n">
         <v>80</v>
       </c>
-      <c r="E20" s="9" t="n">
+      <c r="E20" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="13" t="n">
+      <c r="G20" s="3" t="n">
         <v>150576</v>
       </c>
       <c r="H20" s="18" t="s">
@@ -3644,70 +3647,70 @@
         <v>77</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="L20" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="P20" s="9" t="s">
+      <c r="K20" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>220</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>221</v>
       </c>
       <c r="Q20" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T20" s="9" t="n">
+      <c r="T20" s="10" t="n">
         <v>200133</v>
       </c>
-      <c r="U20" s="9" t="n">
+      <c r="U20" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V20" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="W20" s="9" t="s">
+      <c r="V20" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="W20" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X20" s="9" t="s">
+      <c r="X20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y20" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z20" s="9" t="s">
+      <c r="Y20" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="AA20" s="9" t="n">
+      <c r="Z20" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA20" s="10" t="n">
         <v>144183</v>
       </c>
-      <c r="AB20" s="9" t="s">
+      <c r="AB20" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC20" s="9" t="n">
+      <c r="AC20" s="10" t="n">
         <v>20270</v>
       </c>
-      <c r="AD20" s="9" t="n">
+      <c r="AD20" s="10" t="n">
         <v>1.8</v>
       </c>
-      <c r="AE20" s="9" t="s">
+      <c r="AE20" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AQ20" s="11"/>
-      <c r="AS20" s="11"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AQ20" s="12"/>
+      <c r="AS20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="n">
         <v>1015</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D21" s="14" t="n">
         <v>100</v>
@@ -3716,94 +3719,94 @@
         <v>3</v>
       </c>
       <c r="F21" s="14"/>
-      <c r="G21" s="13" t="n">
+      <c r="G21" s="3" t="n">
         <v>130536</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="3" t="s">
         <v>178</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="L21" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="P21" s="9" t="s">
-        <v>220</v>
+      <c r="L21" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="P21" s="10" t="s">
+        <v>221</v>
       </c>
       <c r="Q21" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T21" s="9" t="n">
+      <c r="T21" s="10" t="n">
         <v>200133</v>
       </c>
-      <c r="U21" s="9" t="n">
+      <c r="U21" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V21" s="9" t="s">
+      <c r="V21" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="W21" s="9" t="s">
+      <c r="W21" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="X21" s="9" t="s">
+      <c r="X21" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Y21" s="9" t="s">
+      <c r="Y21" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Z21" s="9" t="s">
+      <c r="Z21" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="AA21" s="9" t="n">
+      <c r="AA21" s="10" t="n">
         <v>144183</v>
       </c>
-      <c r="AB21" s="9" t="s">
+      <c r="AB21" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC21" s="9" t="n">
+      <c r="AC21" s="10" t="n">
         <v>20270</v>
       </c>
-      <c r="AD21" s="9" t="n">
+      <c r="AD21" s="10" t="n">
         <v>1.8</v>
       </c>
-      <c r="AE21" s="9" t="s">
+      <c r="AE21" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AQ21" s="11"/>
-      <c r="AR21" s="8"/>
-      <c r="AS21" s="11"/>
-      <c r="AV21" s="8"/>
-      <c r="AY21" s="8"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AQ21" s="12"/>
+      <c r="AR21" s="9"/>
+      <c r="AS21" s="12"/>
+      <c r="AV21" s="9"/>
+      <c r="AY21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="n">
         <v>1016</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D22" s="9" t="n">
+        <v>230</v>
+      </c>
+      <c r="D22" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="E22" s="9" t="n">
+      <c r="E22" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="13" t="n">
+      <c r="G22" s="3" t="n">
         <v>326241</v>
       </c>
       <c r="H22" s="18" t="s">
@@ -3812,71 +3815,71 @@
       <c r="I22" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J22" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="K22" s="10" t="s">
+      <c r="J22" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="K22" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="P22" s="9" t="s">
+      <c r="L22" s="10" t="s">
         <v>233</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>234</v>
       </c>
       <c r="Q22" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T22" s="9" t="n">
+      <c r="T22" s="10" t="n">
         <v>150929</v>
       </c>
-      <c r="U22" s="9" t="n">
+      <c r="U22" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V22" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="W22" s="9" t="s">
+      <c r="V22" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="W22" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X22" s="9" t="s">
+      <c r="X22" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y22" s="9" t="s">
+      <c r="Y22" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="Z22" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="AA22" s="9" t="n">
+      <c r="Z22" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="AA22" s="10" t="n">
         <v>122546</v>
       </c>
-      <c r="AB22" s="9" t="s">
+      <c r="AB22" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC22" s="9" t="n">
+      <c r="AC22" s="10" t="n">
         <v>135369</v>
       </c>
-      <c r="AD22" s="9" t="n">
+      <c r="AD22" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="AE22" s="9" t="s">
+      <c r="AE22" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
-      <c r="AQ22" s="11"/>
-      <c r="AS22" s="11"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AQ22" s="12"/>
+      <c r="AS22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="n">
         <v>1017</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D23" s="26" t="n">
         <v>300</v>
@@ -3889,7 +3892,7 @@
         <v>326271</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I23" s="29" t="s">
         <v>187</v>
@@ -3901,73 +3904,73 @@
         <v>188</v>
       </c>
       <c r="L23" s="31" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M23" s="32"/>
       <c r="N23" s="32"/>
       <c r="O23" s="32"/>
-      <c r="P23" s="9"/>
+      <c r="P23" s="10"/>
       <c r="Q23" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9" t="n">
+      <c r="T23" s="10"/>
+      <c r="U23" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V23" s="9" t="s">
+      <c r="V23" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="W23" s="9" t="s">
+      <c r="W23" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X23" s="9" t="s">
+      <c r="X23" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Y23" s="9" t="s">
+      <c r="Y23" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Z23" s="9" t="s">
+      <c r="Z23" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="9" t="n">
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10" t="n">
         <v>20270</v>
       </c>
-      <c r="AD23" s="9"/>
-      <c r="AE23" s="9" t="s">
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF23" s="10" t="s">
+      <c r="AF23" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="AG23" s="9"/>
-      <c r="AQ23" s="11"/>
-      <c r="AR23" s="8"/>
-      <c r="AS23" s="11"/>
-      <c r="AV23" s="8"/>
-      <c r="AY23" s="8"/>
+      <c r="AG23" s="10"/>
+      <c r="AQ23" s="12"/>
+      <c r="AR23" s="9"/>
+      <c r="AS23" s="12"/>
+      <c r="AV23" s="9"/>
+      <c r="AY23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>1018</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D24" s="9" t="n">
+        <v>239</v>
+      </c>
+      <c r="D24" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="E24" s="9" t="n">
+      <c r="E24" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="13" t="n">
+      <c r="G24" s="3" t="n">
         <v>143689</v>
       </c>
       <c r="H24" s="18" t="s">
@@ -3976,74 +3979,74 @@
       <c r="I24" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J24" s="13" t="s">
-        <v>239</v>
+      <c r="J24" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="L24" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="P24" s="9" t="s">
+      <c r="L24" s="10" t="s">
         <v>241</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>242</v>
       </c>
       <c r="Q24" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T24" s="9" t="n">
+      <c r="T24" s="10" t="n">
         <v>254300</v>
       </c>
-      <c r="U24" s="9" t="n">
+      <c r="U24" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V24" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="W24" s="9" t="s">
+      <c r="V24" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="W24" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X24" s="9" t="s">
+      <c r="X24" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y24" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="Z24" s="9" t="s">
+      <c r="Y24" s="10" t="s">
         <v>244</v>
+      </c>
+      <c r="Z24" s="10" t="s">
+        <v>245</v>
       </c>
       <c r="AA24" s="14" t="n">
         <v>285370</v>
       </c>
-      <c r="AB24" s="9" t="s">
+      <c r="AB24" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC24" s="9" t="n">
+      <c r="AC24" s="10" t="n">
         <v>279685</v>
       </c>
-      <c r="AD24" s="9" t="n">
+      <c r="AD24" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="AE24" s="9" t="s">
+      <c r="AE24" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF24" s="9"/>
-      <c r="AG24" s="9"/>
-      <c r="AQ24" s="11"/>
-      <c r="AR24" s="8"/>
-      <c r="AS24" s="11"/>
-      <c r="AV24" s="8"/>
-      <c r="AY24" s="8"/>
+      <c r="AF24" s="10"/>
+      <c r="AG24" s="10"/>
+      <c r="AQ24" s="12"/>
+      <c r="AR24" s="9"/>
+      <c r="AS24" s="12"/>
+      <c r="AV24" s="9"/>
+      <c r="AY24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>1019</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D25" s="14" t="n">
         <v>160</v>
@@ -4051,7 +4054,7 @@
       <c r="E25" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="10" t="s">
         <v>75</v>
       </c>
       <c r="G25" s="14" t="n">
@@ -4060,164 +4063,164 @@
       <c r="H25" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I25" s="10" t="s">
         <v>77</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="L25" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="P25" s="9" t="s">
+      <c r="K25" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="L25" s="10" t="s">
         <v>248</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>249</v>
       </c>
       <c r="Q25" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T25" s="9" t="n">
+      <c r="T25" s="10" t="n">
         <v>150927</v>
       </c>
-      <c r="U25" s="9" t="n">
+      <c r="U25" s="10" t="n">
         <v>1.3</v>
       </c>
-      <c r="V25" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="W25" s="9" t="s">
+      <c r="V25" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="X25" s="9" t="s">
+      <c r="W25" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="X25" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y25" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="Z25" s="9" t="s">
+      <c r="Y25" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="AA25" s="9" t="n">
+      <c r="Z25" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA25" s="10" t="n">
         <v>146119</v>
       </c>
-      <c r="AB25" s="9" t="s">
+      <c r="AB25" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC25" s="9" t="n">
+      <c r="AC25" s="10" t="n">
         <v>279672</v>
       </c>
-      <c r="AD25" s="9" t="n">
+      <c r="AD25" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AE25" s="9" t="s">
+      <c r="AE25" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF25" s="9"/>
-      <c r="AG25" s="9"/>
-      <c r="AQ25" s="11"/>
-      <c r="AR25" s="8"/>
-      <c r="AS25" s="11"/>
-      <c r="AV25" s="8"/>
-      <c r="AY25" s="8"/>
+      <c r="AF25" s="10"/>
+      <c r="AG25" s="10"/>
+      <c r="AQ25" s="12"/>
+      <c r="AR25" s="9"/>
+      <c r="AS25" s="12"/>
+      <c r="AV25" s="9"/>
+      <c r="AY25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>1020</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D26" s="9" t="n">
+        <v>254</v>
+      </c>
+      <c r="D26" s="10" t="n">
         <v>70</v>
       </c>
-      <c r="E26" s="9" t="n">
+      <c r="E26" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="9" t="n">
+      <c r="G26" s="10" t="n">
         <v>326236</v>
       </c>
       <c r="H26" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J26" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="L26" s="9" t="s">
+      <c r="J26" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="P26" s="9" t="s">
+      <c r="K26" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="L26" s="10" t="s">
         <v>256</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>257</v>
       </c>
       <c r="Q26" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T26" s="9" t="n">
+      <c r="T26" s="10" t="n">
         <v>181026</v>
       </c>
-      <c r="U26" s="9" t="n">
+      <c r="U26" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V26" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="W26" s="9" t="s">
+      <c r="V26" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="W26" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X26" s="9" t="s">
+      <c r="X26" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y26" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="Z26" s="9" t="s">
+      <c r="Y26" s="10" t="s">
         <v>259</v>
+      </c>
+      <c r="Z26" s="10" t="s">
+        <v>260</v>
       </c>
       <c r="AA26" s="14" t="n">
         <v>144198</v>
       </c>
-      <c r="AB26" s="9" t="s">
+      <c r="AB26" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC26" s="9" t="n">
+      <c r="AC26" s="10" t="n">
         <v>285283</v>
       </c>
-      <c r="AD26" s="9" t="n">
+      <c r="AD26" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="AE26" s="9" t="s">
+      <c r="AE26" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AQ26" s="11"/>
-      <c r="AR26" s="8"/>
-      <c r="AS26" s="11"/>
-      <c r="AV26" s="8"/>
-      <c r="AY26" s="8"/>
+      <c r="AF26" s="10"/>
+      <c r="AG26" s="10"/>
+      <c r="AQ26" s="12"/>
+      <c r="AR26" s="9"/>
+      <c r="AS26" s="12"/>
+      <c r="AV26" s="9"/>
+      <c r="AY26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>1021</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D27" s="14" t="n">
         <v>80</v>
@@ -4225,7 +4228,7 @@
       <c r="E27" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="10" t="s">
         <v>75</v>
       </c>
       <c r="G27" s="14" t="n">
@@ -4234,74 +4237,74 @@
       <c r="H27" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="K27" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="L27" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="P27" s="9" t="s">
+      <c r="J27" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L27" s="10" t="s">
         <v>262</v>
+      </c>
+      <c r="P27" s="10" t="s">
+        <v>263</v>
       </c>
       <c r="Q27" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T27" s="9" t="n">
+      <c r="T27" s="10" t="n">
         <v>151069</v>
       </c>
-      <c r="U27" s="9" t="n">
+      <c r="U27" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="V27" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="W27" s="9" t="s">
+      <c r="V27" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="X27" s="9" t="s">
+      <c r="W27" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="X27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y27" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="Z27" s="9" t="s">
+      <c r="Y27" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="AA27" s="9" t="n">
+      <c r="Z27" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="AA27" s="10" t="n">
         <v>281886</v>
       </c>
-      <c r="AB27" s="9" t="s">
+      <c r="AB27" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC27" s="9" t="n">
+      <c r="AC27" s="10" t="n">
         <v>281763</v>
       </c>
-      <c r="AD27" s="9" t="n">
+      <c r="AD27" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="AE27" s="9" t="s">
+      <c r="AE27" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF27" s="9"/>
-      <c r="AG27" s="9"/>
-      <c r="AQ27" s="11"/>
-      <c r="AS27" s="11"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AQ27" s="12"/>
+      <c r="AS27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>1022</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D28" s="14" t="n">
         <v>100</v>
@@ -4309,509 +4312,509 @@
       <c r="E28" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="10" t="n">
+      <c r="G28" s="11" t="n">
         <v>130536</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="I28" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="I28" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="J28" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="L28" s="9" t="s">
+      <c r="J28" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="9" t="s">
-        <v>220</v>
+      <c r="K28" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="10" t="s">
+        <v>221</v>
       </c>
       <c r="Q28" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T28" s="9" t="n">
+      <c r="T28" s="10" t="n">
         <v>200133</v>
       </c>
-      <c r="U28" s="9" t="n">
+      <c r="U28" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V28" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="W28" s="9" t="s">
+      <c r="V28" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="W28" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="X28" s="9" t="s">
+      <c r="X28" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Y28" s="9" t="s">
+      <c r="Y28" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Z28" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="AA28" s="9" t="n">
+      <c r="Z28" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="AA28" s="10" t="n">
         <v>144183</v>
       </c>
-      <c r="AB28" s="9" t="s">
+      <c r="AB28" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC28" s="9" t="n">
+      <c r="AC28" s="10" t="n">
         <v>20270</v>
       </c>
-      <c r="AD28" s="9" t="n">
+      <c r="AD28" s="10" t="n">
         <v>1.8</v>
       </c>
-      <c r="AE28" s="9" t="s">
+      <c r="AE28" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF28" s="9"/>
-      <c r="AG28" s="9"/>
-      <c r="AQ28" s="11"/>
-      <c r="AR28" s="8"/>
-      <c r="AS28" s="11"/>
-      <c r="AV28" s="8"/>
-      <c r="AY28" s="8"/>
+      <c r="AF28" s="10"/>
+      <c r="AG28" s="10"/>
+      <c r="AQ28" s="12"/>
+      <c r="AR28" s="9"/>
+      <c r="AS28" s="12"/>
+      <c r="AV28" s="9"/>
+      <c r="AY28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="n">
+      <c r="A29" s="10" t="n">
         <v>1023</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="D29" s="9" t="n">
+      <c r="B29" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="D29" s="10" t="n">
         <v>150</v>
       </c>
-      <c r="E29" s="9" t="n">
+      <c r="E29" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9" t="n">
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="n">
         <v>129508</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="I29" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="I29" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="L29" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="P29" s="9"/>
+      <c r="L29" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="P29" s="10"/>
       <c r="Q29" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9" t="n">
+      <c r="T29" s="10"/>
+      <c r="U29" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V29" s="9" t="s">
+      <c r="V29" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="W29" s="9" t="s">
+      <c r="W29" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="X29" s="9" t="s">
+      <c r="X29" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Y29" s="9" t="s">
+      <c r="Y29" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Z29" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="AA29" s="9"/>
-      <c r="AB29" s="9"/>
-      <c r="AC29" s="9" t="n">
+      <c r="Z29" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="10"/>
+      <c r="AC29" s="10" t="n">
         <v>20270</v>
       </c>
-      <c r="AD29" s="9"/>
-      <c r="AE29" s="9" t="s">
+      <c r="AD29" s="10"/>
+      <c r="AE29" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF29" s="10" t="s">
+      <c r="AF29" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="AG29" s="9"/>
+      <c r="AG29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="n">
+      <c r="A30" s="10" t="n">
         <v>1024</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="D30" s="9" t="n">
+      <c r="B30" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="D30" s="10" t="n">
         <v>250</v>
       </c>
-      <c r="E30" s="9" t="n">
+      <c r="E30" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9" t="n">
+      <c r="F30" s="10"/>
+      <c r="G30" s="10" t="n">
         <v>319126</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="I30" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="I30" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="J30" s="10" t="s">
+      <c r="J30" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="K30" s="10" t="s">
+      <c r="K30" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="L30" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="P30" s="9"/>
+      <c r="L30" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="P30" s="10"/>
       <c r="Q30" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9" t="n">
+      <c r="T30" s="10"/>
+      <c r="U30" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V30" s="9" t="s">
+      <c r="V30" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="W30" s="9" t="s">
+      <c r="W30" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X30" s="9" t="s">
+      <c r="X30" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Y30" s="9" t="s">
+      <c r="Y30" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Z30" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="AA30" s="9"/>
-      <c r="AB30" s="9"/>
-      <c r="AC30" s="9" t="n">
+      <c r="Z30" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="10" t="n">
         <v>20270</v>
       </c>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="9" t="s">
+      <c r="AD30" s="10"/>
+      <c r="AE30" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF30" s="10" t="s">
+      <c r="AF30" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="AG30" s="9"/>
+      <c r="AG30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="n">
+      <c r="A31" s="10" t="n">
         <v>1025</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D31" s="9" t="n">
+      <c r="B31" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D31" s="10" t="n">
         <v>400</v>
       </c>
-      <c r="E31" s="9" t="n">
+      <c r="E31" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="9" t="n">
+      <c r="G31" s="10" t="n">
         <v>326261</v>
       </c>
       <c r="H31" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J31" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="L31" s="9" t="s">
+      <c r="J31" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="P31" s="9" t="s">
+      <c r="K31" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="L31" s="10" t="s">
         <v>280</v>
+      </c>
+      <c r="P31" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="Q31" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T31" s="9" t="n">
+      <c r="T31" s="10" t="n">
         <v>151576</v>
       </c>
-      <c r="U31" s="9" t="n">
+      <c r="U31" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="V31" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="W31" s="9" t="s">
+      <c r="V31" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W31" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="X31" s="9" t="s">
+      <c r="X31" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y31" s="9" t="s">
+      <c r="Y31" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="Z31" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="AA31" s="9" t="n">
+      <c r="Z31" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="AA31" s="10" t="n">
         <v>281788</v>
       </c>
-      <c r="AB31" s="9" t="s">
+      <c r="AB31" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC31" s="9" t="n">
+      <c r="AC31" s="10" t="n">
         <v>268572</v>
       </c>
-      <c r="AD31" s="9" t="n">
+      <c r="AD31" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="AE31" s="9" t="s">
+      <c r="AE31" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF31" s="9"/>
-      <c r="AG31" s="9"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="n">
+      <c r="A32" s="10" t="n">
         <v>1026</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="D32" s="9" t="n">
+      <c r="B32" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D32" s="10" t="n">
         <v>210</v>
       </c>
-      <c r="E32" s="9" t="n">
+      <c r="E32" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="9" t="n">
+      <c r="G32" s="10" t="n">
         <v>326270</v>
       </c>
       <c r="H32" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J32" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="L32" s="9" t="s">
+      <c r="J32" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="P32" s="9" t="s">
+      <c r="K32" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="L32" s="10" t="s">
         <v>286</v>
+      </c>
+      <c r="P32" s="10" t="s">
+        <v>287</v>
       </c>
       <c r="Q32" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T32" s="9" t="n">
+      <c r="T32" s="10" t="n">
         <v>168944</v>
       </c>
-      <c r="U32" s="9" t="n">
+      <c r="U32" s="10" t="n">
         <v>0.3</v>
       </c>
-      <c r="V32" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="W32" s="9" t="s">
+      <c r="V32" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="W32" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="X32" s="9" t="s">
+      <c r="X32" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y32" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="Z32" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="AA32" s="9" t="n">
+      <c r="Y32" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z32" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="AA32" s="10" t="n">
         <v>285400</v>
       </c>
-      <c r="AB32" s="9" t="s">
+      <c r="AB32" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC32" s="9" t="n">
+      <c r="AC32" s="10" t="n">
         <v>85955</v>
       </c>
-      <c r="AD32" s="9" t="n">
+      <c r="AD32" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="AE32" s="9" t="s">
+      <c r="AE32" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF32" s="9"/>
-      <c r="AG32" s="9"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="n">
+      <c r="A33" s="10" t="n">
         <v>1027</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D33" s="9" t="n">
+      <c r="B33" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D33" s="10" t="n">
         <v>500</v>
       </c>
-      <c r="E33" s="9" t="n">
+      <c r="E33" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="9" t="n">
+      <c r="G33" s="10" t="n">
         <v>142127</v>
       </c>
       <c r="H33" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J33" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="L33" s="9" t="s">
+      <c r="J33" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="P33" s="9" t="s">
+      <c r="K33" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="L33" s="10" t="s">
         <v>291</v>
+      </c>
+      <c r="P33" s="10" t="s">
+        <v>292</v>
       </c>
       <c r="Q33" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="T33" s="9" t="n">
+      <c r="T33" s="10" t="n">
         <v>99608</v>
       </c>
-      <c r="U33" s="9" t="n">
+      <c r="U33" s="10" t="n">
         <v>1.2</v>
       </c>
-      <c r="V33" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="W33" s="9" t="s">
+      <c r="V33" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="W33" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="X33" s="9" t="s">
+      <c r="X33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y33" s="9" t="s">
+      <c r="Y33" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="Z33" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="AA33" s="9" t="n">
+      <c r="Z33" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA33" s="10" t="n">
         <v>281710</v>
       </c>
-      <c r="AB33" s="9" t="s">
+      <c r="AB33" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC33" s="9" t="n">
+      <c r="AC33" s="10" t="n">
         <v>80483</v>
       </c>
-      <c r="AD33" s="9" t="n">
+      <c r="AD33" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="AE33" s="9" t="s">
+      <c r="AE33" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AF33" s="9"/>
-      <c r="AG33" s="9"/>
+      <c r="AF33" s="10"/>
+      <c r="AG33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>1028</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>294</v>
+      <c r="B34" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>295</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>270</v>
       </c>
-      <c r="E34" s="9" t="n">
+      <c r="E34" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G34" s="9" t="n">
+      <c r="G34" s="10" t="n">
         <v>326264</v>
       </c>
       <c r="H34" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="I34" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J34" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="L34" s="9" t="s">
+      <c r="J34" s="10" t="s">
         <v>296</v>
       </c>
+      <c r="K34" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="L34" s="10" t="s">
+        <v>297</v>
+      </c>
       <c r="P34" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="Q34" s="1" t="n">
         <v>16</v>
@@ -4822,25 +4825,25 @@
       <c r="U34" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="V34" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="W34" s="9" t="s">
+      <c r="V34" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="X34" s="9" t="s">
+      <c r="W34" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="X34" s="10" t="s">
         <v>84</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="Z34" s="9" t="s">
-        <v>300</v>
+        <v>265</v>
+      </c>
+      <c r="Z34" s="10" t="s">
+        <v>301</v>
       </c>
       <c r="AA34" s="1" t="n">
         <v>299561</v>
       </c>
-      <c r="AB34" s="9" t="s">
+      <c r="AB34" s="10" t="s">
         <v>173</v>
       </c>
       <c r="AC34" s="1" t="n">
@@ -4849,7 +4852,7 @@
       <c r="AD34" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="AE34" s="9" t="s">
+      <c r="AE34" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4858,10 +4861,10 @@
         <v>1029</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>550</v>
@@ -4869,7 +4872,7 @@
       <c r="E35" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="10" t="s">
         <v>75</v>
       </c>
       <c r="G35" s="1" t="n">
@@ -4878,26 +4881,29 @@
       <c r="H35" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J35" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="L35" s="9" t="s">
+      <c r="J35" s="10" t="s">
         <v>303</v>
       </c>
+      <c r="K35" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="L35" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O35" s="22" t="s">
+        <v>210</v>
+      </c>
       <c r="P35" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="Q35" s="1" t="n">
         <v>16</v>
       </c>
       <c r="S35" s="22" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="T35" s="1" t="n">
         <v>130642</v>
@@ -4905,34 +4911,34 @@
       <c r="U35" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="V35" s="9" t="s">
+      <c r="V35" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="W35" s="9" t="s">
+      <c r="W35" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="X35" s="9" t="s">
+      <c r="X35" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y35" s="9" t="s">
+      <c r="Y35" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="Z35" s="9" t="s">
-        <v>305</v>
+      <c r="Z35" s="10" t="s">
+        <v>306</v>
       </c>
       <c r="AA35" s="1" t="n">
         <v>285356</v>
       </c>
-      <c r="AB35" s="9" t="s">
+      <c r="AB35" s="10" t="s">
         <v>173</v>
       </c>
       <c r="AC35" s="22" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AD35" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AE35" s="9" t="s">
+      <c r="AE35" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4941,10 +4947,10 @@
         <v>1030</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>300</v>
@@ -4952,7 +4958,7 @@
       <c r="E36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="10" t="s">
         <v>75</v>
       </c>
       <c r="G36" s="1" t="n">
@@ -4961,26 +4967,29 @@
       <c r="H36" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J36" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="L36" s="9" t="s">
+      <c r="J36" s="10" t="s">
         <v>309</v>
       </c>
+      <c r="K36" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="L36" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="O36" s="22" t="s">
+        <v>210</v>
+      </c>
       <c r="P36" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q36" s="1" t="n">
         <v>16</v>
       </c>
       <c r="S36" s="22" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="T36" s="1" t="n">
         <v>254276</v>
@@ -4988,34 +4997,34 @@
       <c r="U36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="V36" s="9" t="s">
+      <c r="V36" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="W36" s="9" t="s">
+      <c r="W36" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X36" s="9" t="s">
+      <c r="X36" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y36" s="9" t="s">
+      <c r="Y36" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="Z36" s="9" t="s">
-        <v>312</v>
+      <c r="Z36" s="10" t="s">
+        <v>313</v>
       </c>
       <c r="AA36" s="1" t="n">
         <v>20301</v>
       </c>
-      <c r="AB36" s="9" t="s">
+      <c r="AB36" s="10" t="s">
         <v>173</v>
       </c>
       <c r="AC36" s="22" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AD36" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AE36" s="9" t="s">
+      <c r="AE36" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -5024,10 +5033,10 @@
         <v>1031</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>180</v>
@@ -5035,7 +5044,7 @@
       <c r="E37" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="10" t="s">
         <v>75</v>
       </c>
       <c r="G37" s="1" t="n">
@@ -5044,20 +5053,20 @@
       <c r="H37" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="I37" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J37" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="L37" s="9" t="s">
+      <c r="J37" s="10" t="s">
         <v>316</v>
       </c>
+      <c r="K37" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>317</v>
+      </c>
       <c r="P37" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="Q37" s="1" t="n">
         <v>16</v>
@@ -5068,34 +5077,34 @@
       <c r="U37" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="V37" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="W37" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="X37" s="9" t="s">
+      <c r="V37" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="W37" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="X37" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Y37" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="Z37" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="AA37" s="9" t="n">
+      <c r="Y37" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="Z37" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="AA37" s="10" t="n">
         <v>281710</v>
       </c>
-      <c r="AB37" s="9" t="s">
+      <c r="AB37" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="AC37" s="9" t="n">
+      <c r="AC37" s="10" t="n">
         <v>80483</v>
       </c>
       <c r="AD37" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="AE37" s="9" t="s">
+      <c r="AE37" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -5104,10 +5113,10 @@
         <v>1032</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>80</v>
@@ -5115,7 +5124,7 @@
       <c r="E38" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="10" t="s">
         <v>75</v>
       </c>
       <c r="G38" s="1" t="n">
@@ -5124,20 +5133,20 @@
       <c r="H38" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J38" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="K38" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="L38" s="9" t="s">
+      <c r="J38" s="10" t="s">
         <v>322</v>
       </c>
+      <c r="K38" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>323</v>
+      </c>
       <c r="P38" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Q38" s="1" t="n">
         <v>16</v>

</xml_diff>

<commit_message>
feat：update soil tower excel
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="466">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -1870,7 +1870,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2052,6 +2052,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2241,9 +2245,9 @@
   <dimension ref="A1:AMS54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="R28" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="0" topLeftCell="AF28" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
-      <selection pane="topRight" activeCell="R52" activeCellId="0" sqref="R52"/>
+      <selection pane="topRight" activeCell="AI59" activeCellId="0" sqref="AI59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38850,7 +38854,7 @@
       <c r="AMR48" s="27"/>
       <c r="AMS48" s="27"/>
     </row>
-    <row r="49" s="45" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="19" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="n">
         <v>1043</v>
       </c>
@@ -39951,7 +39955,7 @@
       <c r="AMR49" s="15"/>
       <c r="AMS49" s="15"/>
     </row>
-    <row r="50" s="45" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="19" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="n">
         <v>1044</v>
       </c>
@@ -41048,7 +41052,7 @@
       <c r="AMR50" s="15"/>
       <c r="AMS50" s="15"/>
     </row>
-    <row r="51" s="45" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" s="19" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="n">
         <v>1045</v>
       </c>
@@ -42149,296 +42153,3298 @@
       <c r="AMR51" s="15"/>
       <c r="AMS51" s="15"/>
     </row>
-    <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="n">
+    <row r="52" s="45" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="11" t="n">
         <v>1046</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="C52" s="1" t="n">
+      <c r="C52" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="D52" s="1" t="n">
+      <c r="D52" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="15" t="s">
         <v>451</v>
       </c>
-      <c r="F52" s="1" t="n">
+      <c r="F52" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="G52" s="1" t="n">
+      <c r="G52" s="15" t="n">
         <v>620</v>
       </c>
-      <c r="H52" s="1" t="n">
+      <c r="H52" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="I52" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="J52" s="1" t="n">
+      <c r="J52" s="15" t="n">
         <v>392709</v>
       </c>
-      <c r="K52" s="7" t="s">
+      <c r="K52" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="L52" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="M52" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="N52" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="O52" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="P52" s="15" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q52" s="15" t="n">
+        <v>29</v>
+      </c>
+      <c r="R52" s="15" t="n">
+        <v>500</v>
+      </c>
+      <c r="S52" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="T52" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="U52" s="15"/>
+      <c r="V52" s="15" t="n">
+        <v>500</v>
+      </c>
+      <c r="W52" s="15" t="n">
+        <v>89088</v>
+      </c>
+      <c r="X52" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="Z52" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA52" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB52" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC52" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="AD52" s="15" t="n">
+        <v>144183</v>
+      </c>
+      <c r="AE52" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF52" s="15" t="n">
+        <v>279726</v>
+      </c>
+      <c r="AG52" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH52" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI52" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="AJ52" s="15"/>
+      <c r="AK52" s="15"/>
+      <c r="AL52" s="15"/>
+      <c r="AM52" s="15"/>
+      <c r="AN52" s="15"/>
+      <c r="AO52" s="15"/>
+      <c r="AP52" s="15"/>
+      <c r="AQ52" s="15"/>
+      <c r="AR52" s="15"/>
+      <c r="AS52" s="15"/>
+      <c r="AT52" s="11"/>
+      <c r="AU52" s="15"/>
+      <c r="AV52" s="11"/>
+      <c r="AW52" s="15"/>
+      <c r="AX52" s="15"/>
+      <c r="AY52" s="15"/>
+      <c r="AZ52" s="15"/>
+      <c r="BA52" s="15"/>
+      <c r="BB52" s="15"/>
+      <c r="BC52" s="15"/>
+      <c r="BD52" s="15"/>
+      <c r="BE52" s="15"/>
+      <c r="BF52" s="15"/>
+      <c r="BG52" s="15"/>
+      <c r="BH52" s="15"/>
+      <c r="BI52" s="15"/>
+      <c r="BJ52" s="15"/>
+      <c r="BK52" s="15"/>
+      <c r="BL52" s="15"/>
+      <c r="BM52" s="15"/>
+      <c r="BN52" s="15"/>
+      <c r="BO52" s="15"/>
+      <c r="BP52" s="15"/>
+      <c r="BQ52" s="15"/>
+      <c r="BR52" s="15"/>
+      <c r="BS52" s="15"/>
+      <c r="BT52" s="15"/>
+      <c r="BU52" s="15"/>
+      <c r="BV52" s="15"/>
+      <c r="BW52" s="15"/>
+      <c r="BX52" s="15"/>
+      <c r="BY52" s="15"/>
+      <c r="BZ52" s="15"/>
+      <c r="CA52" s="15"/>
+      <c r="CB52" s="15"/>
+      <c r="CC52" s="15"/>
+      <c r="CD52" s="15"/>
+      <c r="CE52" s="15"/>
+      <c r="CF52" s="15"/>
+      <c r="CG52" s="15"/>
+      <c r="CH52" s="15"/>
+      <c r="CI52" s="15"/>
+      <c r="CJ52" s="15"/>
+      <c r="CK52" s="15"/>
+      <c r="CL52" s="15"/>
+      <c r="CM52" s="15"/>
+      <c r="CN52" s="15"/>
+      <c r="CO52" s="15"/>
+      <c r="CP52" s="15"/>
+      <c r="CQ52" s="15"/>
+      <c r="CR52" s="15"/>
+      <c r="CS52" s="15"/>
+      <c r="CT52" s="15"/>
+      <c r="CU52" s="15"/>
+      <c r="CV52" s="15"/>
+      <c r="CW52" s="15"/>
+      <c r="CX52" s="15"/>
+      <c r="CY52" s="15"/>
+      <c r="CZ52" s="15"/>
+      <c r="DA52" s="15"/>
+      <c r="DB52" s="15"/>
+      <c r="DC52" s="15"/>
+      <c r="DD52" s="15"/>
+      <c r="DE52" s="15"/>
+      <c r="DF52" s="15"/>
+      <c r="DG52" s="15"/>
+      <c r="DH52" s="15"/>
+      <c r="DI52" s="15"/>
+      <c r="DJ52" s="15"/>
+      <c r="DK52" s="15"/>
+      <c r="DL52" s="15"/>
+      <c r="DM52" s="15"/>
+      <c r="DN52" s="15"/>
+      <c r="DO52" s="15"/>
+      <c r="DP52" s="15"/>
+      <c r="DQ52" s="15"/>
+      <c r="DR52" s="15"/>
+      <c r="DS52" s="15"/>
+      <c r="DT52" s="15"/>
+      <c r="DU52" s="15"/>
+      <c r="DV52" s="15"/>
+      <c r="DW52" s="15"/>
+      <c r="DX52" s="15"/>
+      <c r="DY52" s="15"/>
+      <c r="DZ52" s="15"/>
+      <c r="EA52" s="15"/>
+      <c r="EB52" s="15"/>
+      <c r="EC52" s="15"/>
+      <c r="ED52" s="15"/>
+      <c r="EE52" s="15"/>
+      <c r="EF52" s="15"/>
+      <c r="EG52" s="15"/>
+      <c r="EH52" s="15"/>
+      <c r="EI52" s="15"/>
+      <c r="EJ52" s="15"/>
+      <c r="EK52" s="15"/>
+      <c r="EL52" s="15"/>
+      <c r="EM52" s="15"/>
+      <c r="EN52" s="15"/>
+      <c r="EO52" s="15"/>
+      <c r="EP52" s="15"/>
+      <c r="EQ52" s="15"/>
+      <c r="ER52" s="15"/>
+      <c r="ES52" s="15"/>
+      <c r="ET52" s="15"/>
+      <c r="EU52" s="15"/>
+      <c r="EV52" s="15"/>
+      <c r="EW52" s="15"/>
+      <c r="EX52" s="15"/>
+      <c r="EY52" s="15"/>
+      <c r="EZ52" s="15"/>
+      <c r="FA52" s="15"/>
+      <c r="FB52" s="15"/>
+      <c r="FC52" s="15"/>
+      <c r="FD52" s="15"/>
+      <c r="FE52" s="15"/>
+      <c r="FF52" s="15"/>
+      <c r="FG52" s="15"/>
+      <c r="FH52" s="15"/>
+      <c r="FI52" s="15"/>
+      <c r="FJ52" s="15"/>
+      <c r="FK52" s="15"/>
+      <c r="FL52" s="15"/>
+      <c r="FM52" s="15"/>
+      <c r="FN52" s="15"/>
+      <c r="FO52" s="15"/>
+      <c r="FP52" s="15"/>
+      <c r="FQ52" s="15"/>
+      <c r="FR52" s="15"/>
+      <c r="FS52" s="15"/>
+      <c r="FT52" s="15"/>
+      <c r="FU52" s="15"/>
+      <c r="FV52" s="15"/>
+      <c r="FW52" s="15"/>
+      <c r="FX52" s="15"/>
+      <c r="FY52" s="15"/>
+      <c r="FZ52" s="15"/>
+      <c r="GA52" s="15"/>
+      <c r="GB52" s="15"/>
+      <c r="GC52" s="15"/>
+      <c r="GD52" s="15"/>
+      <c r="GE52" s="15"/>
+      <c r="GF52" s="15"/>
+      <c r="GG52" s="15"/>
+      <c r="GH52" s="15"/>
+      <c r="GI52" s="15"/>
+      <c r="GJ52" s="15"/>
+      <c r="GK52" s="15"/>
+      <c r="GL52" s="15"/>
+      <c r="GM52" s="15"/>
+      <c r="GN52" s="15"/>
+      <c r="GO52" s="15"/>
+      <c r="GP52" s="15"/>
+      <c r="GQ52" s="15"/>
+      <c r="GR52" s="15"/>
+      <c r="GS52" s="15"/>
+      <c r="GT52" s="15"/>
+      <c r="GU52" s="15"/>
+      <c r="GV52" s="15"/>
+      <c r="GW52" s="15"/>
+      <c r="GX52" s="15"/>
+      <c r="GY52" s="15"/>
+      <c r="GZ52" s="15"/>
+      <c r="HA52" s="15"/>
+      <c r="HB52" s="15"/>
+      <c r="HC52" s="15"/>
+      <c r="HD52" s="15"/>
+      <c r="HE52" s="15"/>
+      <c r="HF52" s="15"/>
+      <c r="HG52" s="15"/>
+      <c r="HH52" s="15"/>
+      <c r="HI52" s="15"/>
+      <c r="HJ52" s="15"/>
+      <c r="HK52" s="15"/>
+      <c r="HL52" s="15"/>
+      <c r="HM52" s="15"/>
+      <c r="HN52" s="15"/>
+      <c r="HO52" s="15"/>
+      <c r="HP52" s="15"/>
+      <c r="HQ52" s="15"/>
+      <c r="HR52" s="15"/>
+      <c r="HS52" s="15"/>
+      <c r="HT52" s="15"/>
+      <c r="HU52" s="15"/>
+      <c r="HV52" s="15"/>
+      <c r="HW52" s="15"/>
+      <c r="HX52" s="15"/>
+      <c r="HY52" s="15"/>
+      <c r="HZ52" s="15"/>
+      <c r="IA52" s="15"/>
+      <c r="IB52" s="15"/>
+      <c r="IC52" s="15"/>
+      <c r="ID52" s="15"/>
+      <c r="IE52" s="15"/>
+      <c r="IF52" s="15"/>
+      <c r="IG52" s="15"/>
+      <c r="IH52" s="15"/>
+      <c r="II52" s="15"/>
+      <c r="IJ52" s="15"/>
+      <c r="IK52" s="15"/>
+      <c r="IL52" s="15"/>
+      <c r="IM52" s="15"/>
+      <c r="IN52" s="15"/>
+      <c r="IO52" s="15"/>
+      <c r="IP52" s="15"/>
+      <c r="IQ52" s="15"/>
+      <c r="IR52" s="15"/>
+      <c r="IS52" s="15"/>
+      <c r="IT52" s="15"/>
+      <c r="IU52" s="15"/>
+      <c r="IV52" s="15"/>
+      <c r="IW52" s="15"/>
+      <c r="IX52" s="15"/>
+      <c r="IY52" s="15"/>
+      <c r="IZ52" s="15"/>
+      <c r="JA52" s="15"/>
+      <c r="JB52" s="15"/>
+      <c r="JC52" s="15"/>
+      <c r="JD52" s="15"/>
+      <c r="JE52" s="15"/>
+      <c r="JF52" s="15"/>
+      <c r="JG52" s="15"/>
+      <c r="JH52" s="15"/>
+      <c r="JI52" s="15"/>
+      <c r="JJ52" s="15"/>
+      <c r="JK52" s="15"/>
+      <c r="JL52" s="15"/>
+      <c r="JM52" s="15"/>
+      <c r="JN52" s="15"/>
+      <c r="JO52" s="15"/>
+      <c r="JP52" s="15"/>
+      <c r="JQ52" s="15"/>
+      <c r="JR52" s="15"/>
+      <c r="JS52" s="15"/>
+      <c r="JT52" s="15"/>
+      <c r="JU52" s="15"/>
+      <c r="JV52" s="15"/>
+      <c r="JW52" s="15"/>
+      <c r="JX52" s="15"/>
+      <c r="JY52" s="15"/>
+      <c r="JZ52" s="15"/>
+      <c r="KA52" s="15"/>
+      <c r="KB52" s="15"/>
+      <c r="KC52" s="15"/>
+      <c r="KD52" s="15"/>
+      <c r="KE52" s="15"/>
+      <c r="KF52" s="15"/>
+      <c r="KG52" s="15"/>
+      <c r="KH52" s="15"/>
+      <c r="KI52" s="15"/>
+      <c r="KJ52" s="15"/>
+      <c r="KK52" s="15"/>
+      <c r="KL52" s="15"/>
+      <c r="KM52" s="15"/>
+      <c r="KN52" s="15"/>
+      <c r="KO52" s="15"/>
+      <c r="KP52" s="15"/>
+      <c r="KQ52" s="15"/>
+      <c r="KR52" s="15"/>
+      <c r="KS52" s="15"/>
+      <c r="KT52" s="15"/>
+      <c r="KU52" s="15"/>
+      <c r="KV52" s="15"/>
+      <c r="KW52" s="15"/>
+      <c r="KX52" s="15"/>
+      <c r="KY52" s="15"/>
+      <c r="KZ52" s="15"/>
+      <c r="LA52" s="15"/>
+      <c r="LB52" s="15"/>
+      <c r="LC52" s="15"/>
+      <c r="LD52" s="15"/>
+      <c r="LE52" s="15"/>
+      <c r="LF52" s="15"/>
+      <c r="LG52" s="15"/>
+      <c r="LH52" s="15"/>
+      <c r="LI52" s="15"/>
+      <c r="LJ52" s="15"/>
+      <c r="LK52" s="15"/>
+      <c r="LL52" s="15"/>
+      <c r="LM52" s="15"/>
+      <c r="LN52" s="15"/>
+      <c r="LO52" s="15"/>
+      <c r="LP52" s="15"/>
+      <c r="LQ52" s="15"/>
+      <c r="LR52" s="15"/>
+      <c r="LS52" s="15"/>
+      <c r="LT52" s="15"/>
+      <c r="LU52" s="15"/>
+      <c r="LV52" s="15"/>
+      <c r="LW52" s="15"/>
+      <c r="LX52" s="15"/>
+      <c r="LY52" s="15"/>
+      <c r="LZ52" s="15"/>
+      <c r="MA52" s="15"/>
+      <c r="MB52" s="15"/>
+      <c r="MC52" s="15"/>
+      <c r="MD52" s="15"/>
+      <c r="ME52" s="15"/>
+      <c r="MF52" s="15"/>
+      <c r="MG52" s="15"/>
+      <c r="MH52" s="15"/>
+      <c r="MI52" s="15"/>
+      <c r="MJ52" s="15"/>
+      <c r="MK52" s="15"/>
+      <c r="ML52" s="15"/>
+      <c r="MM52" s="15"/>
+      <c r="MN52" s="15"/>
+      <c r="MO52" s="15"/>
+      <c r="MP52" s="15"/>
+      <c r="MQ52" s="15"/>
+      <c r="MR52" s="15"/>
+      <c r="MS52" s="15"/>
+      <c r="MT52" s="15"/>
+      <c r="MU52" s="15"/>
+      <c r="MV52" s="15"/>
+      <c r="MW52" s="15"/>
+      <c r="MX52" s="15"/>
+      <c r="MY52" s="15"/>
+      <c r="MZ52" s="15"/>
+      <c r="NA52" s="15"/>
+      <c r="NB52" s="15"/>
+      <c r="NC52" s="15"/>
+      <c r="ND52" s="15"/>
+      <c r="NE52" s="15"/>
+      <c r="NF52" s="15"/>
+      <c r="NG52" s="15"/>
+      <c r="NH52" s="15"/>
+      <c r="NI52" s="15"/>
+      <c r="NJ52" s="15"/>
+      <c r="NK52" s="15"/>
+      <c r="NL52" s="15"/>
+      <c r="NM52" s="15"/>
+      <c r="NN52" s="15"/>
+      <c r="NO52" s="15"/>
+      <c r="NP52" s="15"/>
+      <c r="NQ52" s="15"/>
+      <c r="NR52" s="15"/>
+      <c r="NS52" s="15"/>
+      <c r="NT52" s="15"/>
+      <c r="NU52" s="15"/>
+      <c r="NV52" s="15"/>
+      <c r="NW52" s="15"/>
+      <c r="NX52" s="15"/>
+      <c r="NY52" s="15"/>
+      <c r="NZ52" s="15"/>
+      <c r="OA52" s="15"/>
+      <c r="OB52" s="15"/>
+      <c r="OC52" s="15"/>
+      <c r="OD52" s="15"/>
+      <c r="OE52" s="15"/>
+      <c r="OF52" s="15"/>
+      <c r="OG52" s="15"/>
+      <c r="OH52" s="15"/>
+      <c r="OI52" s="15"/>
+      <c r="OJ52" s="15"/>
+      <c r="OK52" s="15"/>
+      <c r="OL52" s="15"/>
+      <c r="OM52" s="15"/>
+      <c r="ON52" s="15"/>
+      <c r="OO52" s="15"/>
+      <c r="OP52" s="15"/>
+      <c r="OQ52" s="15"/>
+      <c r="OR52" s="15"/>
+      <c r="OS52" s="15"/>
+      <c r="OT52" s="15"/>
+      <c r="OU52" s="15"/>
+      <c r="OV52" s="15"/>
+      <c r="OW52" s="15"/>
+      <c r="OX52" s="15"/>
+      <c r="OY52" s="15"/>
+      <c r="OZ52" s="15"/>
+      <c r="PA52" s="15"/>
+      <c r="PB52" s="15"/>
+      <c r="PC52" s="15"/>
+      <c r="PD52" s="15"/>
+      <c r="PE52" s="15"/>
+      <c r="PF52" s="15"/>
+      <c r="PG52" s="15"/>
+      <c r="PH52" s="15"/>
+      <c r="PI52" s="15"/>
+      <c r="PJ52" s="15"/>
+      <c r="PK52" s="15"/>
+      <c r="PL52" s="15"/>
+      <c r="PM52" s="15"/>
+      <c r="PN52" s="15"/>
+      <c r="PO52" s="15"/>
+      <c r="PP52" s="15"/>
+      <c r="PQ52" s="15"/>
+      <c r="PR52" s="15"/>
+      <c r="PS52" s="15"/>
+      <c r="PT52" s="15"/>
+      <c r="PU52" s="15"/>
+      <c r="PV52" s="15"/>
+      <c r="PW52" s="15"/>
+      <c r="PX52" s="15"/>
+      <c r="PY52" s="15"/>
+      <c r="PZ52" s="15"/>
+      <c r="QA52" s="15"/>
+      <c r="QB52" s="15"/>
+      <c r="QC52" s="15"/>
+      <c r="QD52" s="15"/>
+      <c r="QE52" s="15"/>
+      <c r="QF52" s="15"/>
+      <c r="QG52" s="15"/>
+      <c r="QH52" s="15"/>
+      <c r="QI52" s="15"/>
+      <c r="QJ52" s="15"/>
+      <c r="QK52" s="15"/>
+      <c r="QL52" s="15"/>
+      <c r="QM52" s="15"/>
+      <c r="QN52" s="15"/>
+      <c r="QO52" s="15"/>
+      <c r="QP52" s="15"/>
+      <c r="QQ52" s="15"/>
+      <c r="QR52" s="15"/>
+      <c r="QS52" s="15"/>
+      <c r="QT52" s="15"/>
+      <c r="QU52" s="15"/>
+      <c r="QV52" s="15"/>
+      <c r="QW52" s="15"/>
+      <c r="QX52" s="15"/>
+      <c r="QY52" s="15"/>
+      <c r="QZ52" s="15"/>
+      <c r="RA52" s="15"/>
+      <c r="RB52" s="15"/>
+      <c r="RC52" s="15"/>
+      <c r="RD52" s="15"/>
+      <c r="RE52" s="15"/>
+      <c r="RF52" s="15"/>
+      <c r="RG52" s="15"/>
+      <c r="RH52" s="15"/>
+      <c r="RI52" s="15"/>
+      <c r="RJ52" s="15"/>
+      <c r="RK52" s="15"/>
+      <c r="RL52" s="15"/>
+      <c r="RM52" s="15"/>
+      <c r="RN52" s="15"/>
+      <c r="RO52" s="15"/>
+      <c r="RP52" s="15"/>
+      <c r="RQ52" s="15"/>
+      <c r="RR52" s="15"/>
+      <c r="RS52" s="15"/>
+      <c r="RT52" s="15"/>
+      <c r="RU52" s="15"/>
+      <c r="RV52" s="15"/>
+      <c r="RW52" s="15"/>
+      <c r="RX52" s="15"/>
+      <c r="RY52" s="15"/>
+      <c r="RZ52" s="15"/>
+      <c r="SA52" s="15"/>
+      <c r="SB52" s="15"/>
+      <c r="SC52" s="15"/>
+      <c r="SD52" s="15"/>
+      <c r="SE52" s="15"/>
+      <c r="SF52" s="15"/>
+      <c r="SG52" s="15"/>
+      <c r="SH52" s="15"/>
+      <c r="SI52" s="15"/>
+      <c r="SJ52" s="15"/>
+      <c r="SK52" s="15"/>
+      <c r="SL52" s="15"/>
+      <c r="SM52" s="15"/>
+      <c r="SN52" s="15"/>
+      <c r="SO52" s="15"/>
+      <c r="SP52" s="15"/>
+      <c r="SQ52" s="15"/>
+      <c r="SR52" s="15"/>
+      <c r="SS52" s="15"/>
+      <c r="ST52" s="15"/>
+      <c r="SU52" s="15"/>
+      <c r="SV52" s="15"/>
+      <c r="SW52" s="15"/>
+      <c r="SX52" s="15"/>
+      <c r="SY52" s="15"/>
+      <c r="SZ52" s="15"/>
+      <c r="TA52" s="15"/>
+      <c r="TB52" s="15"/>
+      <c r="TC52" s="15"/>
+      <c r="TD52" s="15"/>
+      <c r="TE52" s="15"/>
+      <c r="TF52" s="15"/>
+      <c r="TG52" s="15"/>
+      <c r="TH52" s="15"/>
+      <c r="TI52" s="15"/>
+      <c r="TJ52" s="15"/>
+      <c r="TK52" s="15"/>
+      <c r="TL52" s="15"/>
+      <c r="TM52" s="15"/>
+      <c r="TN52" s="15"/>
+      <c r="TO52" s="15"/>
+      <c r="TP52" s="15"/>
+      <c r="TQ52" s="15"/>
+      <c r="TR52" s="15"/>
+      <c r="TS52" s="15"/>
+      <c r="TT52" s="15"/>
+      <c r="TU52" s="15"/>
+      <c r="TV52" s="15"/>
+      <c r="TW52" s="15"/>
+      <c r="TX52" s="15"/>
+      <c r="TY52" s="15"/>
+      <c r="TZ52" s="15"/>
+      <c r="UA52" s="15"/>
+      <c r="UB52" s="15"/>
+      <c r="UC52" s="15"/>
+      <c r="UD52" s="15"/>
+      <c r="UE52" s="15"/>
+      <c r="UF52" s="15"/>
+      <c r="UG52" s="15"/>
+      <c r="UH52" s="15"/>
+      <c r="UI52" s="15"/>
+      <c r="UJ52" s="15"/>
+      <c r="UK52" s="15"/>
+      <c r="UL52" s="15"/>
+      <c r="UM52" s="15"/>
+      <c r="UN52" s="15"/>
+      <c r="UO52" s="15"/>
+      <c r="UP52" s="15"/>
+      <c r="UQ52" s="15"/>
+      <c r="UR52" s="15"/>
+      <c r="US52" s="15"/>
+      <c r="UT52" s="15"/>
+      <c r="UU52" s="15"/>
+      <c r="UV52" s="15"/>
+      <c r="UW52" s="15"/>
+      <c r="UX52" s="15"/>
+      <c r="UY52" s="15"/>
+      <c r="UZ52" s="15"/>
+      <c r="VA52" s="15"/>
+      <c r="VB52" s="15"/>
+      <c r="VC52" s="15"/>
+      <c r="VD52" s="15"/>
+      <c r="VE52" s="15"/>
+      <c r="VF52" s="15"/>
+      <c r="VG52" s="15"/>
+      <c r="VH52" s="15"/>
+      <c r="VI52" s="15"/>
+      <c r="VJ52" s="15"/>
+      <c r="VK52" s="15"/>
+      <c r="VL52" s="15"/>
+      <c r="VM52" s="15"/>
+      <c r="VN52" s="15"/>
+      <c r="VO52" s="15"/>
+      <c r="VP52" s="15"/>
+      <c r="VQ52" s="15"/>
+      <c r="VR52" s="15"/>
+      <c r="VS52" s="15"/>
+      <c r="VT52" s="15"/>
+      <c r="VU52" s="15"/>
+      <c r="VV52" s="15"/>
+      <c r="VW52" s="15"/>
+      <c r="VX52" s="15"/>
+      <c r="VY52" s="15"/>
+      <c r="VZ52" s="15"/>
+      <c r="WA52" s="15"/>
+      <c r="WB52" s="15"/>
+      <c r="WC52" s="15"/>
+      <c r="WD52" s="15"/>
+      <c r="WE52" s="15"/>
+      <c r="WF52" s="15"/>
+      <c r="WG52" s="15"/>
+      <c r="WH52" s="15"/>
+      <c r="WI52" s="15"/>
+      <c r="WJ52" s="15"/>
+      <c r="WK52" s="15"/>
+      <c r="WL52" s="15"/>
+      <c r="WM52" s="15"/>
+      <c r="WN52" s="15"/>
+      <c r="WO52" s="15"/>
+      <c r="WP52" s="15"/>
+      <c r="WQ52" s="15"/>
+      <c r="WR52" s="15"/>
+      <c r="WS52" s="15"/>
+      <c r="WT52" s="15"/>
+      <c r="WU52" s="15"/>
+      <c r="WV52" s="15"/>
+      <c r="WW52" s="15"/>
+      <c r="WX52" s="15"/>
+      <c r="WY52" s="15"/>
+      <c r="WZ52" s="15"/>
+      <c r="XA52" s="15"/>
+      <c r="XB52" s="15"/>
+      <c r="XC52" s="15"/>
+      <c r="XD52" s="15"/>
+      <c r="XE52" s="15"/>
+      <c r="XF52" s="15"/>
+      <c r="XG52" s="15"/>
+      <c r="XH52" s="15"/>
+      <c r="XI52" s="15"/>
+      <c r="XJ52" s="15"/>
+      <c r="XK52" s="15"/>
+      <c r="XL52" s="15"/>
+      <c r="XM52" s="15"/>
+      <c r="XN52" s="15"/>
+      <c r="XO52" s="15"/>
+      <c r="XP52" s="15"/>
+      <c r="XQ52" s="15"/>
+      <c r="XR52" s="15"/>
+      <c r="XS52" s="15"/>
+      <c r="XT52" s="15"/>
+      <c r="XU52" s="15"/>
+      <c r="XV52" s="15"/>
+      <c r="XW52" s="15"/>
+      <c r="XX52" s="15"/>
+      <c r="XY52" s="15"/>
+      <c r="XZ52" s="15"/>
+      <c r="YA52" s="15"/>
+      <c r="YB52" s="15"/>
+      <c r="YC52" s="15"/>
+      <c r="YD52" s="15"/>
+      <c r="YE52" s="15"/>
+      <c r="YF52" s="15"/>
+      <c r="YG52" s="15"/>
+      <c r="YH52" s="15"/>
+      <c r="YI52" s="15"/>
+      <c r="YJ52" s="15"/>
+      <c r="YK52" s="15"/>
+      <c r="YL52" s="15"/>
+      <c r="YM52" s="15"/>
+      <c r="YN52" s="15"/>
+      <c r="YO52" s="15"/>
+      <c r="YP52" s="15"/>
+      <c r="YQ52" s="15"/>
+      <c r="YR52" s="15"/>
+      <c r="YS52" s="15"/>
+      <c r="YT52" s="15"/>
+      <c r="YU52" s="15"/>
+      <c r="YV52" s="15"/>
+      <c r="YW52" s="15"/>
+      <c r="YX52" s="15"/>
+      <c r="YY52" s="15"/>
+      <c r="YZ52" s="15"/>
+      <c r="ZA52" s="15"/>
+      <c r="ZB52" s="15"/>
+      <c r="ZC52" s="15"/>
+      <c r="ZD52" s="15"/>
+      <c r="ZE52" s="15"/>
+      <c r="ZF52" s="15"/>
+      <c r="ZG52" s="15"/>
+      <c r="ZH52" s="15"/>
+      <c r="ZI52" s="15"/>
+      <c r="ZJ52" s="15"/>
+      <c r="ZK52" s="15"/>
+      <c r="ZL52" s="15"/>
+      <c r="ZM52" s="15"/>
+      <c r="ZN52" s="15"/>
+      <c r="ZO52" s="15"/>
+      <c r="ZP52" s="15"/>
+      <c r="ZQ52" s="15"/>
+      <c r="ZR52" s="15"/>
+      <c r="ZS52" s="15"/>
+      <c r="ZT52" s="15"/>
+      <c r="ZU52" s="15"/>
+      <c r="ZV52" s="15"/>
+      <c r="ZW52" s="15"/>
+      <c r="ZX52" s="15"/>
+      <c r="ZY52" s="15"/>
+      <c r="ZZ52" s="15"/>
+      <c r="AAA52" s="15"/>
+      <c r="AAB52" s="15"/>
+      <c r="AAC52" s="15"/>
+      <c r="AAD52" s="15"/>
+      <c r="AAE52" s="15"/>
+      <c r="AAF52" s="15"/>
+      <c r="AAG52" s="15"/>
+      <c r="AAH52" s="15"/>
+      <c r="AAI52" s="15"/>
+      <c r="AAJ52" s="15"/>
+      <c r="AAK52" s="15"/>
+      <c r="AAL52" s="15"/>
+      <c r="AAM52" s="15"/>
+      <c r="AAN52" s="15"/>
+      <c r="AAO52" s="15"/>
+      <c r="AAP52" s="15"/>
+      <c r="AAQ52" s="15"/>
+      <c r="AAR52" s="15"/>
+      <c r="AAS52" s="15"/>
+      <c r="AAT52" s="15"/>
+      <c r="AAU52" s="15"/>
+      <c r="AAV52" s="15"/>
+      <c r="AAW52" s="15"/>
+      <c r="AAX52" s="15"/>
+      <c r="AAY52" s="15"/>
+      <c r="AAZ52" s="15"/>
+      <c r="ABA52" s="15"/>
+      <c r="ABB52" s="15"/>
+      <c r="ABC52" s="15"/>
+      <c r="ABD52" s="15"/>
+      <c r="ABE52" s="15"/>
+      <c r="ABF52" s="15"/>
+      <c r="ABG52" s="15"/>
+      <c r="ABH52" s="15"/>
+      <c r="ABI52" s="15"/>
+      <c r="ABJ52" s="15"/>
+      <c r="ABK52" s="15"/>
+      <c r="ABL52" s="15"/>
+      <c r="ABM52" s="15"/>
+      <c r="ABN52" s="15"/>
+      <c r="ABO52" s="15"/>
+      <c r="ABP52" s="15"/>
+      <c r="ABQ52" s="15"/>
+      <c r="ABR52" s="15"/>
+      <c r="ABS52" s="15"/>
+      <c r="ABT52" s="15"/>
+      <c r="ABU52" s="15"/>
+      <c r="ABV52" s="15"/>
+      <c r="ABW52" s="15"/>
+      <c r="ABX52" s="15"/>
+      <c r="ABY52" s="15"/>
+      <c r="ABZ52" s="15"/>
+      <c r="ACA52" s="15"/>
+      <c r="ACB52" s="15"/>
+      <c r="ACC52" s="15"/>
+      <c r="ACD52" s="15"/>
+      <c r="ACE52" s="15"/>
+      <c r="ACF52" s="15"/>
+      <c r="ACG52" s="15"/>
+      <c r="ACH52" s="15"/>
+      <c r="ACI52" s="15"/>
+      <c r="ACJ52" s="15"/>
+      <c r="ACK52" s="15"/>
+      <c r="ACL52" s="15"/>
+      <c r="ACM52" s="15"/>
+      <c r="ACN52" s="15"/>
+      <c r="ACO52" s="15"/>
+      <c r="ACP52" s="15"/>
+      <c r="ACQ52" s="15"/>
+      <c r="ACR52" s="15"/>
+      <c r="ACS52" s="15"/>
+      <c r="ACT52" s="15"/>
+      <c r="ACU52" s="15"/>
+      <c r="ACV52" s="15"/>
+      <c r="ACW52" s="15"/>
+      <c r="ACX52" s="15"/>
+      <c r="ACY52" s="15"/>
+      <c r="ACZ52" s="15"/>
+      <c r="ADA52" s="15"/>
+      <c r="ADB52" s="15"/>
+      <c r="ADC52" s="15"/>
+      <c r="ADD52" s="15"/>
+      <c r="ADE52" s="15"/>
+      <c r="ADF52" s="15"/>
+      <c r="ADG52" s="15"/>
+      <c r="ADH52" s="15"/>
+      <c r="ADI52" s="15"/>
+      <c r="ADJ52" s="15"/>
+      <c r="ADK52" s="15"/>
+      <c r="ADL52" s="15"/>
+      <c r="ADM52" s="15"/>
+      <c r="ADN52" s="15"/>
+      <c r="ADO52" s="15"/>
+      <c r="ADP52" s="15"/>
+      <c r="ADQ52" s="15"/>
+      <c r="ADR52" s="15"/>
+      <c r="ADS52" s="15"/>
+      <c r="ADT52" s="15"/>
+      <c r="ADU52" s="15"/>
+      <c r="ADV52" s="15"/>
+      <c r="ADW52" s="15"/>
+      <c r="ADX52" s="15"/>
+      <c r="ADY52" s="15"/>
+      <c r="ADZ52" s="15"/>
+      <c r="AEA52" s="15"/>
+      <c r="AEB52" s="15"/>
+      <c r="AEC52" s="15"/>
+      <c r="AED52" s="15"/>
+      <c r="AEE52" s="15"/>
+      <c r="AEF52" s="15"/>
+      <c r="AEG52" s="15"/>
+      <c r="AEH52" s="15"/>
+      <c r="AEI52" s="15"/>
+      <c r="AEJ52" s="15"/>
+      <c r="AEK52" s="15"/>
+      <c r="AEL52" s="15"/>
+      <c r="AEM52" s="15"/>
+      <c r="AEN52" s="15"/>
+      <c r="AEO52" s="15"/>
+      <c r="AEP52" s="15"/>
+      <c r="AEQ52" s="15"/>
+      <c r="AER52" s="15"/>
+      <c r="AES52" s="15"/>
+      <c r="AET52" s="15"/>
+      <c r="AEU52" s="15"/>
+      <c r="AEV52" s="15"/>
+      <c r="AEW52" s="15"/>
+      <c r="AEX52" s="15"/>
+      <c r="AEY52" s="15"/>
+      <c r="AEZ52" s="15"/>
+      <c r="AFA52" s="15"/>
+      <c r="AFB52" s="15"/>
+      <c r="AFC52" s="15"/>
+      <c r="AFD52" s="15"/>
+      <c r="AFE52" s="15"/>
+      <c r="AFF52" s="15"/>
+      <c r="AFG52" s="15"/>
+      <c r="AFH52" s="15"/>
+      <c r="AFI52" s="15"/>
+      <c r="AFJ52" s="15"/>
+      <c r="AFK52" s="15"/>
+      <c r="AFL52" s="15"/>
+      <c r="AFM52" s="15"/>
+      <c r="AFN52" s="15"/>
+      <c r="AFO52" s="15"/>
+      <c r="AFP52" s="15"/>
+      <c r="AFQ52" s="15"/>
+      <c r="AFR52" s="15"/>
+      <c r="AFS52" s="15"/>
+      <c r="AFT52" s="15"/>
+      <c r="AFU52" s="15"/>
+      <c r="AFV52" s="15"/>
+      <c r="AFW52" s="15"/>
+      <c r="AFX52" s="15"/>
+      <c r="AFY52" s="15"/>
+      <c r="AFZ52" s="15"/>
+      <c r="AGA52" s="15"/>
+      <c r="AGB52" s="15"/>
+      <c r="AGC52" s="15"/>
+      <c r="AGD52" s="15"/>
+      <c r="AGE52" s="15"/>
+      <c r="AGF52" s="15"/>
+      <c r="AGG52" s="15"/>
+      <c r="AGH52" s="15"/>
+      <c r="AGI52" s="15"/>
+      <c r="AGJ52" s="15"/>
+      <c r="AGK52" s="15"/>
+      <c r="AGL52" s="15"/>
+      <c r="AGM52" s="15"/>
+      <c r="AGN52" s="15"/>
+      <c r="AGO52" s="15"/>
+      <c r="AGP52" s="15"/>
+      <c r="AGQ52" s="15"/>
+      <c r="AGR52" s="15"/>
+      <c r="AGS52" s="15"/>
+      <c r="AGT52" s="15"/>
+      <c r="AGU52" s="15"/>
+      <c r="AGV52" s="15"/>
+      <c r="AGW52" s="15"/>
+      <c r="AGX52" s="15"/>
+      <c r="AGY52" s="15"/>
+      <c r="AGZ52" s="15"/>
+      <c r="AHA52" s="15"/>
+      <c r="AHB52" s="15"/>
+      <c r="AHC52" s="15"/>
+      <c r="AHD52" s="15"/>
+      <c r="AHE52" s="15"/>
+      <c r="AHF52" s="15"/>
+      <c r="AHG52" s="15"/>
+      <c r="AHH52" s="15"/>
+      <c r="AHI52" s="15"/>
+      <c r="AHJ52" s="15"/>
+      <c r="AHK52" s="15"/>
+      <c r="AHL52" s="15"/>
+      <c r="AHM52" s="15"/>
+      <c r="AHN52" s="15"/>
+      <c r="AHO52" s="15"/>
+      <c r="AHP52" s="15"/>
+      <c r="AHQ52" s="15"/>
+      <c r="AHR52" s="15"/>
+      <c r="AHS52" s="15"/>
+      <c r="AHT52" s="15"/>
+      <c r="AHU52" s="15"/>
+      <c r="AHV52" s="15"/>
+      <c r="AHW52" s="15"/>
+      <c r="AHX52" s="15"/>
+      <c r="AHY52" s="15"/>
+      <c r="AHZ52" s="15"/>
+      <c r="AIA52" s="15"/>
+      <c r="AIB52" s="15"/>
+      <c r="AIC52" s="15"/>
+      <c r="AID52" s="15"/>
+      <c r="AIE52" s="15"/>
+      <c r="AIF52" s="15"/>
+      <c r="AIG52" s="15"/>
+      <c r="AIH52" s="15"/>
+      <c r="AII52" s="15"/>
+      <c r="AIJ52" s="15"/>
+      <c r="AIK52" s="15"/>
+      <c r="AIL52" s="15"/>
+      <c r="AIM52" s="15"/>
+      <c r="AIN52" s="15"/>
+      <c r="AIO52" s="15"/>
+      <c r="AIP52" s="15"/>
+      <c r="AIQ52" s="15"/>
+      <c r="AIR52" s="15"/>
+      <c r="AIS52" s="15"/>
+      <c r="AIT52" s="15"/>
+      <c r="AIU52" s="15"/>
+      <c r="AIV52" s="15"/>
+      <c r="AIW52" s="15"/>
+      <c r="AIX52" s="15"/>
+      <c r="AIY52" s="15"/>
+      <c r="AIZ52" s="15"/>
+      <c r="AJA52" s="15"/>
+      <c r="AJB52" s="15"/>
+      <c r="AJC52" s="15"/>
+      <c r="AJD52" s="15"/>
+      <c r="AJE52" s="15"/>
+      <c r="AJF52" s="15"/>
+      <c r="AJG52" s="15"/>
+      <c r="AJH52" s="15"/>
+      <c r="AJI52" s="15"/>
+      <c r="AJJ52" s="15"/>
+      <c r="AJK52" s="15"/>
+      <c r="AJL52" s="15"/>
+      <c r="AJM52" s="15"/>
+      <c r="AJN52" s="15"/>
+      <c r="AJO52" s="15"/>
+      <c r="AJP52" s="15"/>
+      <c r="AJQ52" s="15"/>
+      <c r="AJR52" s="15"/>
+      <c r="AJS52" s="15"/>
+      <c r="AJT52" s="15"/>
+      <c r="AJU52" s="15"/>
+      <c r="AJV52" s="15"/>
+      <c r="AJW52" s="15"/>
+      <c r="AJX52" s="15"/>
+      <c r="AJY52" s="15"/>
+      <c r="AJZ52" s="15"/>
+      <c r="AKA52" s="15"/>
+      <c r="AKB52" s="15"/>
+      <c r="AKC52" s="15"/>
+      <c r="AKD52" s="15"/>
+      <c r="AKE52" s="15"/>
+      <c r="AKF52" s="15"/>
+      <c r="AKG52" s="15"/>
+      <c r="AKH52" s="15"/>
+      <c r="AKI52" s="15"/>
+      <c r="AKJ52" s="15"/>
+      <c r="AKK52" s="15"/>
+      <c r="AKL52" s="15"/>
+      <c r="AKM52" s="15"/>
+      <c r="AKN52" s="15"/>
+      <c r="AKO52" s="15"/>
+      <c r="AKP52" s="15"/>
+      <c r="AKQ52" s="15"/>
+      <c r="AKR52" s="15"/>
+      <c r="AKS52" s="15"/>
+      <c r="AKT52" s="15"/>
+      <c r="AKU52" s="15"/>
+      <c r="AKV52" s="15"/>
+      <c r="AKW52" s="15"/>
+      <c r="AKX52" s="15"/>
+      <c r="AKY52" s="15"/>
+      <c r="AKZ52" s="15"/>
+      <c r="ALA52" s="15"/>
+      <c r="ALB52" s="15"/>
+      <c r="ALC52" s="15"/>
+      <c r="ALD52" s="15"/>
+      <c r="ALE52" s="15"/>
+      <c r="ALF52" s="15"/>
+      <c r="ALG52" s="15"/>
+      <c r="ALH52" s="15"/>
+      <c r="ALI52" s="15"/>
+      <c r="ALJ52" s="15"/>
+      <c r="ALK52" s="15"/>
+      <c r="ALL52" s="15"/>
+      <c r="ALM52" s="15"/>
+      <c r="ALN52" s="15"/>
+      <c r="ALO52" s="15"/>
+      <c r="ALP52" s="15"/>
+      <c r="ALQ52" s="15"/>
+      <c r="ALR52" s="15"/>
+      <c r="ALS52" s="15"/>
+      <c r="ALT52" s="15"/>
+      <c r="ALU52" s="15"/>
+      <c r="ALV52" s="15"/>
+      <c r="ALW52" s="15"/>
+      <c r="ALX52" s="15"/>
+      <c r="ALY52" s="15"/>
+      <c r="ALZ52" s="15"/>
+      <c r="AMA52" s="15"/>
+      <c r="AMB52" s="15"/>
+      <c r="AMC52" s="15"/>
+      <c r="AMD52" s="15"/>
+      <c r="AME52" s="15"/>
+      <c r="AMF52" s="15"/>
+      <c r="AMG52" s="15"/>
+      <c r="AMH52" s="15"/>
+      <c r="AMI52" s="15"/>
+      <c r="AMJ52" s="15"/>
+      <c r="AMK52" s="15"/>
+      <c r="AML52" s="15"/>
+      <c r="AMM52" s="15"/>
+      <c r="AMN52" s="15"/>
+      <c r="AMO52" s="15"/>
+      <c r="AMP52" s="15"/>
+      <c r="AMQ52" s="15"/>
+      <c r="AMR52" s="15"/>
+      <c r="AMS52" s="15"/>
+    </row>
+    <row r="53" s="45" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="11" t="n">
+        <v>1047</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="C53" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="D53" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15" t="n">
+        <v>700</v>
+      </c>
+      <c r="H53" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J53" s="15" t="n">
+        <v>392714</v>
+      </c>
+      <c r="K53" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="L53" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="M52" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="P52" s="1" t="n">
+      <c r="M53" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="N53" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="O53" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="P53" s="15" t="n">
         <v>28</v>
       </c>
-      <c r="Q52" s="1" t="n">
+      <c r="Q53" s="15" t="n">
         <v>29</v>
       </c>
-      <c r="R52" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="S52" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="T52" s="1" t="n">
+      <c r="R53" s="15"/>
+      <c r="S53" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="T53" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="V52" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="W52" s="1" t="n">
-        <v>89088</v>
-      </c>
-      <c r="X52" s="1" t="n">
+      <c r="U53" s="15"/>
+      <c r="V53" s="15"/>
+      <c r="W53" s="17" t="n">
+        <v>13407</v>
+      </c>
+      <c r="X53" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y53" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="Z53" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA53" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB53" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC53" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="AD53" s="15" t="n">
+        <v>281795</v>
+      </c>
+      <c r="AE53" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF53" s="15" t="n">
+        <v>81687</v>
+      </c>
+      <c r="AG53" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="Y52" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="Z52" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AA52" s="1" t="s">
+      <c r="AH53" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI53" s="17"/>
+      <c r="AJ53" s="15"/>
+      <c r="AK53" s="15"/>
+      <c r="AL53" s="15"/>
+      <c r="AM53" s="15"/>
+      <c r="AN53" s="15"/>
+      <c r="AO53" s="15"/>
+      <c r="AP53" s="15"/>
+      <c r="AQ53" s="15"/>
+      <c r="AR53" s="15"/>
+      <c r="AS53" s="15"/>
+      <c r="AT53" s="11"/>
+      <c r="AU53" s="15"/>
+      <c r="AV53" s="11"/>
+      <c r="AW53" s="15"/>
+      <c r="AX53" s="15"/>
+      <c r="AY53" s="15"/>
+      <c r="AZ53" s="15"/>
+      <c r="BA53" s="15"/>
+      <c r="BB53" s="15"/>
+      <c r="BC53" s="15"/>
+      <c r="BD53" s="15"/>
+      <c r="BE53" s="15"/>
+      <c r="BF53" s="15"/>
+      <c r="BG53" s="15"/>
+      <c r="BH53" s="15"/>
+      <c r="BI53" s="15"/>
+      <c r="BJ53" s="15"/>
+      <c r="BK53" s="15"/>
+      <c r="BL53" s="15"/>
+      <c r="BM53" s="15"/>
+      <c r="BN53" s="15"/>
+      <c r="BO53" s="15"/>
+      <c r="BP53" s="15"/>
+      <c r="BQ53" s="15"/>
+      <c r="BR53" s="15"/>
+      <c r="BS53" s="15"/>
+      <c r="BT53" s="15"/>
+      <c r="BU53" s="15"/>
+      <c r="BV53" s="15"/>
+      <c r="BW53" s="15"/>
+      <c r="BX53" s="15"/>
+      <c r="BY53" s="15"/>
+      <c r="BZ53" s="15"/>
+      <c r="CA53" s="15"/>
+      <c r="CB53" s="15"/>
+      <c r="CC53" s="15"/>
+      <c r="CD53" s="15"/>
+      <c r="CE53" s="15"/>
+      <c r="CF53" s="15"/>
+      <c r="CG53" s="15"/>
+      <c r="CH53" s="15"/>
+      <c r="CI53" s="15"/>
+      <c r="CJ53" s="15"/>
+      <c r="CK53" s="15"/>
+      <c r="CL53" s="15"/>
+      <c r="CM53" s="15"/>
+      <c r="CN53" s="15"/>
+      <c r="CO53" s="15"/>
+      <c r="CP53" s="15"/>
+      <c r="CQ53" s="15"/>
+      <c r="CR53" s="15"/>
+      <c r="CS53" s="15"/>
+      <c r="CT53" s="15"/>
+      <c r="CU53" s="15"/>
+      <c r="CV53" s="15"/>
+      <c r="CW53" s="15"/>
+      <c r="CX53" s="15"/>
+      <c r="CY53" s="15"/>
+      <c r="CZ53" s="15"/>
+      <c r="DA53" s="15"/>
+      <c r="DB53" s="15"/>
+      <c r="DC53" s="15"/>
+      <c r="DD53" s="15"/>
+      <c r="DE53" s="15"/>
+      <c r="DF53" s="15"/>
+      <c r="DG53" s="15"/>
+      <c r="DH53" s="15"/>
+      <c r="DI53" s="15"/>
+      <c r="DJ53" s="15"/>
+      <c r="DK53" s="15"/>
+      <c r="DL53" s="15"/>
+      <c r="DM53" s="15"/>
+      <c r="DN53" s="15"/>
+      <c r="DO53" s="15"/>
+      <c r="DP53" s="15"/>
+      <c r="DQ53" s="15"/>
+      <c r="DR53" s="15"/>
+      <c r="DS53" s="15"/>
+      <c r="DT53" s="15"/>
+      <c r="DU53" s="15"/>
+      <c r="DV53" s="15"/>
+      <c r="DW53" s="15"/>
+      <c r="DX53" s="15"/>
+      <c r="DY53" s="15"/>
+      <c r="DZ53" s="15"/>
+      <c r="EA53" s="15"/>
+      <c r="EB53" s="15"/>
+      <c r="EC53" s="15"/>
+      <c r="ED53" s="15"/>
+      <c r="EE53" s="15"/>
+      <c r="EF53" s="15"/>
+      <c r="EG53" s="15"/>
+      <c r="EH53" s="15"/>
+      <c r="EI53" s="15"/>
+      <c r="EJ53" s="15"/>
+      <c r="EK53" s="15"/>
+      <c r="EL53" s="15"/>
+      <c r="EM53" s="15"/>
+      <c r="EN53" s="15"/>
+      <c r="EO53" s="15"/>
+      <c r="EP53" s="15"/>
+      <c r="EQ53" s="15"/>
+      <c r="ER53" s="15"/>
+      <c r="ES53" s="15"/>
+      <c r="ET53" s="15"/>
+      <c r="EU53" s="15"/>
+      <c r="EV53" s="15"/>
+      <c r="EW53" s="15"/>
+      <c r="EX53" s="15"/>
+      <c r="EY53" s="15"/>
+      <c r="EZ53" s="15"/>
+      <c r="FA53" s="15"/>
+      <c r="FB53" s="15"/>
+      <c r="FC53" s="15"/>
+      <c r="FD53" s="15"/>
+      <c r="FE53" s="15"/>
+      <c r="FF53" s="15"/>
+      <c r="FG53" s="15"/>
+      <c r="FH53" s="15"/>
+      <c r="FI53" s="15"/>
+      <c r="FJ53" s="15"/>
+      <c r="FK53" s="15"/>
+      <c r="FL53" s="15"/>
+      <c r="FM53" s="15"/>
+      <c r="FN53" s="15"/>
+      <c r="FO53" s="15"/>
+      <c r="FP53" s="15"/>
+      <c r="FQ53" s="15"/>
+      <c r="FR53" s="15"/>
+      <c r="FS53" s="15"/>
+      <c r="FT53" s="15"/>
+      <c r="FU53" s="15"/>
+      <c r="FV53" s="15"/>
+      <c r="FW53" s="15"/>
+      <c r="FX53" s="15"/>
+      <c r="FY53" s="15"/>
+      <c r="FZ53" s="15"/>
+      <c r="GA53" s="15"/>
+      <c r="GB53" s="15"/>
+      <c r="GC53" s="15"/>
+      <c r="GD53" s="15"/>
+      <c r="GE53" s="15"/>
+      <c r="GF53" s="15"/>
+      <c r="GG53" s="15"/>
+      <c r="GH53" s="15"/>
+      <c r="GI53" s="15"/>
+      <c r="GJ53" s="15"/>
+      <c r="GK53" s="15"/>
+      <c r="GL53" s="15"/>
+      <c r="GM53" s="15"/>
+      <c r="GN53" s="15"/>
+      <c r="GO53" s="15"/>
+      <c r="GP53" s="15"/>
+      <c r="GQ53" s="15"/>
+      <c r="GR53" s="15"/>
+      <c r="GS53" s="15"/>
+      <c r="GT53" s="15"/>
+      <c r="GU53" s="15"/>
+      <c r="GV53" s="15"/>
+      <c r="GW53" s="15"/>
+      <c r="GX53" s="15"/>
+      <c r="GY53" s="15"/>
+      <c r="GZ53" s="15"/>
+      <c r="HA53" s="15"/>
+      <c r="HB53" s="15"/>
+      <c r="HC53" s="15"/>
+      <c r="HD53" s="15"/>
+      <c r="HE53" s="15"/>
+      <c r="HF53" s="15"/>
+      <c r="HG53" s="15"/>
+      <c r="HH53" s="15"/>
+      <c r="HI53" s="15"/>
+      <c r="HJ53" s="15"/>
+      <c r="HK53" s="15"/>
+      <c r="HL53" s="15"/>
+      <c r="HM53" s="15"/>
+      <c r="HN53" s="15"/>
+      <c r="HO53" s="15"/>
+      <c r="HP53" s="15"/>
+      <c r="HQ53" s="15"/>
+      <c r="HR53" s="15"/>
+      <c r="HS53" s="15"/>
+      <c r="HT53" s="15"/>
+      <c r="HU53" s="15"/>
+      <c r="HV53" s="15"/>
+      <c r="HW53" s="15"/>
+      <c r="HX53" s="15"/>
+      <c r="HY53" s="15"/>
+      <c r="HZ53" s="15"/>
+      <c r="IA53" s="15"/>
+      <c r="IB53" s="15"/>
+      <c r="IC53" s="15"/>
+      <c r="ID53" s="15"/>
+      <c r="IE53" s="15"/>
+      <c r="IF53" s="15"/>
+      <c r="IG53" s="15"/>
+      <c r="IH53" s="15"/>
+      <c r="II53" s="15"/>
+      <c r="IJ53" s="15"/>
+      <c r="IK53" s="15"/>
+      <c r="IL53" s="15"/>
+      <c r="IM53" s="15"/>
+      <c r="IN53" s="15"/>
+      <c r="IO53" s="15"/>
+      <c r="IP53" s="15"/>
+      <c r="IQ53" s="15"/>
+      <c r="IR53" s="15"/>
+      <c r="IS53" s="15"/>
+      <c r="IT53" s="15"/>
+      <c r="IU53" s="15"/>
+      <c r="IV53" s="15"/>
+      <c r="IW53" s="15"/>
+      <c r="IX53" s="15"/>
+      <c r="IY53" s="15"/>
+      <c r="IZ53" s="15"/>
+      <c r="JA53" s="15"/>
+      <c r="JB53" s="15"/>
+      <c r="JC53" s="15"/>
+      <c r="JD53" s="15"/>
+      <c r="JE53" s="15"/>
+      <c r="JF53" s="15"/>
+      <c r="JG53" s="15"/>
+      <c r="JH53" s="15"/>
+      <c r="JI53" s="15"/>
+      <c r="JJ53" s="15"/>
+      <c r="JK53" s="15"/>
+      <c r="JL53" s="15"/>
+      <c r="JM53" s="15"/>
+      <c r="JN53" s="15"/>
+      <c r="JO53" s="15"/>
+      <c r="JP53" s="15"/>
+      <c r="JQ53" s="15"/>
+      <c r="JR53" s="15"/>
+      <c r="JS53" s="15"/>
+      <c r="JT53" s="15"/>
+      <c r="JU53" s="15"/>
+      <c r="JV53" s="15"/>
+      <c r="JW53" s="15"/>
+      <c r="JX53" s="15"/>
+      <c r="JY53" s="15"/>
+      <c r="JZ53" s="15"/>
+      <c r="KA53" s="15"/>
+      <c r="KB53" s="15"/>
+      <c r="KC53" s="15"/>
+      <c r="KD53" s="15"/>
+      <c r="KE53" s="15"/>
+      <c r="KF53" s="15"/>
+      <c r="KG53" s="15"/>
+      <c r="KH53" s="15"/>
+      <c r="KI53" s="15"/>
+      <c r="KJ53" s="15"/>
+      <c r="KK53" s="15"/>
+      <c r="KL53" s="15"/>
+      <c r="KM53" s="15"/>
+      <c r="KN53" s="15"/>
+      <c r="KO53" s="15"/>
+      <c r="KP53" s="15"/>
+      <c r="KQ53" s="15"/>
+      <c r="KR53" s="15"/>
+      <c r="KS53" s="15"/>
+      <c r="KT53" s="15"/>
+      <c r="KU53" s="15"/>
+      <c r="KV53" s="15"/>
+      <c r="KW53" s="15"/>
+      <c r="KX53" s="15"/>
+      <c r="KY53" s="15"/>
+      <c r="KZ53" s="15"/>
+      <c r="LA53" s="15"/>
+      <c r="LB53" s="15"/>
+      <c r="LC53" s="15"/>
+      <c r="LD53" s="15"/>
+      <c r="LE53" s="15"/>
+      <c r="LF53" s="15"/>
+      <c r="LG53" s="15"/>
+      <c r="LH53" s="15"/>
+      <c r="LI53" s="15"/>
+      <c r="LJ53" s="15"/>
+      <c r="LK53" s="15"/>
+      <c r="LL53" s="15"/>
+      <c r="LM53" s="15"/>
+      <c r="LN53" s="15"/>
+      <c r="LO53" s="15"/>
+      <c r="LP53" s="15"/>
+      <c r="LQ53" s="15"/>
+      <c r="LR53" s="15"/>
+      <c r="LS53" s="15"/>
+      <c r="LT53" s="15"/>
+      <c r="LU53" s="15"/>
+      <c r="LV53" s="15"/>
+      <c r="LW53" s="15"/>
+      <c r="LX53" s="15"/>
+      <c r="LY53" s="15"/>
+      <c r="LZ53" s="15"/>
+      <c r="MA53" s="15"/>
+      <c r="MB53" s="15"/>
+      <c r="MC53" s="15"/>
+      <c r="MD53" s="15"/>
+      <c r="ME53" s="15"/>
+      <c r="MF53" s="15"/>
+      <c r="MG53" s="15"/>
+      <c r="MH53" s="15"/>
+      <c r="MI53" s="15"/>
+      <c r="MJ53" s="15"/>
+      <c r="MK53" s="15"/>
+      <c r="ML53" s="15"/>
+      <c r="MM53" s="15"/>
+      <c r="MN53" s="15"/>
+      <c r="MO53" s="15"/>
+      <c r="MP53" s="15"/>
+      <c r="MQ53" s="15"/>
+      <c r="MR53" s="15"/>
+      <c r="MS53" s="15"/>
+      <c r="MT53" s="15"/>
+      <c r="MU53" s="15"/>
+      <c r="MV53" s="15"/>
+      <c r="MW53" s="15"/>
+      <c r="MX53" s="15"/>
+      <c r="MY53" s="15"/>
+      <c r="MZ53" s="15"/>
+      <c r="NA53" s="15"/>
+      <c r="NB53" s="15"/>
+      <c r="NC53" s="15"/>
+      <c r="ND53" s="15"/>
+      <c r="NE53" s="15"/>
+      <c r="NF53" s="15"/>
+      <c r="NG53" s="15"/>
+      <c r="NH53" s="15"/>
+      <c r="NI53" s="15"/>
+      <c r="NJ53" s="15"/>
+      <c r="NK53" s="15"/>
+      <c r="NL53" s="15"/>
+      <c r="NM53" s="15"/>
+      <c r="NN53" s="15"/>
+      <c r="NO53" s="15"/>
+      <c r="NP53" s="15"/>
+      <c r="NQ53" s="15"/>
+      <c r="NR53" s="15"/>
+      <c r="NS53" s="15"/>
+      <c r="NT53" s="15"/>
+      <c r="NU53" s="15"/>
+      <c r="NV53" s="15"/>
+      <c r="NW53" s="15"/>
+      <c r="NX53" s="15"/>
+      <c r="NY53" s="15"/>
+      <c r="NZ53" s="15"/>
+      <c r="OA53" s="15"/>
+      <c r="OB53" s="15"/>
+      <c r="OC53" s="15"/>
+      <c r="OD53" s="15"/>
+      <c r="OE53" s="15"/>
+      <c r="OF53" s="15"/>
+      <c r="OG53" s="15"/>
+      <c r="OH53" s="15"/>
+      <c r="OI53" s="15"/>
+      <c r="OJ53" s="15"/>
+      <c r="OK53" s="15"/>
+      <c r="OL53" s="15"/>
+      <c r="OM53" s="15"/>
+      <c r="ON53" s="15"/>
+      <c r="OO53" s="15"/>
+      <c r="OP53" s="15"/>
+      <c r="OQ53" s="15"/>
+      <c r="OR53" s="15"/>
+      <c r="OS53" s="15"/>
+      <c r="OT53" s="15"/>
+      <c r="OU53" s="15"/>
+      <c r="OV53" s="15"/>
+      <c r="OW53" s="15"/>
+      <c r="OX53" s="15"/>
+      <c r="OY53" s="15"/>
+      <c r="OZ53" s="15"/>
+      <c r="PA53" s="15"/>
+      <c r="PB53" s="15"/>
+      <c r="PC53" s="15"/>
+      <c r="PD53" s="15"/>
+      <c r="PE53" s="15"/>
+      <c r="PF53" s="15"/>
+      <c r="PG53" s="15"/>
+      <c r="PH53" s="15"/>
+      <c r="PI53" s="15"/>
+      <c r="PJ53" s="15"/>
+      <c r="PK53" s="15"/>
+      <c r="PL53" s="15"/>
+      <c r="PM53" s="15"/>
+      <c r="PN53" s="15"/>
+      <c r="PO53" s="15"/>
+      <c r="PP53" s="15"/>
+      <c r="PQ53" s="15"/>
+      <c r="PR53" s="15"/>
+      <c r="PS53" s="15"/>
+      <c r="PT53" s="15"/>
+      <c r="PU53" s="15"/>
+      <c r="PV53" s="15"/>
+      <c r="PW53" s="15"/>
+      <c r="PX53" s="15"/>
+      <c r="PY53" s="15"/>
+      <c r="PZ53" s="15"/>
+      <c r="QA53" s="15"/>
+      <c r="QB53" s="15"/>
+      <c r="QC53" s="15"/>
+      <c r="QD53" s="15"/>
+      <c r="QE53" s="15"/>
+      <c r="QF53" s="15"/>
+      <c r="QG53" s="15"/>
+      <c r="QH53" s="15"/>
+      <c r="QI53" s="15"/>
+      <c r="QJ53" s="15"/>
+      <c r="QK53" s="15"/>
+      <c r="QL53" s="15"/>
+      <c r="QM53" s="15"/>
+      <c r="QN53" s="15"/>
+      <c r="QO53" s="15"/>
+      <c r="QP53" s="15"/>
+      <c r="QQ53" s="15"/>
+      <c r="QR53" s="15"/>
+      <c r="QS53" s="15"/>
+      <c r="QT53" s="15"/>
+      <c r="QU53" s="15"/>
+      <c r="QV53" s="15"/>
+      <c r="QW53" s="15"/>
+      <c r="QX53" s="15"/>
+      <c r="QY53" s="15"/>
+      <c r="QZ53" s="15"/>
+      <c r="RA53" s="15"/>
+      <c r="RB53" s="15"/>
+      <c r="RC53" s="15"/>
+      <c r="RD53" s="15"/>
+      <c r="RE53" s="15"/>
+      <c r="RF53" s="15"/>
+      <c r="RG53" s="15"/>
+      <c r="RH53" s="15"/>
+      <c r="RI53" s="15"/>
+      <c r="RJ53" s="15"/>
+      <c r="RK53" s="15"/>
+      <c r="RL53" s="15"/>
+      <c r="RM53" s="15"/>
+      <c r="RN53" s="15"/>
+      <c r="RO53" s="15"/>
+      <c r="RP53" s="15"/>
+      <c r="RQ53" s="15"/>
+      <c r="RR53" s="15"/>
+      <c r="RS53" s="15"/>
+      <c r="RT53" s="15"/>
+      <c r="RU53" s="15"/>
+      <c r="RV53" s="15"/>
+      <c r="RW53" s="15"/>
+      <c r="RX53" s="15"/>
+      <c r="RY53" s="15"/>
+      <c r="RZ53" s="15"/>
+      <c r="SA53" s="15"/>
+      <c r="SB53" s="15"/>
+      <c r="SC53" s="15"/>
+      <c r="SD53" s="15"/>
+      <c r="SE53" s="15"/>
+      <c r="SF53" s="15"/>
+      <c r="SG53" s="15"/>
+      <c r="SH53" s="15"/>
+      <c r="SI53" s="15"/>
+      <c r="SJ53" s="15"/>
+      <c r="SK53" s="15"/>
+      <c r="SL53" s="15"/>
+      <c r="SM53" s="15"/>
+      <c r="SN53" s="15"/>
+      <c r="SO53" s="15"/>
+      <c r="SP53" s="15"/>
+      <c r="SQ53" s="15"/>
+      <c r="SR53" s="15"/>
+      <c r="SS53" s="15"/>
+      <c r="ST53" s="15"/>
+      <c r="SU53" s="15"/>
+      <c r="SV53" s="15"/>
+      <c r="SW53" s="15"/>
+      <c r="SX53" s="15"/>
+      <c r="SY53" s="15"/>
+      <c r="SZ53" s="15"/>
+      <c r="TA53" s="15"/>
+      <c r="TB53" s="15"/>
+      <c r="TC53" s="15"/>
+      <c r="TD53" s="15"/>
+      <c r="TE53" s="15"/>
+      <c r="TF53" s="15"/>
+      <c r="TG53" s="15"/>
+      <c r="TH53" s="15"/>
+      <c r="TI53" s="15"/>
+      <c r="TJ53" s="15"/>
+      <c r="TK53" s="15"/>
+      <c r="TL53" s="15"/>
+      <c r="TM53" s="15"/>
+      <c r="TN53" s="15"/>
+      <c r="TO53" s="15"/>
+      <c r="TP53" s="15"/>
+      <c r="TQ53" s="15"/>
+      <c r="TR53" s="15"/>
+      <c r="TS53" s="15"/>
+      <c r="TT53" s="15"/>
+      <c r="TU53" s="15"/>
+      <c r="TV53" s="15"/>
+      <c r="TW53" s="15"/>
+      <c r="TX53" s="15"/>
+      <c r="TY53" s="15"/>
+      <c r="TZ53" s="15"/>
+      <c r="UA53" s="15"/>
+      <c r="UB53" s="15"/>
+      <c r="UC53" s="15"/>
+      <c r="UD53" s="15"/>
+      <c r="UE53" s="15"/>
+      <c r="UF53" s="15"/>
+      <c r="UG53" s="15"/>
+      <c r="UH53" s="15"/>
+      <c r="UI53" s="15"/>
+      <c r="UJ53" s="15"/>
+      <c r="UK53" s="15"/>
+      <c r="UL53" s="15"/>
+      <c r="UM53" s="15"/>
+      <c r="UN53" s="15"/>
+      <c r="UO53" s="15"/>
+      <c r="UP53" s="15"/>
+      <c r="UQ53" s="15"/>
+      <c r="UR53" s="15"/>
+      <c r="US53" s="15"/>
+      <c r="UT53" s="15"/>
+      <c r="UU53" s="15"/>
+      <c r="UV53" s="15"/>
+      <c r="UW53" s="15"/>
+      <c r="UX53" s="15"/>
+      <c r="UY53" s="15"/>
+      <c r="UZ53" s="15"/>
+      <c r="VA53" s="15"/>
+      <c r="VB53" s="15"/>
+      <c r="VC53" s="15"/>
+      <c r="VD53" s="15"/>
+      <c r="VE53" s="15"/>
+      <c r="VF53" s="15"/>
+      <c r="VG53" s="15"/>
+      <c r="VH53" s="15"/>
+      <c r="VI53" s="15"/>
+      <c r="VJ53" s="15"/>
+      <c r="VK53" s="15"/>
+      <c r="VL53" s="15"/>
+      <c r="VM53" s="15"/>
+      <c r="VN53" s="15"/>
+      <c r="VO53" s="15"/>
+      <c r="VP53" s="15"/>
+      <c r="VQ53" s="15"/>
+      <c r="VR53" s="15"/>
+      <c r="VS53" s="15"/>
+      <c r="VT53" s="15"/>
+      <c r="VU53" s="15"/>
+      <c r="VV53" s="15"/>
+      <c r="VW53" s="15"/>
+      <c r="VX53" s="15"/>
+      <c r="VY53" s="15"/>
+      <c r="VZ53" s="15"/>
+      <c r="WA53" s="15"/>
+      <c r="WB53" s="15"/>
+      <c r="WC53" s="15"/>
+      <c r="WD53" s="15"/>
+      <c r="WE53" s="15"/>
+      <c r="WF53" s="15"/>
+      <c r="WG53" s="15"/>
+      <c r="WH53" s="15"/>
+      <c r="WI53" s="15"/>
+      <c r="WJ53" s="15"/>
+      <c r="WK53" s="15"/>
+      <c r="WL53" s="15"/>
+      <c r="WM53" s="15"/>
+      <c r="WN53" s="15"/>
+      <c r="WO53" s="15"/>
+      <c r="WP53" s="15"/>
+      <c r="WQ53" s="15"/>
+      <c r="WR53" s="15"/>
+      <c r="WS53" s="15"/>
+      <c r="WT53" s="15"/>
+      <c r="WU53" s="15"/>
+      <c r="WV53" s="15"/>
+      <c r="WW53" s="15"/>
+      <c r="WX53" s="15"/>
+      <c r="WY53" s="15"/>
+      <c r="WZ53" s="15"/>
+      <c r="XA53" s="15"/>
+      <c r="XB53" s="15"/>
+      <c r="XC53" s="15"/>
+      <c r="XD53" s="15"/>
+      <c r="XE53" s="15"/>
+      <c r="XF53" s="15"/>
+      <c r="XG53" s="15"/>
+      <c r="XH53" s="15"/>
+      <c r="XI53" s="15"/>
+      <c r="XJ53" s="15"/>
+      <c r="XK53" s="15"/>
+      <c r="XL53" s="15"/>
+      <c r="XM53" s="15"/>
+      <c r="XN53" s="15"/>
+      <c r="XO53" s="15"/>
+      <c r="XP53" s="15"/>
+      <c r="XQ53" s="15"/>
+      <c r="XR53" s="15"/>
+      <c r="XS53" s="15"/>
+      <c r="XT53" s="15"/>
+      <c r="XU53" s="15"/>
+      <c r="XV53" s="15"/>
+      <c r="XW53" s="15"/>
+      <c r="XX53" s="15"/>
+      <c r="XY53" s="15"/>
+      <c r="XZ53" s="15"/>
+      <c r="YA53" s="15"/>
+      <c r="YB53" s="15"/>
+      <c r="YC53" s="15"/>
+      <c r="YD53" s="15"/>
+      <c r="YE53" s="15"/>
+      <c r="YF53" s="15"/>
+      <c r="YG53" s="15"/>
+      <c r="YH53" s="15"/>
+      <c r="YI53" s="15"/>
+      <c r="YJ53" s="15"/>
+      <c r="YK53" s="15"/>
+      <c r="YL53" s="15"/>
+      <c r="YM53" s="15"/>
+      <c r="YN53" s="15"/>
+      <c r="YO53" s="15"/>
+      <c r="YP53" s="15"/>
+      <c r="YQ53" s="15"/>
+      <c r="YR53" s="15"/>
+      <c r="YS53" s="15"/>
+      <c r="YT53" s="15"/>
+      <c r="YU53" s="15"/>
+      <c r="YV53" s="15"/>
+      <c r="YW53" s="15"/>
+      <c r="YX53" s="15"/>
+      <c r="YY53" s="15"/>
+      <c r="YZ53" s="15"/>
+      <c r="ZA53" s="15"/>
+      <c r="ZB53" s="15"/>
+      <c r="ZC53" s="15"/>
+      <c r="ZD53" s="15"/>
+      <c r="ZE53" s="15"/>
+      <c r="ZF53" s="15"/>
+      <c r="ZG53" s="15"/>
+      <c r="ZH53" s="15"/>
+      <c r="ZI53" s="15"/>
+      <c r="ZJ53" s="15"/>
+      <c r="ZK53" s="15"/>
+      <c r="ZL53" s="15"/>
+      <c r="ZM53" s="15"/>
+      <c r="ZN53" s="15"/>
+      <c r="ZO53" s="15"/>
+      <c r="ZP53" s="15"/>
+      <c r="ZQ53" s="15"/>
+      <c r="ZR53" s="15"/>
+      <c r="ZS53" s="15"/>
+      <c r="ZT53" s="15"/>
+      <c r="ZU53" s="15"/>
+      <c r="ZV53" s="15"/>
+      <c r="ZW53" s="15"/>
+      <c r="ZX53" s="15"/>
+      <c r="ZY53" s="15"/>
+      <c r="ZZ53" s="15"/>
+      <c r="AAA53" s="15"/>
+      <c r="AAB53" s="15"/>
+      <c r="AAC53" s="15"/>
+      <c r="AAD53" s="15"/>
+      <c r="AAE53" s="15"/>
+      <c r="AAF53" s="15"/>
+      <c r="AAG53" s="15"/>
+      <c r="AAH53" s="15"/>
+      <c r="AAI53" s="15"/>
+      <c r="AAJ53" s="15"/>
+      <c r="AAK53" s="15"/>
+      <c r="AAL53" s="15"/>
+      <c r="AAM53" s="15"/>
+      <c r="AAN53" s="15"/>
+      <c r="AAO53" s="15"/>
+      <c r="AAP53" s="15"/>
+      <c r="AAQ53" s="15"/>
+      <c r="AAR53" s="15"/>
+      <c r="AAS53" s="15"/>
+      <c r="AAT53" s="15"/>
+      <c r="AAU53" s="15"/>
+      <c r="AAV53" s="15"/>
+      <c r="AAW53" s="15"/>
+      <c r="AAX53" s="15"/>
+      <c r="AAY53" s="15"/>
+      <c r="AAZ53" s="15"/>
+      <c r="ABA53" s="15"/>
+      <c r="ABB53" s="15"/>
+      <c r="ABC53" s="15"/>
+      <c r="ABD53" s="15"/>
+      <c r="ABE53" s="15"/>
+      <c r="ABF53" s="15"/>
+      <c r="ABG53" s="15"/>
+      <c r="ABH53" s="15"/>
+      <c r="ABI53" s="15"/>
+      <c r="ABJ53" s="15"/>
+      <c r="ABK53" s="15"/>
+      <c r="ABL53" s="15"/>
+      <c r="ABM53" s="15"/>
+      <c r="ABN53" s="15"/>
+      <c r="ABO53" s="15"/>
+      <c r="ABP53" s="15"/>
+      <c r="ABQ53" s="15"/>
+      <c r="ABR53" s="15"/>
+      <c r="ABS53" s="15"/>
+      <c r="ABT53" s="15"/>
+      <c r="ABU53" s="15"/>
+      <c r="ABV53" s="15"/>
+      <c r="ABW53" s="15"/>
+      <c r="ABX53" s="15"/>
+      <c r="ABY53" s="15"/>
+      <c r="ABZ53" s="15"/>
+      <c r="ACA53" s="15"/>
+      <c r="ACB53" s="15"/>
+      <c r="ACC53" s="15"/>
+      <c r="ACD53" s="15"/>
+      <c r="ACE53" s="15"/>
+      <c r="ACF53" s="15"/>
+      <c r="ACG53" s="15"/>
+      <c r="ACH53" s="15"/>
+      <c r="ACI53" s="15"/>
+      <c r="ACJ53" s="15"/>
+      <c r="ACK53" s="15"/>
+      <c r="ACL53" s="15"/>
+      <c r="ACM53" s="15"/>
+      <c r="ACN53" s="15"/>
+      <c r="ACO53" s="15"/>
+      <c r="ACP53" s="15"/>
+      <c r="ACQ53" s="15"/>
+      <c r="ACR53" s="15"/>
+      <c r="ACS53" s="15"/>
+      <c r="ACT53" s="15"/>
+      <c r="ACU53" s="15"/>
+      <c r="ACV53" s="15"/>
+      <c r="ACW53" s="15"/>
+      <c r="ACX53" s="15"/>
+      <c r="ACY53" s="15"/>
+      <c r="ACZ53" s="15"/>
+      <c r="ADA53" s="15"/>
+      <c r="ADB53" s="15"/>
+      <c r="ADC53" s="15"/>
+      <c r="ADD53" s="15"/>
+      <c r="ADE53" s="15"/>
+      <c r="ADF53" s="15"/>
+      <c r="ADG53" s="15"/>
+      <c r="ADH53" s="15"/>
+      <c r="ADI53" s="15"/>
+      <c r="ADJ53" s="15"/>
+      <c r="ADK53" s="15"/>
+      <c r="ADL53" s="15"/>
+      <c r="ADM53" s="15"/>
+      <c r="ADN53" s="15"/>
+      <c r="ADO53" s="15"/>
+      <c r="ADP53" s="15"/>
+      <c r="ADQ53" s="15"/>
+      <c r="ADR53" s="15"/>
+      <c r="ADS53" s="15"/>
+      <c r="ADT53" s="15"/>
+      <c r="ADU53" s="15"/>
+      <c r="ADV53" s="15"/>
+      <c r="ADW53" s="15"/>
+      <c r="ADX53" s="15"/>
+      <c r="ADY53" s="15"/>
+      <c r="ADZ53" s="15"/>
+      <c r="AEA53" s="15"/>
+      <c r="AEB53" s="15"/>
+      <c r="AEC53" s="15"/>
+      <c r="AED53" s="15"/>
+      <c r="AEE53" s="15"/>
+      <c r="AEF53" s="15"/>
+      <c r="AEG53" s="15"/>
+      <c r="AEH53" s="15"/>
+      <c r="AEI53" s="15"/>
+      <c r="AEJ53" s="15"/>
+      <c r="AEK53" s="15"/>
+      <c r="AEL53" s="15"/>
+      <c r="AEM53" s="15"/>
+      <c r="AEN53" s="15"/>
+      <c r="AEO53" s="15"/>
+      <c r="AEP53" s="15"/>
+      <c r="AEQ53" s="15"/>
+      <c r="AER53" s="15"/>
+      <c r="AES53" s="15"/>
+      <c r="AET53" s="15"/>
+      <c r="AEU53" s="15"/>
+      <c r="AEV53" s="15"/>
+      <c r="AEW53" s="15"/>
+      <c r="AEX53" s="15"/>
+      <c r="AEY53" s="15"/>
+      <c r="AEZ53" s="15"/>
+      <c r="AFA53" s="15"/>
+      <c r="AFB53" s="15"/>
+      <c r="AFC53" s="15"/>
+      <c r="AFD53" s="15"/>
+      <c r="AFE53" s="15"/>
+      <c r="AFF53" s="15"/>
+      <c r="AFG53" s="15"/>
+      <c r="AFH53" s="15"/>
+      <c r="AFI53" s="15"/>
+      <c r="AFJ53" s="15"/>
+      <c r="AFK53" s="15"/>
+      <c r="AFL53" s="15"/>
+      <c r="AFM53" s="15"/>
+      <c r="AFN53" s="15"/>
+      <c r="AFO53" s="15"/>
+      <c r="AFP53" s="15"/>
+      <c r="AFQ53" s="15"/>
+      <c r="AFR53" s="15"/>
+      <c r="AFS53" s="15"/>
+      <c r="AFT53" s="15"/>
+      <c r="AFU53" s="15"/>
+      <c r="AFV53" s="15"/>
+      <c r="AFW53" s="15"/>
+      <c r="AFX53" s="15"/>
+      <c r="AFY53" s="15"/>
+      <c r="AFZ53" s="15"/>
+      <c r="AGA53" s="15"/>
+      <c r="AGB53" s="15"/>
+      <c r="AGC53" s="15"/>
+      <c r="AGD53" s="15"/>
+      <c r="AGE53" s="15"/>
+      <c r="AGF53" s="15"/>
+      <c r="AGG53" s="15"/>
+      <c r="AGH53" s="15"/>
+      <c r="AGI53" s="15"/>
+      <c r="AGJ53" s="15"/>
+      <c r="AGK53" s="15"/>
+      <c r="AGL53" s="15"/>
+      <c r="AGM53" s="15"/>
+      <c r="AGN53" s="15"/>
+      <c r="AGO53" s="15"/>
+      <c r="AGP53" s="15"/>
+      <c r="AGQ53" s="15"/>
+      <c r="AGR53" s="15"/>
+      <c r="AGS53" s="15"/>
+      <c r="AGT53" s="15"/>
+      <c r="AGU53" s="15"/>
+      <c r="AGV53" s="15"/>
+      <c r="AGW53" s="15"/>
+      <c r="AGX53" s="15"/>
+      <c r="AGY53" s="15"/>
+      <c r="AGZ53" s="15"/>
+      <c r="AHA53" s="15"/>
+      <c r="AHB53" s="15"/>
+      <c r="AHC53" s="15"/>
+      <c r="AHD53" s="15"/>
+      <c r="AHE53" s="15"/>
+      <c r="AHF53" s="15"/>
+      <c r="AHG53" s="15"/>
+      <c r="AHH53" s="15"/>
+      <c r="AHI53" s="15"/>
+      <c r="AHJ53" s="15"/>
+      <c r="AHK53" s="15"/>
+      <c r="AHL53" s="15"/>
+      <c r="AHM53" s="15"/>
+      <c r="AHN53" s="15"/>
+      <c r="AHO53" s="15"/>
+      <c r="AHP53" s="15"/>
+      <c r="AHQ53" s="15"/>
+      <c r="AHR53" s="15"/>
+      <c r="AHS53" s="15"/>
+      <c r="AHT53" s="15"/>
+      <c r="AHU53" s="15"/>
+      <c r="AHV53" s="15"/>
+      <c r="AHW53" s="15"/>
+      <c r="AHX53" s="15"/>
+      <c r="AHY53" s="15"/>
+      <c r="AHZ53" s="15"/>
+      <c r="AIA53" s="15"/>
+      <c r="AIB53" s="15"/>
+      <c r="AIC53" s="15"/>
+      <c r="AID53" s="15"/>
+      <c r="AIE53" s="15"/>
+      <c r="AIF53" s="15"/>
+      <c r="AIG53" s="15"/>
+      <c r="AIH53" s="15"/>
+      <c r="AII53" s="15"/>
+      <c r="AIJ53" s="15"/>
+      <c r="AIK53" s="15"/>
+      <c r="AIL53" s="15"/>
+      <c r="AIM53" s="15"/>
+      <c r="AIN53" s="15"/>
+      <c r="AIO53" s="15"/>
+      <c r="AIP53" s="15"/>
+      <c r="AIQ53" s="15"/>
+      <c r="AIR53" s="15"/>
+      <c r="AIS53" s="15"/>
+      <c r="AIT53" s="15"/>
+      <c r="AIU53" s="15"/>
+      <c r="AIV53" s="15"/>
+      <c r="AIW53" s="15"/>
+      <c r="AIX53" s="15"/>
+      <c r="AIY53" s="15"/>
+      <c r="AIZ53" s="15"/>
+      <c r="AJA53" s="15"/>
+      <c r="AJB53" s="15"/>
+      <c r="AJC53" s="15"/>
+      <c r="AJD53" s="15"/>
+      <c r="AJE53" s="15"/>
+      <c r="AJF53" s="15"/>
+      <c r="AJG53" s="15"/>
+      <c r="AJH53" s="15"/>
+      <c r="AJI53" s="15"/>
+      <c r="AJJ53" s="15"/>
+      <c r="AJK53" s="15"/>
+      <c r="AJL53" s="15"/>
+      <c r="AJM53" s="15"/>
+      <c r="AJN53" s="15"/>
+      <c r="AJO53" s="15"/>
+      <c r="AJP53" s="15"/>
+      <c r="AJQ53" s="15"/>
+      <c r="AJR53" s="15"/>
+      <c r="AJS53" s="15"/>
+      <c r="AJT53" s="15"/>
+      <c r="AJU53" s="15"/>
+      <c r="AJV53" s="15"/>
+      <c r="AJW53" s="15"/>
+      <c r="AJX53" s="15"/>
+      <c r="AJY53" s="15"/>
+      <c r="AJZ53" s="15"/>
+      <c r="AKA53" s="15"/>
+      <c r="AKB53" s="15"/>
+      <c r="AKC53" s="15"/>
+      <c r="AKD53" s="15"/>
+      <c r="AKE53" s="15"/>
+      <c r="AKF53" s="15"/>
+      <c r="AKG53" s="15"/>
+      <c r="AKH53" s="15"/>
+      <c r="AKI53" s="15"/>
+      <c r="AKJ53" s="15"/>
+      <c r="AKK53" s="15"/>
+      <c r="AKL53" s="15"/>
+      <c r="AKM53" s="15"/>
+      <c r="AKN53" s="15"/>
+      <c r="AKO53" s="15"/>
+      <c r="AKP53" s="15"/>
+      <c r="AKQ53" s="15"/>
+      <c r="AKR53" s="15"/>
+      <c r="AKS53" s="15"/>
+      <c r="AKT53" s="15"/>
+      <c r="AKU53" s="15"/>
+      <c r="AKV53" s="15"/>
+      <c r="AKW53" s="15"/>
+      <c r="AKX53" s="15"/>
+      <c r="AKY53" s="15"/>
+      <c r="AKZ53" s="15"/>
+      <c r="ALA53" s="15"/>
+      <c r="ALB53" s="15"/>
+      <c r="ALC53" s="15"/>
+      <c r="ALD53" s="15"/>
+      <c r="ALE53" s="15"/>
+      <c r="ALF53" s="15"/>
+      <c r="ALG53" s="15"/>
+      <c r="ALH53" s="15"/>
+      <c r="ALI53" s="15"/>
+      <c r="ALJ53" s="15"/>
+      <c r="ALK53" s="15"/>
+      <c r="ALL53" s="15"/>
+      <c r="ALM53" s="15"/>
+      <c r="ALN53" s="15"/>
+      <c r="ALO53" s="15"/>
+      <c r="ALP53" s="15"/>
+      <c r="ALQ53" s="15"/>
+      <c r="ALR53" s="15"/>
+      <c r="ALS53" s="15"/>
+      <c r="ALT53" s="15"/>
+      <c r="ALU53" s="15"/>
+      <c r="ALV53" s="15"/>
+      <c r="ALW53" s="15"/>
+      <c r="ALX53" s="15"/>
+      <c r="ALY53" s="15"/>
+      <c r="ALZ53" s="15"/>
+      <c r="AMA53" s="15"/>
+      <c r="AMB53" s="15"/>
+      <c r="AMC53" s="15"/>
+      <c r="AMD53" s="15"/>
+      <c r="AME53" s="15"/>
+      <c r="AMF53" s="15"/>
+      <c r="AMG53" s="15"/>
+      <c r="AMH53" s="15"/>
+      <c r="AMI53" s="15"/>
+      <c r="AMJ53" s="15"/>
+      <c r="AMK53" s="15"/>
+      <c r="AML53" s="15"/>
+      <c r="AMM53" s="15"/>
+      <c r="AMN53" s="15"/>
+      <c r="AMO53" s="15"/>
+      <c r="AMP53" s="15"/>
+      <c r="AMQ53" s="15"/>
+      <c r="AMR53" s="15"/>
+      <c r="AMS53" s="15"/>
+    </row>
+    <row r="54" s="46" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="24" t="n">
+        <v>1048</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>463</v>
+      </c>
+      <c r="C54" s="27" t="n">
+        <v>6</v>
+      </c>
+      <c r="D54" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="F54" s="27"/>
+      <c r="G54" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="H54" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I54" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="J54" s="27" t="n">
+        <v>392715</v>
+      </c>
+      <c r="K54" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="L54" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="M54" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="N54" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="O54" s="27" t="s">
+        <v>465</v>
+      </c>
+      <c r="P54" s="27" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q54" s="27" t="n">
+        <v>29</v>
+      </c>
+      <c r="R54" s="27"/>
+      <c r="S54" s="27"/>
+      <c r="T54" s="27" t="n">
+        <v>16</v>
+      </c>
+      <c r="U54" s="27"/>
+      <c r="V54" s="27"/>
+      <c r="W54" s="32" t="n">
+        <v>107535</v>
+      </c>
+      <c r="X54" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y54" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="Z54" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA54" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB54" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="AB52" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC52" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="AD52" s="1" t="n">
+      <c r="AC54" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="AD54" s="27" t="n">
         <v>144183</v>
       </c>
-      <c r="AE52" s="1" t="s">
+      <c r="AE54" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="AF52" s="1" t="n">
-        <v>279726</v>
-      </c>
-      <c r="AG52" s="1" t="n">
+      <c r="AF54" s="27" t="n">
+        <v>20270</v>
+      </c>
+      <c r="AG54" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="AH52" s="1" t="s">
+      <c r="AH54" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="AI52" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="n">
-        <v>1047</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>457</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D53" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="G53" s="1" t="n">
-        <v>700</v>
-      </c>
-      <c r="H53" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J53" s="1" t="n">
-        <v>392714</v>
-      </c>
-      <c r="K53" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="P53" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="Q53" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="S53" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="T53" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="W53" s="8" t="n">
-        <v>107535</v>
-      </c>
-      <c r="X53" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y53" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="Z53" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AA53" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB53" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC53" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="AD53" s="1" t="n">
-        <v>281795</v>
-      </c>
-      <c r="AE53" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF53" s="1" t="n">
-        <v>81687</v>
-      </c>
-      <c r="AG53" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH53" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI53" s="8" t="s">
+      <c r="AI54" s="32" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="n">
-        <v>1048</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D54" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="G54" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="H54" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J54" s="1" t="n">
-        <v>392715</v>
-      </c>
-      <c r="K54" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="M54" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="N54" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="P54" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="Q54" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="T54" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="W54" s="8" t="n">
-        <v>107535</v>
-      </c>
-      <c r="X54" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y54" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="Z54" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA54" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB54" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC54" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="AD54" s="1" t="n">
-        <v>144183</v>
-      </c>
-      <c r="AE54" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF54" s="1" t="n">
-        <v>20270</v>
-      </c>
-      <c r="AG54" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH54" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI54" s="8" t="s">
-        <v>199</v>
-      </c>
+      <c r="AJ54" s="27"/>
+      <c r="AK54" s="27"/>
+      <c r="AL54" s="27"/>
+      <c r="AM54" s="27"/>
+      <c r="AN54" s="27"/>
+      <c r="AO54" s="27"/>
+      <c r="AP54" s="27"/>
+      <c r="AQ54" s="27"/>
+      <c r="AR54" s="27"/>
+      <c r="AS54" s="27"/>
+      <c r="AT54" s="24"/>
+      <c r="AU54" s="27"/>
+      <c r="AV54" s="24"/>
+      <c r="AW54" s="27"/>
+      <c r="AX54" s="27"/>
+      <c r="AY54" s="27"/>
+      <c r="AZ54" s="27"/>
+      <c r="BA54" s="27"/>
+      <c r="BB54" s="27"/>
+      <c r="BC54" s="27"/>
+      <c r="BD54" s="27"/>
+      <c r="BE54" s="27"/>
+      <c r="BF54" s="27"/>
+      <c r="BG54" s="27"/>
+      <c r="BH54" s="27"/>
+      <c r="BI54" s="27"/>
+      <c r="BJ54" s="27"/>
+      <c r="BK54" s="27"/>
+      <c r="BL54" s="27"/>
+      <c r="BM54" s="27"/>
+      <c r="BN54" s="27"/>
+      <c r="BO54" s="27"/>
+      <c r="BP54" s="27"/>
+      <c r="BQ54" s="27"/>
+      <c r="BR54" s="27"/>
+      <c r="BS54" s="27"/>
+      <c r="BT54" s="27"/>
+      <c r="BU54" s="27"/>
+      <c r="BV54" s="27"/>
+      <c r="BW54" s="27"/>
+      <c r="BX54" s="27"/>
+      <c r="BY54" s="27"/>
+      <c r="BZ54" s="27"/>
+      <c r="CA54" s="27"/>
+      <c r="CB54" s="27"/>
+      <c r="CC54" s="27"/>
+      <c r="CD54" s="27"/>
+      <c r="CE54" s="27"/>
+      <c r="CF54" s="27"/>
+      <c r="CG54" s="27"/>
+      <c r="CH54" s="27"/>
+      <c r="CI54" s="27"/>
+      <c r="CJ54" s="27"/>
+      <c r="CK54" s="27"/>
+      <c r="CL54" s="27"/>
+      <c r="CM54" s="27"/>
+      <c r="CN54" s="27"/>
+      <c r="CO54" s="27"/>
+      <c r="CP54" s="27"/>
+      <c r="CQ54" s="27"/>
+      <c r="CR54" s="27"/>
+      <c r="CS54" s="27"/>
+      <c r="CT54" s="27"/>
+      <c r="CU54" s="27"/>
+      <c r="CV54" s="27"/>
+      <c r="CW54" s="27"/>
+      <c r="CX54" s="27"/>
+      <c r="CY54" s="27"/>
+      <c r="CZ54" s="27"/>
+      <c r="DA54" s="27"/>
+      <c r="DB54" s="27"/>
+      <c r="DC54" s="27"/>
+      <c r="DD54" s="27"/>
+      <c r="DE54" s="27"/>
+      <c r="DF54" s="27"/>
+      <c r="DG54" s="27"/>
+      <c r="DH54" s="27"/>
+      <c r="DI54" s="27"/>
+      <c r="DJ54" s="27"/>
+      <c r="DK54" s="27"/>
+      <c r="DL54" s="27"/>
+      <c r="DM54" s="27"/>
+      <c r="DN54" s="27"/>
+      <c r="DO54" s="27"/>
+      <c r="DP54" s="27"/>
+      <c r="DQ54" s="27"/>
+      <c r="DR54" s="27"/>
+      <c r="DS54" s="27"/>
+      <c r="DT54" s="27"/>
+      <c r="DU54" s="27"/>
+      <c r="DV54" s="27"/>
+      <c r="DW54" s="27"/>
+      <c r="DX54" s="27"/>
+      <c r="DY54" s="27"/>
+      <c r="DZ54" s="27"/>
+      <c r="EA54" s="27"/>
+      <c r="EB54" s="27"/>
+      <c r="EC54" s="27"/>
+      <c r="ED54" s="27"/>
+      <c r="EE54" s="27"/>
+      <c r="EF54" s="27"/>
+      <c r="EG54" s="27"/>
+      <c r="EH54" s="27"/>
+      <c r="EI54" s="27"/>
+      <c r="EJ54" s="27"/>
+      <c r="EK54" s="27"/>
+      <c r="EL54" s="27"/>
+      <c r="EM54" s="27"/>
+      <c r="EN54" s="27"/>
+      <c r="EO54" s="27"/>
+      <c r="EP54" s="27"/>
+      <c r="EQ54" s="27"/>
+      <c r="ER54" s="27"/>
+      <c r="ES54" s="27"/>
+      <c r="ET54" s="27"/>
+      <c r="EU54" s="27"/>
+      <c r="EV54" s="27"/>
+      <c r="EW54" s="27"/>
+      <c r="EX54" s="27"/>
+      <c r="EY54" s="27"/>
+      <c r="EZ54" s="27"/>
+      <c r="FA54" s="27"/>
+      <c r="FB54" s="27"/>
+      <c r="FC54" s="27"/>
+      <c r="FD54" s="27"/>
+      <c r="FE54" s="27"/>
+      <c r="FF54" s="27"/>
+      <c r="FG54" s="27"/>
+      <c r="FH54" s="27"/>
+      <c r="FI54" s="27"/>
+      <c r="FJ54" s="27"/>
+      <c r="FK54" s="27"/>
+      <c r="FL54" s="27"/>
+      <c r="FM54" s="27"/>
+      <c r="FN54" s="27"/>
+      <c r="FO54" s="27"/>
+      <c r="FP54" s="27"/>
+      <c r="FQ54" s="27"/>
+      <c r="FR54" s="27"/>
+      <c r="FS54" s="27"/>
+      <c r="FT54" s="27"/>
+      <c r="FU54" s="27"/>
+      <c r="FV54" s="27"/>
+      <c r="FW54" s="27"/>
+      <c r="FX54" s="27"/>
+      <c r="FY54" s="27"/>
+      <c r="FZ54" s="27"/>
+      <c r="GA54" s="27"/>
+      <c r="GB54" s="27"/>
+      <c r="GC54" s="27"/>
+      <c r="GD54" s="27"/>
+      <c r="GE54" s="27"/>
+      <c r="GF54" s="27"/>
+      <c r="GG54" s="27"/>
+      <c r="GH54" s="27"/>
+      <c r="GI54" s="27"/>
+      <c r="GJ54" s="27"/>
+      <c r="GK54" s="27"/>
+      <c r="GL54" s="27"/>
+      <c r="GM54" s="27"/>
+      <c r="GN54" s="27"/>
+      <c r="GO54" s="27"/>
+      <c r="GP54" s="27"/>
+      <c r="GQ54" s="27"/>
+      <c r="GR54" s="27"/>
+      <c r="GS54" s="27"/>
+      <c r="GT54" s="27"/>
+      <c r="GU54" s="27"/>
+      <c r="GV54" s="27"/>
+      <c r="GW54" s="27"/>
+      <c r="GX54" s="27"/>
+      <c r="GY54" s="27"/>
+      <c r="GZ54" s="27"/>
+      <c r="HA54" s="27"/>
+      <c r="HB54" s="27"/>
+      <c r="HC54" s="27"/>
+      <c r="HD54" s="27"/>
+      <c r="HE54" s="27"/>
+      <c r="HF54" s="27"/>
+      <c r="HG54" s="27"/>
+      <c r="HH54" s="27"/>
+      <c r="HI54" s="27"/>
+      <c r="HJ54" s="27"/>
+      <c r="HK54" s="27"/>
+      <c r="HL54" s="27"/>
+      <c r="HM54" s="27"/>
+      <c r="HN54" s="27"/>
+      <c r="HO54" s="27"/>
+      <c r="HP54" s="27"/>
+      <c r="HQ54" s="27"/>
+      <c r="HR54" s="27"/>
+      <c r="HS54" s="27"/>
+      <c r="HT54" s="27"/>
+      <c r="HU54" s="27"/>
+      <c r="HV54" s="27"/>
+      <c r="HW54" s="27"/>
+      <c r="HX54" s="27"/>
+      <c r="HY54" s="27"/>
+      <c r="HZ54" s="27"/>
+      <c r="IA54" s="27"/>
+      <c r="IB54" s="27"/>
+      <c r="IC54" s="27"/>
+      <c r="ID54" s="27"/>
+      <c r="IE54" s="27"/>
+      <c r="IF54" s="27"/>
+      <c r="IG54" s="27"/>
+      <c r="IH54" s="27"/>
+      <c r="II54" s="27"/>
+      <c r="IJ54" s="27"/>
+      <c r="IK54" s="27"/>
+      <c r="IL54" s="27"/>
+      <c r="IM54" s="27"/>
+      <c r="IN54" s="27"/>
+      <c r="IO54" s="27"/>
+      <c r="IP54" s="27"/>
+      <c r="IQ54" s="27"/>
+      <c r="IR54" s="27"/>
+      <c r="IS54" s="27"/>
+      <c r="IT54" s="27"/>
+      <c r="IU54" s="27"/>
+      <c r="IV54" s="27"/>
+      <c r="IW54" s="27"/>
+      <c r="IX54" s="27"/>
+      <c r="IY54" s="27"/>
+      <c r="IZ54" s="27"/>
+      <c r="JA54" s="27"/>
+      <c r="JB54" s="27"/>
+      <c r="JC54" s="27"/>
+      <c r="JD54" s="27"/>
+      <c r="JE54" s="27"/>
+      <c r="JF54" s="27"/>
+      <c r="JG54" s="27"/>
+      <c r="JH54" s="27"/>
+      <c r="JI54" s="27"/>
+      <c r="JJ54" s="27"/>
+      <c r="JK54" s="27"/>
+      <c r="JL54" s="27"/>
+      <c r="JM54" s="27"/>
+      <c r="JN54" s="27"/>
+      <c r="JO54" s="27"/>
+      <c r="JP54" s="27"/>
+      <c r="JQ54" s="27"/>
+      <c r="JR54" s="27"/>
+      <c r="JS54" s="27"/>
+      <c r="JT54" s="27"/>
+      <c r="JU54" s="27"/>
+      <c r="JV54" s="27"/>
+      <c r="JW54" s="27"/>
+      <c r="JX54" s="27"/>
+      <c r="JY54" s="27"/>
+      <c r="JZ54" s="27"/>
+      <c r="KA54" s="27"/>
+      <c r="KB54" s="27"/>
+      <c r="KC54" s="27"/>
+      <c r="KD54" s="27"/>
+      <c r="KE54" s="27"/>
+      <c r="KF54" s="27"/>
+      <c r="KG54" s="27"/>
+      <c r="KH54" s="27"/>
+      <c r="KI54" s="27"/>
+      <c r="KJ54" s="27"/>
+      <c r="KK54" s="27"/>
+      <c r="KL54" s="27"/>
+      <c r="KM54" s="27"/>
+      <c r="KN54" s="27"/>
+      <c r="KO54" s="27"/>
+      <c r="KP54" s="27"/>
+      <c r="KQ54" s="27"/>
+      <c r="KR54" s="27"/>
+      <c r="KS54" s="27"/>
+      <c r="KT54" s="27"/>
+      <c r="KU54" s="27"/>
+      <c r="KV54" s="27"/>
+      <c r="KW54" s="27"/>
+      <c r="KX54" s="27"/>
+      <c r="KY54" s="27"/>
+      <c r="KZ54" s="27"/>
+      <c r="LA54" s="27"/>
+      <c r="LB54" s="27"/>
+      <c r="LC54" s="27"/>
+      <c r="LD54" s="27"/>
+      <c r="LE54" s="27"/>
+      <c r="LF54" s="27"/>
+      <c r="LG54" s="27"/>
+      <c r="LH54" s="27"/>
+      <c r="LI54" s="27"/>
+      <c r="LJ54" s="27"/>
+      <c r="LK54" s="27"/>
+      <c r="LL54" s="27"/>
+      <c r="LM54" s="27"/>
+      <c r="LN54" s="27"/>
+      <c r="LO54" s="27"/>
+      <c r="LP54" s="27"/>
+      <c r="LQ54" s="27"/>
+      <c r="LR54" s="27"/>
+      <c r="LS54" s="27"/>
+      <c r="LT54" s="27"/>
+      <c r="LU54" s="27"/>
+      <c r="LV54" s="27"/>
+      <c r="LW54" s="27"/>
+      <c r="LX54" s="27"/>
+      <c r="LY54" s="27"/>
+      <c r="LZ54" s="27"/>
+      <c r="MA54" s="27"/>
+      <c r="MB54" s="27"/>
+      <c r="MC54" s="27"/>
+      <c r="MD54" s="27"/>
+      <c r="ME54" s="27"/>
+      <c r="MF54" s="27"/>
+      <c r="MG54" s="27"/>
+      <c r="MH54" s="27"/>
+      <c r="MI54" s="27"/>
+      <c r="MJ54" s="27"/>
+      <c r="MK54" s="27"/>
+      <c r="ML54" s="27"/>
+      <c r="MM54" s="27"/>
+      <c r="MN54" s="27"/>
+      <c r="MO54" s="27"/>
+      <c r="MP54" s="27"/>
+      <c r="MQ54" s="27"/>
+      <c r="MR54" s="27"/>
+      <c r="MS54" s="27"/>
+      <c r="MT54" s="27"/>
+      <c r="MU54" s="27"/>
+      <c r="MV54" s="27"/>
+      <c r="MW54" s="27"/>
+      <c r="MX54" s="27"/>
+      <c r="MY54" s="27"/>
+      <c r="MZ54" s="27"/>
+      <c r="NA54" s="27"/>
+      <c r="NB54" s="27"/>
+      <c r="NC54" s="27"/>
+      <c r="ND54" s="27"/>
+      <c r="NE54" s="27"/>
+      <c r="NF54" s="27"/>
+      <c r="NG54" s="27"/>
+      <c r="NH54" s="27"/>
+      <c r="NI54" s="27"/>
+      <c r="NJ54" s="27"/>
+      <c r="NK54" s="27"/>
+      <c r="NL54" s="27"/>
+      <c r="NM54" s="27"/>
+      <c r="NN54" s="27"/>
+      <c r="NO54" s="27"/>
+      <c r="NP54" s="27"/>
+      <c r="NQ54" s="27"/>
+      <c r="NR54" s="27"/>
+      <c r="NS54" s="27"/>
+      <c r="NT54" s="27"/>
+      <c r="NU54" s="27"/>
+      <c r="NV54" s="27"/>
+      <c r="NW54" s="27"/>
+      <c r="NX54" s="27"/>
+      <c r="NY54" s="27"/>
+      <c r="NZ54" s="27"/>
+      <c r="OA54" s="27"/>
+      <c r="OB54" s="27"/>
+      <c r="OC54" s="27"/>
+      <c r="OD54" s="27"/>
+      <c r="OE54" s="27"/>
+      <c r="OF54" s="27"/>
+      <c r="OG54" s="27"/>
+      <c r="OH54" s="27"/>
+      <c r="OI54" s="27"/>
+      <c r="OJ54" s="27"/>
+      <c r="OK54" s="27"/>
+      <c r="OL54" s="27"/>
+      <c r="OM54" s="27"/>
+      <c r="ON54" s="27"/>
+      <c r="OO54" s="27"/>
+      <c r="OP54" s="27"/>
+      <c r="OQ54" s="27"/>
+      <c r="OR54" s="27"/>
+      <c r="OS54" s="27"/>
+      <c r="OT54" s="27"/>
+      <c r="OU54" s="27"/>
+      <c r="OV54" s="27"/>
+      <c r="OW54" s="27"/>
+      <c r="OX54" s="27"/>
+      <c r="OY54" s="27"/>
+      <c r="OZ54" s="27"/>
+      <c r="PA54" s="27"/>
+      <c r="PB54" s="27"/>
+      <c r="PC54" s="27"/>
+      <c r="PD54" s="27"/>
+      <c r="PE54" s="27"/>
+      <c r="PF54" s="27"/>
+      <c r="PG54" s="27"/>
+      <c r="PH54" s="27"/>
+      <c r="PI54" s="27"/>
+      <c r="PJ54" s="27"/>
+      <c r="PK54" s="27"/>
+      <c r="PL54" s="27"/>
+      <c r="PM54" s="27"/>
+      <c r="PN54" s="27"/>
+      <c r="PO54" s="27"/>
+      <c r="PP54" s="27"/>
+      <c r="PQ54" s="27"/>
+      <c r="PR54" s="27"/>
+      <c r="PS54" s="27"/>
+      <c r="PT54" s="27"/>
+      <c r="PU54" s="27"/>
+      <c r="PV54" s="27"/>
+      <c r="PW54" s="27"/>
+      <c r="PX54" s="27"/>
+      <c r="PY54" s="27"/>
+      <c r="PZ54" s="27"/>
+      <c r="QA54" s="27"/>
+      <c r="QB54" s="27"/>
+      <c r="QC54" s="27"/>
+      <c r="QD54" s="27"/>
+      <c r="QE54" s="27"/>
+      <c r="QF54" s="27"/>
+      <c r="QG54" s="27"/>
+      <c r="QH54" s="27"/>
+      <c r="QI54" s="27"/>
+      <c r="QJ54" s="27"/>
+      <c r="QK54" s="27"/>
+      <c r="QL54" s="27"/>
+      <c r="QM54" s="27"/>
+      <c r="QN54" s="27"/>
+      <c r="QO54" s="27"/>
+      <c r="QP54" s="27"/>
+      <c r="QQ54" s="27"/>
+      <c r="QR54" s="27"/>
+      <c r="QS54" s="27"/>
+      <c r="QT54" s="27"/>
+      <c r="QU54" s="27"/>
+      <c r="QV54" s="27"/>
+      <c r="QW54" s="27"/>
+      <c r="QX54" s="27"/>
+      <c r="QY54" s="27"/>
+      <c r="QZ54" s="27"/>
+      <c r="RA54" s="27"/>
+      <c r="RB54" s="27"/>
+      <c r="RC54" s="27"/>
+      <c r="RD54" s="27"/>
+      <c r="RE54" s="27"/>
+      <c r="RF54" s="27"/>
+      <c r="RG54" s="27"/>
+      <c r="RH54" s="27"/>
+      <c r="RI54" s="27"/>
+      <c r="RJ54" s="27"/>
+      <c r="RK54" s="27"/>
+      <c r="RL54" s="27"/>
+      <c r="RM54" s="27"/>
+      <c r="RN54" s="27"/>
+      <c r="RO54" s="27"/>
+      <c r="RP54" s="27"/>
+      <c r="RQ54" s="27"/>
+      <c r="RR54" s="27"/>
+      <c r="RS54" s="27"/>
+      <c r="RT54" s="27"/>
+      <c r="RU54" s="27"/>
+      <c r="RV54" s="27"/>
+      <c r="RW54" s="27"/>
+      <c r="RX54" s="27"/>
+      <c r="RY54" s="27"/>
+      <c r="RZ54" s="27"/>
+      <c r="SA54" s="27"/>
+      <c r="SB54" s="27"/>
+      <c r="SC54" s="27"/>
+      <c r="SD54" s="27"/>
+      <c r="SE54" s="27"/>
+      <c r="SF54" s="27"/>
+      <c r="SG54" s="27"/>
+      <c r="SH54" s="27"/>
+      <c r="SI54" s="27"/>
+      <c r="SJ54" s="27"/>
+      <c r="SK54" s="27"/>
+      <c r="SL54" s="27"/>
+      <c r="SM54" s="27"/>
+      <c r="SN54" s="27"/>
+      <c r="SO54" s="27"/>
+      <c r="SP54" s="27"/>
+      <c r="SQ54" s="27"/>
+      <c r="SR54" s="27"/>
+      <c r="SS54" s="27"/>
+      <c r="ST54" s="27"/>
+      <c r="SU54" s="27"/>
+      <c r="SV54" s="27"/>
+      <c r="SW54" s="27"/>
+      <c r="SX54" s="27"/>
+      <c r="SY54" s="27"/>
+      <c r="SZ54" s="27"/>
+      <c r="TA54" s="27"/>
+      <c r="TB54" s="27"/>
+      <c r="TC54" s="27"/>
+      <c r="TD54" s="27"/>
+      <c r="TE54" s="27"/>
+      <c r="TF54" s="27"/>
+      <c r="TG54" s="27"/>
+      <c r="TH54" s="27"/>
+      <c r="TI54" s="27"/>
+      <c r="TJ54" s="27"/>
+      <c r="TK54" s="27"/>
+      <c r="TL54" s="27"/>
+      <c r="TM54" s="27"/>
+      <c r="TN54" s="27"/>
+      <c r="TO54" s="27"/>
+      <c r="TP54" s="27"/>
+      <c r="TQ54" s="27"/>
+      <c r="TR54" s="27"/>
+      <c r="TS54" s="27"/>
+      <c r="TT54" s="27"/>
+      <c r="TU54" s="27"/>
+      <c r="TV54" s="27"/>
+      <c r="TW54" s="27"/>
+      <c r="TX54" s="27"/>
+      <c r="TY54" s="27"/>
+      <c r="TZ54" s="27"/>
+      <c r="UA54" s="27"/>
+      <c r="UB54" s="27"/>
+      <c r="UC54" s="27"/>
+      <c r="UD54" s="27"/>
+      <c r="UE54" s="27"/>
+      <c r="UF54" s="27"/>
+      <c r="UG54" s="27"/>
+      <c r="UH54" s="27"/>
+      <c r="UI54" s="27"/>
+      <c r="UJ54" s="27"/>
+      <c r="UK54" s="27"/>
+      <c r="UL54" s="27"/>
+      <c r="UM54" s="27"/>
+      <c r="UN54" s="27"/>
+      <c r="UO54" s="27"/>
+      <c r="UP54" s="27"/>
+      <c r="UQ54" s="27"/>
+      <c r="UR54" s="27"/>
+      <c r="US54" s="27"/>
+      <c r="UT54" s="27"/>
+      <c r="UU54" s="27"/>
+      <c r="UV54" s="27"/>
+      <c r="UW54" s="27"/>
+      <c r="UX54" s="27"/>
+      <c r="UY54" s="27"/>
+      <c r="UZ54" s="27"/>
+      <c r="VA54" s="27"/>
+      <c r="VB54" s="27"/>
+      <c r="VC54" s="27"/>
+      <c r="VD54" s="27"/>
+      <c r="VE54" s="27"/>
+      <c r="VF54" s="27"/>
+      <c r="VG54" s="27"/>
+      <c r="VH54" s="27"/>
+      <c r="VI54" s="27"/>
+      <c r="VJ54" s="27"/>
+      <c r="VK54" s="27"/>
+      <c r="VL54" s="27"/>
+      <c r="VM54" s="27"/>
+      <c r="VN54" s="27"/>
+      <c r="VO54" s="27"/>
+      <c r="VP54" s="27"/>
+      <c r="VQ54" s="27"/>
+      <c r="VR54" s="27"/>
+      <c r="VS54" s="27"/>
+      <c r="VT54" s="27"/>
+      <c r="VU54" s="27"/>
+      <c r="VV54" s="27"/>
+      <c r="VW54" s="27"/>
+      <c r="VX54" s="27"/>
+      <c r="VY54" s="27"/>
+      <c r="VZ54" s="27"/>
+      <c r="WA54" s="27"/>
+      <c r="WB54" s="27"/>
+      <c r="WC54" s="27"/>
+      <c r="WD54" s="27"/>
+      <c r="WE54" s="27"/>
+      <c r="WF54" s="27"/>
+      <c r="WG54" s="27"/>
+      <c r="WH54" s="27"/>
+      <c r="WI54" s="27"/>
+      <c r="WJ54" s="27"/>
+      <c r="WK54" s="27"/>
+      <c r="WL54" s="27"/>
+      <c r="WM54" s="27"/>
+      <c r="WN54" s="27"/>
+      <c r="WO54" s="27"/>
+      <c r="WP54" s="27"/>
+      <c r="WQ54" s="27"/>
+      <c r="WR54" s="27"/>
+      <c r="WS54" s="27"/>
+      <c r="WT54" s="27"/>
+      <c r="WU54" s="27"/>
+      <c r="WV54" s="27"/>
+      <c r="WW54" s="27"/>
+      <c r="WX54" s="27"/>
+      <c r="WY54" s="27"/>
+      <c r="WZ54" s="27"/>
+      <c r="XA54" s="27"/>
+      <c r="XB54" s="27"/>
+      <c r="XC54" s="27"/>
+      <c r="XD54" s="27"/>
+      <c r="XE54" s="27"/>
+      <c r="XF54" s="27"/>
+      <c r="XG54" s="27"/>
+      <c r="XH54" s="27"/>
+      <c r="XI54" s="27"/>
+      <c r="XJ54" s="27"/>
+      <c r="XK54" s="27"/>
+      <c r="XL54" s="27"/>
+      <c r="XM54" s="27"/>
+      <c r="XN54" s="27"/>
+      <c r="XO54" s="27"/>
+      <c r="XP54" s="27"/>
+      <c r="XQ54" s="27"/>
+      <c r="XR54" s="27"/>
+      <c r="XS54" s="27"/>
+      <c r="XT54" s="27"/>
+      <c r="XU54" s="27"/>
+      <c r="XV54" s="27"/>
+      <c r="XW54" s="27"/>
+      <c r="XX54" s="27"/>
+      <c r="XY54" s="27"/>
+      <c r="XZ54" s="27"/>
+      <c r="YA54" s="27"/>
+      <c r="YB54" s="27"/>
+      <c r="YC54" s="27"/>
+      <c r="YD54" s="27"/>
+      <c r="YE54" s="27"/>
+      <c r="YF54" s="27"/>
+      <c r="YG54" s="27"/>
+      <c r="YH54" s="27"/>
+      <c r="YI54" s="27"/>
+      <c r="YJ54" s="27"/>
+      <c r="YK54" s="27"/>
+      <c r="YL54" s="27"/>
+      <c r="YM54" s="27"/>
+      <c r="YN54" s="27"/>
+      <c r="YO54" s="27"/>
+      <c r="YP54" s="27"/>
+      <c r="YQ54" s="27"/>
+      <c r="YR54" s="27"/>
+      <c r="YS54" s="27"/>
+      <c r="YT54" s="27"/>
+      <c r="YU54" s="27"/>
+      <c r="YV54" s="27"/>
+      <c r="YW54" s="27"/>
+      <c r="YX54" s="27"/>
+      <c r="YY54" s="27"/>
+      <c r="YZ54" s="27"/>
+      <c r="ZA54" s="27"/>
+      <c r="ZB54" s="27"/>
+      <c r="ZC54" s="27"/>
+      <c r="ZD54" s="27"/>
+      <c r="ZE54" s="27"/>
+      <c r="ZF54" s="27"/>
+      <c r="ZG54" s="27"/>
+      <c r="ZH54" s="27"/>
+      <c r="ZI54" s="27"/>
+      <c r="ZJ54" s="27"/>
+      <c r="ZK54" s="27"/>
+      <c r="ZL54" s="27"/>
+      <c r="ZM54" s="27"/>
+      <c r="ZN54" s="27"/>
+      <c r="ZO54" s="27"/>
+      <c r="ZP54" s="27"/>
+      <c r="ZQ54" s="27"/>
+      <c r="ZR54" s="27"/>
+      <c r="ZS54" s="27"/>
+      <c r="ZT54" s="27"/>
+      <c r="ZU54" s="27"/>
+      <c r="ZV54" s="27"/>
+      <c r="ZW54" s="27"/>
+      <c r="ZX54" s="27"/>
+      <c r="ZY54" s="27"/>
+      <c r="ZZ54" s="27"/>
+      <c r="AAA54" s="27"/>
+      <c r="AAB54" s="27"/>
+      <c r="AAC54" s="27"/>
+      <c r="AAD54" s="27"/>
+      <c r="AAE54" s="27"/>
+      <c r="AAF54" s="27"/>
+      <c r="AAG54" s="27"/>
+      <c r="AAH54" s="27"/>
+      <c r="AAI54" s="27"/>
+      <c r="AAJ54" s="27"/>
+      <c r="AAK54" s="27"/>
+      <c r="AAL54" s="27"/>
+      <c r="AAM54" s="27"/>
+      <c r="AAN54" s="27"/>
+      <c r="AAO54" s="27"/>
+      <c r="AAP54" s="27"/>
+      <c r="AAQ54" s="27"/>
+      <c r="AAR54" s="27"/>
+      <c r="AAS54" s="27"/>
+      <c r="AAT54" s="27"/>
+      <c r="AAU54" s="27"/>
+      <c r="AAV54" s="27"/>
+      <c r="AAW54" s="27"/>
+      <c r="AAX54" s="27"/>
+      <c r="AAY54" s="27"/>
+      <c r="AAZ54" s="27"/>
+      <c r="ABA54" s="27"/>
+      <c r="ABB54" s="27"/>
+      <c r="ABC54" s="27"/>
+      <c r="ABD54" s="27"/>
+      <c r="ABE54" s="27"/>
+      <c r="ABF54" s="27"/>
+      <c r="ABG54" s="27"/>
+      <c r="ABH54" s="27"/>
+      <c r="ABI54" s="27"/>
+      <c r="ABJ54" s="27"/>
+      <c r="ABK54" s="27"/>
+      <c r="ABL54" s="27"/>
+      <c r="ABM54" s="27"/>
+      <c r="ABN54" s="27"/>
+      <c r="ABO54" s="27"/>
+      <c r="ABP54" s="27"/>
+      <c r="ABQ54" s="27"/>
+      <c r="ABR54" s="27"/>
+      <c r="ABS54" s="27"/>
+      <c r="ABT54" s="27"/>
+      <c r="ABU54" s="27"/>
+      <c r="ABV54" s="27"/>
+      <c r="ABW54" s="27"/>
+      <c r="ABX54" s="27"/>
+      <c r="ABY54" s="27"/>
+      <c r="ABZ54" s="27"/>
+      <c r="ACA54" s="27"/>
+      <c r="ACB54" s="27"/>
+      <c r="ACC54" s="27"/>
+      <c r="ACD54" s="27"/>
+      <c r="ACE54" s="27"/>
+      <c r="ACF54" s="27"/>
+      <c r="ACG54" s="27"/>
+      <c r="ACH54" s="27"/>
+      <c r="ACI54" s="27"/>
+      <c r="ACJ54" s="27"/>
+      <c r="ACK54" s="27"/>
+      <c r="ACL54" s="27"/>
+      <c r="ACM54" s="27"/>
+      <c r="ACN54" s="27"/>
+      <c r="ACO54" s="27"/>
+      <c r="ACP54" s="27"/>
+      <c r="ACQ54" s="27"/>
+      <c r="ACR54" s="27"/>
+      <c r="ACS54" s="27"/>
+      <c r="ACT54" s="27"/>
+      <c r="ACU54" s="27"/>
+      <c r="ACV54" s="27"/>
+      <c r="ACW54" s="27"/>
+      <c r="ACX54" s="27"/>
+      <c r="ACY54" s="27"/>
+      <c r="ACZ54" s="27"/>
+      <c r="ADA54" s="27"/>
+      <c r="ADB54" s="27"/>
+      <c r="ADC54" s="27"/>
+      <c r="ADD54" s="27"/>
+      <c r="ADE54" s="27"/>
+      <c r="ADF54" s="27"/>
+      <c r="ADG54" s="27"/>
+      <c r="ADH54" s="27"/>
+      <c r="ADI54" s="27"/>
+      <c r="ADJ54" s="27"/>
+      <c r="ADK54" s="27"/>
+      <c r="ADL54" s="27"/>
+      <c r="ADM54" s="27"/>
+      <c r="ADN54" s="27"/>
+      <c r="ADO54" s="27"/>
+      <c r="ADP54" s="27"/>
+      <c r="ADQ54" s="27"/>
+      <c r="ADR54" s="27"/>
+      <c r="ADS54" s="27"/>
+      <c r="ADT54" s="27"/>
+      <c r="ADU54" s="27"/>
+      <c r="ADV54" s="27"/>
+      <c r="ADW54" s="27"/>
+      <c r="ADX54" s="27"/>
+      <c r="ADY54" s="27"/>
+      <c r="ADZ54" s="27"/>
+      <c r="AEA54" s="27"/>
+      <c r="AEB54" s="27"/>
+      <c r="AEC54" s="27"/>
+      <c r="AED54" s="27"/>
+      <c r="AEE54" s="27"/>
+      <c r="AEF54" s="27"/>
+      <c r="AEG54" s="27"/>
+      <c r="AEH54" s="27"/>
+      <c r="AEI54" s="27"/>
+      <c r="AEJ54" s="27"/>
+      <c r="AEK54" s="27"/>
+      <c r="AEL54" s="27"/>
+      <c r="AEM54" s="27"/>
+      <c r="AEN54" s="27"/>
+      <c r="AEO54" s="27"/>
+      <c r="AEP54" s="27"/>
+      <c r="AEQ54" s="27"/>
+      <c r="AER54" s="27"/>
+      <c r="AES54" s="27"/>
+      <c r="AET54" s="27"/>
+      <c r="AEU54" s="27"/>
+      <c r="AEV54" s="27"/>
+      <c r="AEW54" s="27"/>
+      <c r="AEX54" s="27"/>
+      <c r="AEY54" s="27"/>
+      <c r="AEZ54" s="27"/>
+      <c r="AFA54" s="27"/>
+      <c r="AFB54" s="27"/>
+      <c r="AFC54" s="27"/>
+      <c r="AFD54" s="27"/>
+      <c r="AFE54" s="27"/>
+      <c r="AFF54" s="27"/>
+      <c r="AFG54" s="27"/>
+      <c r="AFH54" s="27"/>
+      <c r="AFI54" s="27"/>
+      <c r="AFJ54" s="27"/>
+      <c r="AFK54" s="27"/>
+      <c r="AFL54" s="27"/>
+      <c r="AFM54" s="27"/>
+      <c r="AFN54" s="27"/>
+      <c r="AFO54" s="27"/>
+      <c r="AFP54" s="27"/>
+      <c r="AFQ54" s="27"/>
+      <c r="AFR54" s="27"/>
+      <c r="AFS54" s="27"/>
+      <c r="AFT54" s="27"/>
+      <c r="AFU54" s="27"/>
+      <c r="AFV54" s="27"/>
+      <c r="AFW54" s="27"/>
+      <c r="AFX54" s="27"/>
+      <c r="AFY54" s="27"/>
+      <c r="AFZ54" s="27"/>
+      <c r="AGA54" s="27"/>
+      <c r="AGB54" s="27"/>
+      <c r="AGC54" s="27"/>
+      <c r="AGD54" s="27"/>
+      <c r="AGE54" s="27"/>
+      <c r="AGF54" s="27"/>
+      <c r="AGG54" s="27"/>
+      <c r="AGH54" s="27"/>
+      <c r="AGI54" s="27"/>
+      <c r="AGJ54" s="27"/>
+      <c r="AGK54" s="27"/>
+      <c r="AGL54" s="27"/>
+      <c r="AGM54" s="27"/>
+      <c r="AGN54" s="27"/>
+      <c r="AGO54" s="27"/>
+      <c r="AGP54" s="27"/>
+      <c r="AGQ54" s="27"/>
+      <c r="AGR54" s="27"/>
+      <c r="AGS54" s="27"/>
+      <c r="AGT54" s="27"/>
+      <c r="AGU54" s="27"/>
+      <c r="AGV54" s="27"/>
+      <c r="AGW54" s="27"/>
+      <c r="AGX54" s="27"/>
+      <c r="AGY54" s="27"/>
+      <c r="AGZ54" s="27"/>
+      <c r="AHA54" s="27"/>
+      <c r="AHB54" s="27"/>
+      <c r="AHC54" s="27"/>
+      <c r="AHD54" s="27"/>
+      <c r="AHE54" s="27"/>
+      <c r="AHF54" s="27"/>
+      <c r="AHG54" s="27"/>
+      <c r="AHH54" s="27"/>
+      <c r="AHI54" s="27"/>
+      <c r="AHJ54" s="27"/>
+      <c r="AHK54" s="27"/>
+      <c r="AHL54" s="27"/>
+      <c r="AHM54" s="27"/>
+      <c r="AHN54" s="27"/>
+      <c r="AHO54" s="27"/>
+      <c r="AHP54" s="27"/>
+      <c r="AHQ54" s="27"/>
+      <c r="AHR54" s="27"/>
+      <c r="AHS54" s="27"/>
+      <c r="AHT54" s="27"/>
+      <c r="AHU54" s="27"/>
+      <c r="AHV54" s="27"/>
+      <c r="AHW54" s="27"/>
+      <c r="AHX54" s="27"/>
+      <c r="AHY54" s="27"/>
+      <c r="AHZ54" s="27"/>
+      <c r="AIA54" s="27"/>
+      <c r="AIB54" s="27"/>
+      <c r="AIC54" s="27"/>
+      <c r="AID54" s="27"/>
+      <c r="AIE54" s="27"/>
+      <c r="AIF54" s="27"/>
+      <c r="AIG54" s="27"/>
+      <c r="AIH54" s="27"/>
+      <c r="AII54" s="27"/>
+      <c r="AIJ54" s="27"/>
+      <c r="AIK54" s="27"/>
+      <c r="AIL54" s="27"/>
+      <c r="AIM54" s="27"/>
+      <c r="AIN54" s="27"/>
+      <c r="AIO54" s="27"/>
+      <c r="AIP54" s="27"/>
+      <c r="AIQ54" s="27"/>
+      <c r="AIR54" s="27"/>
+      <c r="AIS54" s="27"/>
+      <c r="AIT54" s="27"/>
+      <c r="AIU54" s="27"/>
+      <c r="AIV54" s="27"/>
+      <c r="AIW54" s="27"/>
+      <c r="AIX54" s="27"/>
+      <c r="AIY54" s="27"/>
+      <c r="AIZ54" s="27"/>
+      <c r="AJA54" s="27"/>
+      <c r="AJB54" s="27"/>
+      <c r="AJC54" s="27"/>
+      <c r="AJD54" s="27"/>
+      <c r="AJE54" s="27"/>
+      <c r="AJF54" s="27"/>
+      <c r="AJG54" s="27"/>
+      <c r="AJH54" s="27"/>
+      <c r="AJI54" s="27"/>
+      <c r="AJJ54" s="27"/>
+      <c r="AJK54" s="27"/>
+      <c r="AJL54" s="27"/>
+      <c r="AJM54" s="27"/>
+      <c r="AJN54" s="27"/>
+      <c r="AJO54" s="27"/>
+      <c r="AJP54" s="27"/>
+      <c r="AJQ54" s="27"/>
+      <c r="AJR54" s="27"/>
+      <c r="AJS54" s="27"/>
+      <c r="AJT54" s="27"/>
+      <c r="AJU54" s="27"/>
+      <c r="AJV54" s="27"/>
+      <c r="AJW54" s="27"/>
+      <c r="AJX54" s="27"/>
+      <c r="AJY54" s="27"/>
+      <c r="AJZ54" s="27"/>
+      <c r="AKA54" s="27"/>
+      <c r="AKB54" s="27"/>
+      <c r="AKC54" s="27"/>
+      <c r="AKD54" s="27"/>
+      <c r="AKE54" s="27"/>
+      <c r="AKF54" s="27"/>
+      <c r="AKG54" s="27"/>
+      <c r="AKH54" s="27"/>
+      <c r="AKI54" s="27"/>
+      <c r="AKJ54" s="27"/>
+      <c r="AKK54" s="27"/>
+      <c r="AKL54" s="27"/>
+      <c r="AKM54" s="27"/>
+      <c r="AKN54" s="27"/>
+      <c r="AKO54" s="27"/>
+      <c r="AKP54" s="27"/>
+      <c r="AKQ54" s="27"/>
+      <c r="AKR54" s="27"/>
+      <c r="AKS54" s="27"/>
+      <c r="AKT54" s="27"/>
+      <c r="AKU54" s="27"/>
+      <c r="AKV54" s="27"/>
+      <c r="AKW54" s="27"/>
+      <c r="AKX54" s="27"/>
+      <c r="AKY54" s="27"/>
+      <c r="AKZ54" s="27"/>
+      <c r="ALA54" s="27"/>
+      <c r="ALB54" s="27"/>
+      <c r="ALC54" s="27"/>
+      <c r="ALD54" s="27"/>
+      <c r="ALE54" s="27"/>
+      <c r="ALF54" s="27"/>
+      <c r="ALG54" s="27"/>
+      <c r="ALH54" s="27"/>
+      <c r="ALI54" s="27"/>
+      <c r="ALJ54" s="27"/>
+      <c r="ALK54" s="27"/>
+      <c r="ALL54" s="27"/>
+      <c r="ALM54" s="27"/>
+      <c r="ALN54" s="27"/>
+      <c r="ALO54" s="27"/>
+      <c r="ALP54" s="27"/>
+      <c r="ALQ54" s="27"/>
+      <c r="ALR54" s="27"/>
+      <c r="ALS54" s="27"/>
+      <c r="ALT54" s="27"/>
+      <c r="ALU54" s="27"/>
+      <c r="ALV54" s="27"/>
+      <c r="ALW54" s="27"/>
+      <c r="ALX54" s="27"/>
+      <c r="ALY54" s="27"/>
+      <c r="ALZ54" s="27"/>
+      <c r="AMA54" s="27"/>
+      <c r="AMB54" s="27"/>
+      <c r="AMC54" s="27"/>
+      <c r="AMD54" s="27"/>
+      <c r="AME54" s="27"/>
+      <c r="AMF54" s="27"/>
+      <c r="AMG54" s="27"/>
+      <c r="AMH54" s="27"/>
+      <c r="AMI54" s="27"/>
+      <c r="AMJ54" s="27"/>
+      <c r="AMK54" s="27"/>
+      <c r="AML54" s="27"/>
+      <c r="AMM54" s="27"/>
+      <c r="AMN54" s="27"/>
+      <c r="AMO54" s="27"/>
+      <c r="AMP54" s="27"/>
+      <c r="AMQ54" s="27"/>
+      <c r="AMR54" s="27"/>
+      <c r="AMS54" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat：update new buff and tower excel change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="390">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -588,19 +588,22 @@
     <t xml:space="preserve">attackDamage|findRange</t>
   </si>
   <si>
-    <t xml:space="preserve">250|450|750</t>
+    <t xml:space="preserve">150|300|450</t>
   </si>
   <si>
-    <t xml:space="preserve">120|300|600</t>
+    <t xml:space="preserve">75|150|225</t>
   </si>
   <si>
     <t xml:space="preserve">2156CCFE49B0B0F804086C96D2F8166C|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
   </si>
   <si>
+    <t xml:space="preserve">5|5|5</t>
+  </si>
+  <si>
     <t xml:space="preserve">100|150|250</t>
   </si>
   <si>
-    <t xml:space="preserve">2001||2002||2003</t>
+    <t xml:space="preserve">4023||4024||4025</t>
   </si>
   <si>
     <t xml:space="preserve">Tower_name_20</t>
@@ -717,9 +720,6 @@
     <t xml:space="preserve">AB4D06E34849041AB9D5C084904B8036|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
   </si>
   <si>
-    <t xml:space="preserve">5|5|5</t>
-  </si>
-  <si>
     <t xml:space="preserve">15|25|40</t>
   </si>
   <si>
@@ -730,6 +730,12 @@
   </si>
   <si>
     <t xml:space="preserve">Tower_attackTags_9|Tower_attackTags_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200|400|600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100|200|300</t>
   </si>
   <si>
     <t xml:space="preserve">2413BE794DFD89225C6BB1984BF3B39A|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
@@ -744,16 +750,31 @@
     <t xml:space="preserve">40|60|80</t>
   </si>
   <si>
+    <t xml:space="preserve">4026||4027||4028</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tower_name_26</t>
   </si>
   <si>
     <t xml:space="preserve">暗龙娘7</t>
   </si>
   <si>
+    <t xml:space="preserve">250|400|550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">125|200|275</t>
+  </si>
+  <si>
     <t xml:space="preserve">4E3FA2424F946AAFD47668983B3506B9|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
   </si>
   <si>
+    <t xml:space="preserve">10|10|10</t>
+  </si>
+  <si>
     <t xml:space="preserve">60|80|100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4029||4030||4031</t>
   </si>
   <si>
     <t xml:space="preserve">Tower_name_27</t>
@@ -1032,7 +1053,16 @@
     <t xml:space="preserve">火龙少6</t>
   </si>
   <si>
+    <t xml:space="preserve">400|650|900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200|325|450</t>
+  </si>
+  <si>
     <t xml:space="preserve">6992D1454962F1D5D06B77B19228941B|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4032||4033||4034</t>
   </si>
   <si>
     <t xml:space="preserve">Tower_name_39</t>
@@ -1304,16 +1334,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">60|120|180</t>
+    <t xml:space="preserve">350|500|800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">175|250|400</t>
   </si>
   <si>
     <t xml:space="preserve">A9EDEC8F43483A421EBD97A16A7F99BD|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
   </si>
   <si>
-    <t xml:space="preserve">15|12|9</t>
+    <t xml:space="preserve">10|20|30</t>
   </si>
   <si>
-    <t xml:space="preserve">10|20|30</t>
+    <t xml:space="preserve">4035||4036||4037</t>
   </si>
 </sst>
 </file>
@@ -1909,10 +1942,10 @@
   </sheetPr>
   <dimension ref="A1:AMS54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="D7" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="topRight" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="L4" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topRight" activeCell="P46" activeCellId="0" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15260,7 +15293,7 @@
         <v>1</v>
       </c>
       <c r="Y23" s="44" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="Z23" s="44" t="s">
         <v>88</v>
@@ -15269,10 +15302,10 @@
         <v>132</v>
       </c>
       <c r="AB23" s="44" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="AC23" s="44" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AD23" s="44" t="n">
         <v>279748</v>
@@ -15286,7 +15319,7 @@
         <v>101</v>
       </c>
       <c r="AI23" s="43" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AJ23" s="44"/>
       <c r="AK23" s="44"/>
@@ -16292,7 +16325,7 @@
         <v>1008</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C24" s="14" t="n">
         <v>2</v>
@@ -16301,7 +16334,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="18" t="n">
@@ -16321,13 +16354,13 @@
         <v>83</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O24" s="18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="P24" s="18" t="n">
         <v>16</v>
@@ -16339,7 +16372,7 @@
         <v>600</v>
       </c>
       <c r="S24" s="18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="T24" s="18" t="n">
         <v>16</v>
@@ -16355,7 +16388,7 @@
         <v>1</v>
       </c>
       <c r="Y24" s="18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Z24" s="18" t="s">
         <v>88</v>
@@ -16367,7 +16400,7 @@
         <v>120</v>
       </c>
       <c r="AC24" s="18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AD24" s="16" t="n">
         <v>285370</v>
@@ -16376,7 +16409,7 @@
         <v>91</v>
       </c>
       <c r="AF24" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AG24" s="18" t="n">
         <v>1.5</v>
@@ -17389,7 +17422,7 @@
         <v>1009</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C25" s="14" t="n">
         <v>2</v>
@@ -17398,7 +17431,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F25" s="14" t="n">
         <v>7</v>
@@ -17420,13 +17453,13 @@
         <v>83</v>
       </c>
       <c r="M25" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="N25" s="20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O25" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="P25" s="18" t="n">
         <v>18</v>
@@ -17438,7 +17471,7 @@
         <v>400</v>
       </c>
       <c r="S25" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T25" s="18" t="n">
         <v>16</v>
@@ -17454,19 +17487,19 @@
         <v>1.3</v>
       </c>
       <c r="Y25" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Z25" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AA25" s="18" t="s">
         <v>89</v>
       </c>
       <c r="AB25" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AC25" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AD25" s="18" t="n">
         <v>146119</v>
@@ -17484,7 +17517,7 @@
         <v>101</v>
       </c>
       <c r="AI25" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AJ25" s="18"/>
       <c r="AK25" s="18"/>
@@ -18490,7 +18523,7 @@
         <v>1010</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C26" s="14" t="n">
         <v>2</v>
@@ -18499,7 +18532,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="18" t="n">
@@ -18521,13 +18554,13 @@
         <v>83</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N26" s="20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O26" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="P26" s="18" t="n">
         <v>18</v>
@@ -18539,7 +18572,7 @@
         <v>200</v>
       </c>
       <c r="S26" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="T26" s="18" t="n">
         <v>16</v>
@@ -18555,7 +18588,7 @@
         <v>1.5</v>
       </c>
       <c r="Y26" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Z26" s="18" t="s">
         <v>88</v>
@@ -18564,10 +18597,10 @@
         <v>89</v>
       </c>
       <c r="AB26" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AC26" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AD26" s="16" t="n">
         <v>144198</v>
@@ -19589,7 +19622,7 @@
         <v>1011</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C27" s="47" t="n">
         <v>2</v>
@@ -19598,7 +19631,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="47" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F27" s="47" t="n">
         <v>3</v>
@@ -19620,13 +19653,13 @@
         <v>83</v>
       </c>
       <c r="M27" s="51" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="N27" s="51" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="O27" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="P27" s="49" t="n">
         <v>18</v>
@@ -19638,7 +19671,7 @@
         <v>500</v>
       </c>
       <c r="S27" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="T27" s="49" t="n">
         <v>16</v>
@@ -19654,19 +19687,19 @@
         <v>0.8</v>
       </c>
       <c r="Y27" s="49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="Z27" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AA27" s="49" t="s">
         <v>89</v>
       </c>
       <c r="AB27" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AC27" s="49" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD27" s="49" t="n">
         <v>281886</v>
@@ -19684,7 +19717,7 @@
         <v>101</v>
       </c>
       <c r="AI27" s="49" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AJ27" s="49"/>
       <c r="AK27" s="49"/>
@@ -20690,7 +20723,7 @@
         <v>1012</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C28" s="27" t="n">
         <v>2</v>
@@ -20699,7 +20732,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F28" s="27"/>
       <c r="G28" s="29" t="n">
@@ -20719,13 +20752,13 @@
         <v>126</v>
       </c>
       <c r="M28" s="35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N28" s="35" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O28" s="30" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="P28" s="29" t="n">
         <v>20</v>
@@ -20751,7 +20784,7 @@
         <v>1</v>
       </c>
       <c r="Y28" s="30" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="Z28" s="30" t="s">
         <v>131</v>
@@ -21814,13 +21847,13 @@
         <v>145</v>
       </c>
       <c r="M29" s="43" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="N29" s="43" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="O29" s="44" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="P29" s="44"/>
       <c r="Q29" s="44"/>
@@ -21836,10 +21869,10 @@
         <v>1</v>
       </c>
       <c r="Y29" s="44" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="Z29" s="44" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AA29" s="44" t="s">
         <v>132</v>
@@ -21848,7 +21881,7 @@
         <v>132</v>
       </c>
       <c r="AC29" s="44" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AD29" s="44" t="n">
         <v>285237</v>
@@ -21862,7 +21895,7 @@
         <v>101</v>
       </c>
       <c r="AI29" s="43" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="AJ29" s="44"/>
       <c r="AK29" s="44"/>
@@ -22868,7 +22901,7 @@
         <v>1014</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C30" s="38" t="n">
         <v>2</v>
@@ -22877,7 +22910,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F30" s="44"/>
       <c r="G30" s="44" t="n">
@@ -22897,13 +22930,13 @@
         <v>145</v>
       </c>
       <c r="M30" s="43" t="s">
-        <v>146</v>
+        <v>203</v>
       </c>
       <c r="N30" s="43" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
       <c r="O30" s="44" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="P30" s="44"/>
       <c r="Q30" s="44"/>
@@ -22919,7 +22952,7 @@
         <v>1</v>
       </c>
       <c r="Y30" s="44" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="Z30" s="44" t="s">
         <v>88</v>
@@ -22931,7 +22964,7 @@
         <v>132</v>
       </c>
       <c r="AC30" s="44" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="AD30" s="44" t="n">
         <v>285459</v>
@@ -22945,7 +22978,7 @@
         <v>101</v>
       </c>
       <c r="AI30" s="43" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="AJ30" s="44"/>
       <c r="AK30" s="44"/>
@@ -23951,7 +23984,7 @@
         <v>1015</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C31" s="49" t="n">
         <v>3</v>
@@ -23960,7 +23993,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="49" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="F31" s="49" t="n">
         <v>9</v>
@@ -23982,13 +24015,13 @@
         <v>83</v>
       </c>
       <c r="M31" s="49" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="N31" s="49" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="O31" s="49" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="P31" s="49" t="n">
         <v>22</v>
@@ -24000,14 +24033,14 @@
         <v>300</v>
       </c>
       <c r="S31" s="49" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="T31" s="49" t="n">
         <v>16</v>
       </c>
       <c r="U31" s="49"/>
       <c r="V31" s="49" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="W31" s="49" t="n">
         <v>151576</v>
@@ -24016,10 +24049,10 @@
         <v>1</v>
       </c>
       <c r="Y31" s="49" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="Z31" s="49" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AA31" s="49" t="s">
         <v>89</v>
@@ -24028,7 +24061,7 @@
         <v>99</v>
       </c>
       <c r="AC31" s="49" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AD31" s="49" t="n">
         <v>281788</v>
@@ -24037,7 +24070,7 @@
         <v>91</v>
       </c>
       <c r="AF31" s="49" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="AG31" s="49" t="n">
         <v>0.4</v>
@@ -24046,7 +24079,7 @@
         <v>101</v>
       </c>
       <c r="AI31" s="49" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ31" s="49"/>
       <c r="AK31" s="49"/>
@@ -25052,7 +25085,7 @@
         <v>1016</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="C32" s="49" t="n">
         <v>3</v>
@@ -25061,7 +25094,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="49" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="F32" s="49" t="n">
         <v>7</v>
@@ -25083,13 +25116,13 @@
         <v>83</v>
       </c>
       <c r="M32" s="49" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="N32" s="49" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O32" s="49" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="P32" s="49" t="n">
         <v>22</v>
@@ -25101,14 +25134,14 @@
         <v>200</v>
       </c>
       <c r="S32" s="49" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="T32" s="49" t="n">
         <v>16</v>
       </c>
       <c r="U32" s="49"/>
       <c r="V32" s="49" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="W32" s="49" t="n">
         <v>168944</v>
@@ -25120,16 +25153,16 @@
         <v>119</v>
       </c>
       <c r="Z32" s="49" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="AA32" s="49" t="s">
         <v>89</v>
       </c>
       <c r="AB32" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AC32" s="49" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="AD32" s="49" t="n">
         <v>285400</v>
@@ -25138,7 +25171,7 @@
         <v>91</v>
       </c>
       <c r="AF32" s="49" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AG32" s="49" t="n">
         <v>0.4</v>
@@ -25147,7 +25180,7 @@
         <v>101</v>
       </c>
       <c r="AI32" s="49" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="AJ32" s="49"/>
       <c r="AK32" s="49"/>
@@ -26153,7 +26186,7 @@
         <v>1017</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C33" s="49" t="n">
         <v>3</v>
@@ -26162,7 +26195,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="49" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="F33" s="49" t="n">
         <v>2</v>
@@ -26186,13 +26219,13 @@
         <v>83</v>
       </c>
       <c r="M33" s="49" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="N33" s="49" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="O33" s="49" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="P33" s="49" t="n">
         <v>22</v>
@@ -26204,7 +26237,7 @@
         <v>100</v>
       </c>
       <c r="S33" s="49" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="T33" s="49" t="n">
         <v>16</v>
@@ -26220,10 +26253,10 @@
         <v>1.2</v>
       </c>
       <c r="Y33" s="49" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="Z33" s="49" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="AA33" s="49" t="s">
         <v>89</v>
@@ -26232,7 +26265,7 @@
         <v>99</v>
       </c>
       <c r="AC33" s="49" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="AD33" s="49" t="n">
         <v>281710</v>
@@ -27254,7 +27287,7 @@
         <v>1018</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="C34" s="49" t="n">
         <v>3</v>
@@ -27263,7 +27296,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="49" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="F34" s="49" t="n">
         <v>4</v>
@@ -27285,13 +27318,13 @@
         <v>83</v>
       </c>
       <c r="M34" s="49" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="N34" s="49" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="O34" s="49" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="P34" s="49" t="n">
         <v>22</v>
@@ -27300,17 +27333,17 @@
         <v>23</v>
       </c>
       <c r="R34" s="49" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="S34" s="49" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="T34" s="49" t="n">
         <v>16</v>
       </c>
       <c r="U34" s="49"/>
       <c r="V34" s="49" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="W34" s="49" t="n">
         <v>288335</v>
@@ -27319,19 +27352,19 @@
         <v>0.5</v>
       </c>
       <c r="Y34" s="49" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z34" s="49" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="AA34" s="49" t="s">
         <v>89</v>
       </c>
       <c r="AB34" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AC34" s="49" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="AD34" s="49" t="n">
         <v>299561</v>
@@ -27340,7 +27373,7 @@
         <v>91</v>
       </c>
       <c r="AF34" s="49" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AG34" s="49" t="n">
         <v>2</v>
@@ -27349,7 +27382,7 @@
         <v>101</v>
       </c>
       <c r="AI34" s="49" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="AJ34" s="49"/>
       <c r="AK34" s="49"/>
@@ -28355,7 +28388,7 @@
         <v>1019</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C35" s="49" t="n">
         <v>3</v>
@@ -28364,7 +28397,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="49" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="F35" s="49"/>
       <c r="G35" s="49" t="n">
@@ -28384,13 +28417,13 @@
         <v>83</v>
       </c>
       <c r="M35" s="49" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="N35" s="49" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="O35" s="49" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="P35" s="49" t="n">
         <v>22</v>
@@ -28402,7 +28435,7 @@
         <v>117</v>
       </c>
       <c r="S35" s="49" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="T35" s="49" t="n">
         <v>16</v>
@@ -28430,7 +28463,7 @@
         <v>99</v>
       </c>
       <c r="AC35" s="49" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="AD35" s="49" t="n">
         <v>285356</v>
@@ -28439,7 +28472,7 @@
         <v>91</v>
       </c>
       <c r="AF35" s="49" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="AG35" s="49" t="n">
         <v>2</v>
@@ -29452,7 +29485,7 @@
         <v>1020</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C36" s="49" t="n">
         <v>3</v>
@@ -29461,7 +29494,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="49" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="F36" s="49" t="n">
         <v>2</v>
@@ -29485,13 +29518,13 @@
         <v>83</v>
       </c>
       <c r="M36" s="49" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="N36" s="49" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="O36" s="49" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="P36" s="49" t="n">
         <v>22</v>
@@ -29500,17 +29533,17 @@
         <v>23</v>
       </c>
       <c r="R36" s="49" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="S36" s="49" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="T36" s="49" t="n">
         <v>16</v>
       </c>
       <c r="U36" s="49"/>
       <c r="V36" s="49" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="W36" s="49" t="n">
         <v>254276</v>
@@ -29531,16 +29564,16 @@
         <v>99</v>
       </c>
       <c r="AC36" s="49" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="AD36" s="49" t="n">
         <v>20301</v>
       </c>
       <c r="AE36" s="49" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="AF36" s="49" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="AG36" s="49" t="n">
         <v>3</v>
@@ -30553,7 +30586,7 @@
         <v>1021</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C37" s="49" t="n">
         <v>4</v>
@@ -30562,7 +30595,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="49" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="F37" s="49" t="n">
         <v>8</v>
@@ -30586,13 +30619,13 @@
         <v>83</v>
       </c>
       <c r="M37" s="49" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="N37" s="49" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="O37" s="49" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="P37" s="49" t="n">
         <v>24</v>
@@ -30604,7 +30637,7 @@
         <v>100</v>
       </c>
       <c r="S37" s="49" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="T37" s="49" t="n">
         <v>16</v>
@@ -30620,7 +30653,7 @@
         <v>1</v>
       </c>
       <c r="Y37" s="49" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="Z37" s="49" t="s">
         <v>88</v>
@@ -30632,7 +30665,7 @@
         <v>109</v>
       </c>
       <c r="AC37" s="49" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="AD37" s="49" t="n">
         <v>281710</v>
@@ -30650,7 +30683,7 @@
         <v>101</v>
       </c>
       <c r="AI37" s="56" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="AJ37" s="49"/>
       <c r="AK37" s="49"/>
@@ -31656,7 +31689,7 @@
         <v>1022</v>
       </c>
       <c r="B38" s="46" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C38" s="49" t="n">
         <v>4</v>
@@ -31665,7 +31698,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="49" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="F38" s="49" t="n">
         <v>4</v>
@@ -31687,13 +31720,13 @@
         <v>83</v>
       </c>
       <c r="M38" s="49" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="N38" s="49" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="O38" s="49" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="P38" s="49" t="n">
         <v>24</v>
@@ -31705,14 +31738,14 @@
         <v>200</v>
       </c>
       <c r="S38" s="49" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="T38" s="49" t="n">
         <v>16</v>
       </c>
       <c r="U38" s="49"/>
       <c r="V38" s="49" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="W38" s="49" t="n">
         <v>271321</v>
@@ -31721,7 +31754,7 @@
         <v>0.8</v>
       </c>
       <c r="Y38" s="49" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="Z38" s="49" t="s">
         <v>88</v>
@@ -31730,10 +31763,10 @@
         <v>89</v>
       </c>
       <c r="AB38" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AC38" s="49" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="AD38" s="49" t="n">
         <v>281871</v>
@@ -31742,7 +31775,7 @@
         <v>91</v>
       </c>
       <c r="AF38" s="49" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="AG38" s="49" t="n">
         <v>1</v>
@@ -31751,7 +31784,7 @@
         <v>101</v>
       </c>
       <c r="AI38" s="49" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="AJ38" s="49"/>
       <c r="AK38" s="49"/>
@@ -32757,7 +32790,7 @@
         <v>1023</v>
       </c>
       <c r="B39" s="46" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C39" s="49" t="n">
         <v>4</v>
@@ -32766,7 +32799,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="F39" s="49" t="n">
         <v>10</v>
@@ -32790,13 +32823,13 @@
         <v>83</v>
       </c>
       <c r="M39" s="49" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="N39" s="49" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="O39" s="49" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="P39" s="49" t="n">
         <v>24</v>
@@ -32808,7 +32841,7 @@
         <v>200</v>
       </c>
       <c r="S39" s="49" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="T39" s="49" t="n">
         <v>16</v>
@@ -32824,7 +32857,7 @@
         <v>1.5</v>
       </c>
       <c r="Y39" s="49" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="Z39" s="49" t="s">
         <v>88</v>
@@ -32836,7 +32869,7 @@
         <v>99</v>
       </c>
       <c r="AC39" s="49" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="AD39" s="49" t="n">
         <v>300932</v>
@@ -33858,7 +33891,7 @@
         <v>1024</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C40" s="49" t="n">
         <v>4</v>
@@ -33867,7 +33900,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="49" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="F40" s="49"/>
       <c r="G40" s="49" t="n">
@@ -33887,13 +33920,13 @@
         <v>83</v>
       </c>
       <c r="M40" s="49" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="N40" s="49" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="O40" s="49" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="P40" s="49" t="n">
         <v>24</v>
@@ -33905,7 +33938,7 @@
         <v>300</v>
       </c>
       <c r="S40" s="49" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="T40" s="49" t="n">
         <v>16</v>
@@ -33921,7 +33954,7 @@
         <v>1.5</v>
       </c>
       <c r="Y40" s="49" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="Z40" s="49" t="s">
         <v>88</v>
@@ -33933,7 +33966,7 @@
         <v>99</v>
       </c>
       <c r="AC40" s="49" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="AD40" s="49" t="n">
         <v>117391</v>
@@ -34955,7 +34988,7 @@
         <v>1025</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="C41" s="49" t="n">
         <v>4</v>
@@ -34964,7 +34997,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="49" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="F41" s="49" t="n">
         <v>6</v>
@@ -34986,13 +35019,13 @@
         <v>83</v>
       </c>
       <c r="M41" s="49" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="N41" s="49" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="O41" s="49" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="P41" s="49" t="n">
         <v>24</v>
@@ -35004,7 +35037,7 @@
         <v>100</v>
       </c>
       <c r="S41" s="49" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="T41" s="49" t="n">
         <v>16</v>
@@ -35023,16 +35056,16 @@
         <v>87</v>
       </c>
       <c r="Z41" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AA41" s="49" t="s">
         <v>89</v>
       </c>
       <c r="AB41" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AC41" s="49" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="AD41" s="49" t="n">
         <v>285445</v>
@@ -35050,7 +35083,7 @@
         <v>101</v>
       </c>
       <c r="AI41" s="49" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="AJ41" s="49"/>
       <c r="AK41" s="49"/>
@@ -36056,7 +36089,7 @@
         <v>1026</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C42" s="44" t="n">
         <v>4</v>
@@ -36065,7 +36098,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="44" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="F42" s="44"/>
       <c r="G42" s="44" t="n">
@@ -36085,13 +36118,13 @@
         <v>145</v>
       </c>
       <c r="M42" s="43" t="s">
-        <v>146</v>
+        <v>301</v>
       </c>
       <c r="N42" s="43" t="s">
-        <v>146</v>
+        <v>302</v>
       </c>
       <c r="O42" s="44" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="P42" s="44" t="n">
         <v>24</v>
@@ -36111,10 +36144,10 @@
         <v>1</v>
       </c>
       <c r="Y42" s="44" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="Z42" s="44" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AA42" s="44" t="s">
         <v>132</v>
@@ -36123,7 +36156,7 @@
         <v>132</v>
       </c>
       <c r="AC42" s="44" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AD42" s="44" t="n">
         <v>94268</v>
@@ -36137,7 +36170,7 @@
         <v>101</v>
       </c>
       <c r="AI42" s="43" t="s">
-        <v>150</v>
+        <v>304</v>
       </c>
       <c r="AJ42" s="44"/>
       <c r="AK42" s="44"/>
@@ -37143,7 +37176,7 @@
         <v>1027</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="C43" s="18" t="n">
         <v>5</v>
@@ -37152,7 +37185,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="F43" s="18"/>
       <c r="G43" s="18" t="n">
@@ -37172,13 +37205,13 @@
         <v>83</v>
       </c>
       <c r="M43" s="18" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="N43" s="18" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="O43" s="18" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="P43" s="18" t="n">
         <v>26</v>
@@ -37190,7 +37223,7 @@
         <v>100</v>
       </c>
       <c r="S43" s="18" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="T43" s="18" t="n">
         <v>16</v>
@@ -37216,7 +37249,7 @@
         <v>109</v>
       </c>
       <c r="AC43" s="18" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="AD43" s="18" t="n">
         <v>279765</v>
@@ -37234,7 +37267,7 @@
         <v>101</v>
       </c>
       <c r="AI43" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AJ43" s="18"/>
       <c r="AK43" s="18"/>
@@ -38240,7 +38273,7 @@
         <v>1028</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="C44" s="18" t="n">
         <v>5</v>
@@ -38249,7 +38282,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="F44" s="18"/>
       <c r="G44" s="18" t="n">
@@ -38269,13 +38302,13 @@
         <v>83</v>
       </c>
       <c r="M44" s="18" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="N44" s="18" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="O44" s="18" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="P44" s="18" t="n">
         <v>44</v>
@@ -38287,7 +38320,7 @@
         <v>100</v>
       </c>
       <c r="S44" s="18" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="T44" s="18" t="n">
         <v>16</v>
@@ -38303,7 +38336,7 @@
         <v>1.4</v>
       </c>
       <c r="Y44" s="18" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="Z44" s="18" t="s">
         <v>88</v>
@@ -38315,7 +38348,7 @@
         <v>109</v>
       </c>
       <c r="AC44" s="18" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="AD44" s="18" t="n">
         <v>85944</v>
@@ -39337,7 +39370,7 @@
         <v>1029</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="C45" s="18" t="n">
         <v>5</v>
@@ -39346,7 +39379,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="F45" s="18" t="n">
         <v>3</v>
@@ -39368,13 +39401,13 @@
         <v>83</v>
       </c>
       <c r="M45" s="18" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="N45" s="18" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="O45" s="18" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="P45" s="18" t="n">
         <v>46</v>
@@ -39386,7 +39419,7 @@
         <v>400</v>
       </c>
       <c r="S45" s="18" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="T45" s="18" t="n">
         <v>16</v>
@@ -39402,10 +39435,10 @@
         <v>1</v>
       </c>
       <c r="Y45" s="18" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="Z45" s="18" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AA45" s="18" t="s">
         <v>89</v>
@@ -39414,7 +39447,7 @@
         <v>99</v>
       </c>
       <c r="AC45" s="18" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="AD45" s="18" t="n">
         <v>326802</v>
@@ -39432,7 +39465,7 @@
         <v>101</v>
       </c>
       <c r="AI45" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AJ45" s="18"/>
       <c r="AK45" s="18"/>
@@ -40438,7 +40471,7 @@
         <v>1030</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C46" s="18" t="n">
         <v>5</v>
@@ -40447,7 +40480,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="F46" s="18" t="n">
         <v>6</v>
@@ -40469,13 +40502,13 @@
         <v>83</v>
       </c>
       <c r="M46" s="18" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="N46" s="18" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="O46" s="18" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="P46" s="18" t="n">
         <v>48</v>
@@ -40485,7 +40518,7 @@
       </c>
       <c r="R46" s="18"/>
       <c r="S46" s="18" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="T46" s="18" t="n">
         <v>16</v>
@@ -40501,7 +40534,7 @@
         <v>1</v>
       </c>
       <c r="Y46" s="18" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="Z46" s="18" t="s">
         <v>109</v>
@@ -40513,7 +40546,7 @@
         <v>88</v>
       </c>
       <c r="AC46" s="18" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="AD46" s="18" t="n">
         <v>281871</v>
@@ -40531,7 +40564,7 @@
         <v>101</v>
       </c>
       <c r="AI46" s="49" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="AJ46" s="18"/>
       <c r="AK46" s="18"/>
@@ -41537,7 +41570,7 @@
         <v>1031</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="C47" s="30" t="n">
         <v>5</v>
@@ -41546,7 +41579,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="30" t="n">
@@ -41566,13 +41599,13 @@
         <v>126</v>
       </c>
       <c r="M47" s="30" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="N47" s="30" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="O47" s="30" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="P47" s="30" t="n">
         <v>40</v>
@@ -41584,7 +41617,7 @@
         <v>1000</v>
       </c>
       <c r="S47" s="30" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="T47" s="30" t="n">
         <v>16</v>
@@ -41598,7 +41631,7 @@
         <v>0.6</v>
       </c>
       <c r="Y47" s="30" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="Z47" s="30" t="s">
         <v>88</v>
@@ -41610,7 +41643,7 @@
         <v>88</v>
       </c>
       <c r="AC47" s="30" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="AD47" s="30" t="n">
         <v>285673</v>
@@ -42632,7 +42665,7 @@
         <v>1032</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="C48" s="27" t="n">
         <v>5</v>
@@ -42641,7 +42674,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="29" t="n">
@@ -42661,13 +42694,13 @@
         <v>126</v>
       </c>
       <c r="M48" s="30" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="N48" s="30" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="O48" s="30" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="P48" s="29" t="n">
         <v>42</v>
@@ -42703,7 +42736,7 @@
         <v>88</v>
       </c>
       <c r="AC48" s="30" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="AD48" s="30" t="n">
         <v>144183</v>
@@ -43725,7 +43758,7 @@
         <v>1033</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="C49" s="18" t="n">
         <v>6</v>
@@ -43734,7 +43767,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="F49" s="18" t="n">
         <v>5</v>
@@ -43756,13 +43789,13 @@
         <v>83</v>
       </c>
       <c r="M49" s="18" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="N49" s="18" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="O49" s="18" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="P49" s="18" t="n">
         <v>28</v>
@@ -43774,7 +43807,7 @@
         <v>350</v>
       </c>
       <c r="S49" s="18" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="T49" s="18" t="n">
         <v>16</v>
@@ -43790,10 +43823,10 @@
         <v>1.5</v>
       </c>
       <c r="Y49" s="18" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="Z49" s="18" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AA49" s="18" t="s">
         <v>89</v>
@@ -43802,7 +43835,7 @@
         <v>99</v>
       </c>
       <c r="AC49" s="18" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="AD49" s="18" t="n">
         <v>303259</v>
@@ -43820,7 +43853,7 @@
         <v>101</v>
       </c>
       <c r="AI49" s="18" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="AJ49" s="18"/>
       <c r="AK49" s="18"/>
@@ -44826,7 +44859,7 @@
         <v>1034</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="C50" s="18" t="n">
         <v>6</v>
@@ -44835,7 +44868,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="18" t="n">
@@ -44855,13 +44888,13 @@
         <v>83</v>
       </c>
       <c r="M50" s="18" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="N50" s="18" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="O50" s="18" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="P50" s="18" t="n">
         <v>30</v>
@@ -44873,7 +44906,7 @@
         <v>650</v>
       </c>
       <c r="S50" s="18" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="T50" s="18" t="n">
         <v>16</v>
@@ -44889,10 +44922,10 @@
         <v>1</v>
       </c>
       <c r="Y50" s="18" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="Z50" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AA50" s="18" t="s">
         <v>89</v>
@@ -44901,7 +44934,7 @@
         <v>88</v>
       </c>
       <c r="AC50" s="18" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="AD50" s="18" t="n">
         <v>305224</v>
@@ -45923,7 +45956,7 @@
         <v>1035</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="C51" s="18" t="n">
         <v>6</v>
@@ -45932,7 +45965,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="F51" s="18" t="n">
         <v>3</v>
@@ -45954,13 +45987,13 @@
         <v>83</v>
       </c>
       <c r="M51" s="18" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="N51" s="18" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="O51" s="18" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="P51" s="18" t="n">
         <v>32</v>
@@ -45972,7 +46005,7 @@
         <v>1000</v>
       </c>
       <c r="S51" s="18" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="T51" s="18" t="n">
         <v>16</v>
@@ -45988,7 +46021,7 @@
         <v>1</v>
       </c>
       <c r="Y51" s="18" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="Z51" s="18" t="s">
         <v>88</v>
@@ -46000,7 +46033,7 @@
         <v>109</v>
       </c>
       <c r="AC51" s="18" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="AD51" s="18" t="n">
         <v>269209</v>
@@ -46018,7 +46051,7 @@
         <v>101</v>
       </c>
       <c r="AI51" s="18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AJ51" s="18"/>
       <c r="AK51" s="18"/>
@@ -47024,7 +47057,7 @@
         <v>1036</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="C52" s="18" t="n">
         <v>6</v>
@@ -47033,7 +47066,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="F52" s="18" t="n">
         <v>6</v>
@@ -47045,7 +47078,7 @@
         <v>1</v>
       </c>
       <c r="I52" s="18" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="J52" s="18" t="n">
         <v>392709</v>
@@ -47057,13 +47090,13 @@
         <v>83</v>
       </c>
       <c r="M52" s="18" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="N52" s="18" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="O52" s="18" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="P52" s="18" t="n">
         <v>38</v>
@@ -47075,7 +47108,7 @@
         <v>500</v>
       </c>
       <c r="S52" s="18" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="T52" s="18" t="n">
         <v>16</v>
@@ -47091,7 +47124,7 @@
         <v>1</v>
       </c>
       <c r="Y52" s="18" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="Z52" s="18" t="s">
         <v>109</v>
@@ -47103,7 +47136,7 @@
         <v>99</v>
       </c>
       <c r="AC52" s="18" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="AD52" s="18" t="n">
         <v>144183</v>
@@ -47121,7 +47154,7 @@
         <v>101</v>
       </c>
       <c r="AI52" s="18" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="AJ52" s="18"/>
       <c r="AK52" s="18"/>
@@ -48127,7 +48160,7 @@
         <v>1037</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="C53" s="18" t="n">
         <v>6</v>
@@ -48136,7 +48169,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="F53" s="18"/>
       <c r="G53" s="18" t="n">
@@ -48146,7 +48179,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="18" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="J53" s="18" t="n">
         <v>392714</v>
@@ -48158,13 +48191,13 @@
         <v>83</v>
       </c>
       <c r="M53" s="18" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="N53" s="18" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="O53" s="18" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="P53" s="18" t="n">
         <v>34</v>
@@ -48174,7 +48207,7 @@
       </c>
       <c r="R53" s="18"/>
       <c r="S53" s="18" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="T53" s="18" t="n">
         <v>16</v>
@@ -48188,7 +48221,7 @@
         <v>2</v>
       </c>
       <c r="Y53" s="18" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="Z53" s="18" t="s">
         <v>99</v>
@@ -48200,7 +48233,7 @@
         <v>99</v>
       </c>
       <c r="AC53" s="18" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="AD53" s="18" t="n">
         <v>281795</v>
@@ -49222,7 +49255,7 @@
         <v>1038</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="C54" s="44" t="n">
         <v>6</v>
@@ -49231,7 +49264,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="44" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="F54" s="44"/>
       <c r="G54" s="39" t="n">
@@ -49241,25 +49274,25 @@
         <v>2</v>
       </c>
       <c r="I54" s="44" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="J54" s="44" t="n">
         <v>392715</v>
       </c>
       <c r="K54" s="55" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="L54" s="44" t="s">
         <v>126</v>
       </c>
       <c r="M54" s="43" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="N54" s="43" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="O54" s="44" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="P54" s="44" t="n">
         <v>36</v>
@@ -49281,7 +49314,7 @@
         <v>1</v>
       </c>
       <c r="Y54" s="44" t="s">
-        <v>377</v>
+        <v>197</v>
       </c>
       <c r="Z54" s="44" t="s">
         <v>131</v>
@@ -49293,7 +49326,7 @@
         <v>89</v>
       </c>
       <c r="AC54" s="44" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="AD54" s="44" t="n">
         <v>144183</v>
@@ -49311,7 +49344,7 @@
         <v>101</v>
       </c>
       <c r="AI54" s="43" t="s">
-        <v>150</v>
+        <v>389</v>
       </c>
       <c r="AJ54" s="44"/>
       <c r="AK54" s="44"/>

</xml_diff>

<commit_message>
feat: update UI and config
更新UI和多语言和塔表
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4908C72F-0134-4F70-A1A7-084694AD3BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9658782-629E-4412-8A57-574EE76B1652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="398">
   <si>
     <t>int</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>elementTy</t>
-  </si>
-  <si>
-    <t>adap</t>
   </si>
   <si>
     <t>nameCN</t>
@@ -593,9 +590,6 @@
     <t>5|5|5</t>
   </si>
   <si>
-    <t>100|150|250</t>
-  </si>
-  <si>
     <t>4023||4024||4025</t>
   </si>
   <si>
@@ -740,9 +734,6 @@
     <t>2|2|2</t>
   </si>
   <si>
-    <t>40|60|80</t>
-  </si>
-  <si>
     <t>4026||4027||4028</t>
   </si>
   <si>
@@ -762,9 +753,6 @@
   </si>
   <si>
     <t>10|10|10</t>
-  </si>
-  <si>
-    <t>60|80|100</t>
   </si>
   <si>
     <t>4029||4030||4031</t>
@@ -1390,7 +1378,27 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>80|100|120</t>
+    <t>150|300|400</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>30|40|50</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>80|90|100</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>250|350|450</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>50|60|80</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>adap</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1870,10 +1878,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMS54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="AK43" sqref="AK43"/>
+      <selection pane="topRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -2071,103 +2079,103 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
@@ -2197,112 +2205,112 @@
     </row>
     <row r="3" spans="1:1031" ht="95.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AA3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AB3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AF3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AH3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AH3" s="5" t="s">
+      <c r="AI3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AI3" s="5" t="s">
+      <c r="AJ3" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
@@ -2332,7 +2340,7 @@
     </row>
     <row r="4" spans="1:1031" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:1031" x14ac:dyDescent="0.35">
@@ -8527,7 +8535,7 @@
         <v>1001</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="11">
         <v>1</v>
@@ -8536,7 +8544,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="13">
@@ -8550,19 +8558,19 @@
         <v>392760</v>
       </c>
       <c r="K17" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L17" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="M17" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="N17" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="O17" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="N17" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="P17" s="15">
         <v>2</v>
@@ -8574,7 +8582,7 @@
         <v>200</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T17" s="15">
         <v>16</v>
@@ -8588,25 +8596,25 @@
         <v>0.3</v>
       </c>
       <c r="Y17" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Z17" s="15" t="s">
+      <c r="AA17" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA17" s="15" t="s">
+      <c r="AB17" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC17" s="15" t="s">
         <v>89</v>
-      </c>
-      <c r="AB17" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC17" s="15" t="s">
-        <v>90</v>
       </c>
       <c r="AD17" s="15">
         <v>144183</v>
       </c>
       <c r="AE17" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF17" s="15">
         <v>279719</v>
@@ -8615,7 +8623,7 @@
         <v>0.5</v>
       </c>
       <c r="AH17" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AI17" s="15"/>
       <c r="AJ17" s="15"/>
@@ -9622,7 +9630,7 @@
         <v>1002</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="11">
         <v>1</v>
@@ -9631,7 +9639,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="13">
@@ -9645,19 +9653,19 @@
         <v>392757</v>
       </c>
       <c r="K18" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="L18" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="L18" s="22" t="s">
-        <v>83</v>
-      </c>
       <c r="M18" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="N18" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="O18" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="N18" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="O18" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="P18" s="15">
         <v>4</v>
@@ -9669,7 +9677,7 @@
         <v>300</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T18" s="15">
         <v>16</v>
@@ -9685,25 +9693,25 @@
         <v>1.5</v>
       </c>
       <c r="Y18" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA18" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB18" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="Z18" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA18" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB18" s="15" t="s">
+      <c r="AC18" s="15" t="s">
         <v>99</v>
-      </c>
-      <c r="AC18" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="AD18" s="15">
         <v>284848</v>
       </c>
       <c r="AE18" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF18" s="15">
         <v>121794</v>
@@ -9712,7 +9720,7 @@
         <v>2.5</v>
       </c>
       <c r="AH18" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI18" s="15"/>
       <c r="AJ18" s="15"/>
@@ -10719,7 +10727,7 @@
         <v>1003</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="11">
         <v>1</v>
@@ -10728,7 +10736,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="11">
         <v>8</v>
@@ -10746,38 +10754,38 @@
         <v>392761</v>
       </c>
       <c r="K19" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="L19" s="22" t="s">
-        <v>83</v>
-      </c>
       <c r="M19" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="N19" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="O19" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="N19" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="O19" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="P19" s="15">
         <v>6</v>
       </c>
       <c r="Q19" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="R19" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="R19" s="15" t="s">
+      <c r="S19" s="15" t="s">
         <v>107</v>
-      </c>
-      <c r="S19" s="15" t="s">
-        <v>108</v>
       </c>
       <c r="T19" s="15">
         <v>16</v>
       </c>
       <c r="U19" s="15"/>
       <c r="V19" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W19" s="15">
         <v>151551</v>
@@ -10786,34 +10794,34 @@
         <v>1</v>
       </c>
       <c r="Y19" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z19" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA19" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB19" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="AA19" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB19" s="15" t="s">
+      <c r="AC19" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="AC19" s="15" t="s">
-        <v>111</v>
       </c>
       <c r="AD19" s="15">
         <v>144183</v>
       </c>
       <c r="AE19" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF19" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AG19" s="15">
         <v>3</v>
       </c>
       <c r="AH19" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI19" s="15">
         <v>4008</v>
@@ -11822,7 +11830,7 @@
         <v>1004</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20" s="11">
         <v>1</v>
@@ -11831,7 +11839,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F20" s="11">
         <v>7</v>
@@ -11847,19 +11855,19 @@
         <v>392755</v>
       </c>
       <c r="K20" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="L20" s="22" t="s">
-        <v>83</v>
-      </c>
       <c r="M20" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="O20" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>116</v>
       </c>
       <c r="P20" s="15">
         <v>8</v>
@@ -11868,17 +11876,17 @@
         <v>9</v>
       </c>
       <c r="R20" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="S20" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="S20" s="15" t="s">
-        <v>118</v>
       </c>
       <c r="T20" s="15">
         <v>16</v>
       </c>
       <c r="U20" s="15"/>
       <c r="V20" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W20" s="15">
         <v>200133</v>
@@ -11887,34 +11895,34 @@
         <v>1</v>
       </c>
       <c r="Y20" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z20" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA20" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB20" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="Z20" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA20" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB20" s="15" t="s">
-        <v>120</v>
-      </c>
       <c r="AC20" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AD20" s="15">
         <v>144183</v>
       </c>
       <c r="AE20" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF20" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="AF20" s="15" t="s">
-        <v>122</v>
       </c>
       <c r="AG20" s="15">
         <v>1.8</v>
       </c>
       <c r="AH20" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI20" s="15">
         <v>4002</v>
@@ -12923,7 +12931,7 @@
         <v>1005</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" s="24">
         <v>1</v>
@@ -12932,7 +12940,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="26">
@@ -12946,19 +12954,19 @@
         <v>392758</v>
       </c>
       <c r="K21" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="L21" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="L21" s="29" t="s">
+      <c r="M21" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="N21" s="54" t="s">
+        <v>375</v>
+      </c>
+      <c r="O21" s="27" t="s">
         <v>126</v>
-      </c>
-      <c r="M21" s="27" t="s">
-        <v>378</v>
-      </c>
-      <c r="N21" s="54" t="s">
-        <v>379</v>
-      </c>
-      <c r="O21" s="27" t="s">
-        <v>127</v>
       </c>
       <c r="P21" s="27">
         <v>10</v>
@@ -12982,25 +12990,25 @@
         <v>1</v>
       </c>
       <c r="Y21" s="27" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="Z21" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA21" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="AA21" s="27" t="s">
-        <v>129</v>
-      </c>
       <c r="AB21" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AC21" s="27" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="AD21" s="27">
         <v>279748</v>
       </c>
       <c r="AE21" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF21" s="27">
         <v>281056</v>
@@ -13009,7 +13017,7 @@
         <v>1.8</v>
       </c>
       <c r="AH21" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI21" s="27"/>
       <c r="AJ21" s="27"/>
@@ -14016,7 +14024,7 @@
         <v>1006</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="11">
         <v>1</v>
@@ -14025,7 +14033,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F22" s="11">
         <v>1</v>
@@ -14041,19 +14049,19 @@
         <v>392754</v>
       </c>
       <c r="K22" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="M22" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="L22" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="M22" s="15" t="s">
+      <c r="N22" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="N22" s="17" t="s">
+      <c r="O22" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="O22" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="P22" s="15">
         <v>12</v>
@@ -14063,7 +14071,7 @@
       </c>
       <c r="R22" s="15"/>
       <c r="S22" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T22" s="15">
         <v>16</v>
@@ -14079,25 +14087,25 @@
         <v>1</v>
       </c>
       <c r="Y22" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z22" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA22" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA22" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="AB22" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC22" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD22" s="15">
         <v>122546</v>
       </c>
       <c r="AE22" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AF22" s="15">
         <v>135369</v>
@@ -14106,7 +14114,7 @@
         <v>2</v>
       </c>
       <c r="AH22" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI22" s="15">
         <v>4009</v>
@@ -15115,7 +15123,7 @@
         <v>1007</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="34">
         <v>1</v>
@@ -15124,7 +15132,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="35">
@@ -15138,19 +15146,19 @@
         <v>392759</v>
       </c>
       <c r="K23" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="L23" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="L23" s="38" t="s">
+      <c r="M23" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="M23" s="36" t="s">
+      <c r="N23" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="N23" s="39" t="s">
+      <c r="O23" s="40" t="s">
         <v>143</v>
-      </c>
-      <c r="O23" s="40" t="s">
-        <v>144</v>
       </c>
       <c r="P23" s="40">
         <v>14</v>
@@ -15172,19 +15180,19 @@
         <v>1</v>
       </c>
       <c r="Y23" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Z23" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AA23" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB23" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC23" s="40" t="s">
-        <v>146</v>
+        <v>392</v>
       </c>
       <c r="AD23" s="40">
         <v>279748</v>
@@ -15195,10 +15203,10 @@
       </c>
       <c r="AG23" s="40"/>
       <c r="AH23" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI23" s="39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AJ23" s="40"/>
       <c r="AK23" s="40"/>
@@ -16204,7 +16212,7 @@
         <v>1008</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C24" s="11">
         <v>2</v>
@@ -16213,7 +16221,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="15">
@@ -16227,19 +16235,19 @@
         <v>392702</v>
       </c>
       <c r="K24" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N24" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O24" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P24" s="15">
         <v>16</v>
@@ -16248,17 +16256,17 @@
         <v>17</v>
       </c>
       <c r="R24" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="T24" s="15">
         <v>16</v>
       </c>
       <c r="U24" s="15"/>
       <c r="V24" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="W24" s="15">
         <v>254300</v>
@@ -16267,34 +16275,34 @@
         <v>1</v>
       </c>
       <c r="Y24" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Z24" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA24" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA24" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="AB24" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC24" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AD24" s="13">
         <v>285370</v>
       </c>
       <c r="AE24" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF24" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AG24" s="15">
         <v>1.5</v>
       </c>
       <c r="AH24" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI24" s="15"/>
       <c r="AJ24" s="15"/>
@@ -17301,7 +17309,7 @@
         <v>1009</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C25" s="11">
         <v>2</v>
@@ -17310,7 +17318,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F25" s="11">
         <v>7</v>
@@ -17326,19 +17334,19 @@
         <v>392756</v>
       </c>
       <c r="K25" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L25" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="L25" s="15" t="s">
-        <v>83</v>
-      </c>
       <c r="M25" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N25" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O25" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P25" s="15">
         <v>18</v>
@@ -17350,7 +17358,7 @@
         <v>400</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T25" s="15">
         <v>16</v>
@@ -17366,25 +17374,25 @@
         <v>1.3</v>
       </c>
       <c r="Y25" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z25" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA25" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB25" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="Z25" s="15" t="s">
+      <c r="AC25" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="AA25" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB25" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC25" s="15" t="s">
-        <v>165</v>
       </c>
       <c r="AD25" s="15">
         <v>146119</v>
       </c>
       <c r="AE25" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF25" s="15">
         <v>279672</v>
@@ -17393,10 +17401,10 @@
         <v>1.5</v>
       </c>
       <c r="AH25" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI25" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AJ25" s="15"/>
       <c r="AK25" s="15"/>
@@ -18402,7 +18410,7 @@
         <v>1010</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C26" s="11">
         <v>2</v>
@@ -18411,7 +18419,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="15">
@@ -18427,19 +18435,19 @@
         <v>392763</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="N26" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O26" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="P26" s="15">
         <v>18</v>
@@ -18451,7 +18459,7 @@
         <v>600</v>
       </c>
       <c r="S26" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="T26" s="15">
         <v>16</v>
@@ -18467,25 +18475,25 @@
         <v>1.5</v>
       </c>
       <c r="Y26" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Z26" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA26" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA26" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="AB26" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AC26" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AD26" s="13">
         <v>144198</v>
       </c>
       <c r="AE26" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF26" s="15">
         <v>285283</v>
@@ -18494,7 +18502,7 @@
         <v>0.4</v>
       </c>
       <c r="AH26" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI26" s="15"/>
       <c r="AJ26" s="15"/>
@@ -19501,7 +19509,7 @@
         <v>1011</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C27" s="43">
         <v>2</v>
@@ -19510,7 +19518,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F27" s="43">
         <v>3</v>
@@ -19526,19 +19534,19 @@
         <v>392765</v>
       </c>
       <c r="K27" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="L27" s="45" t="s">
-        <v>83</v>
-      </c>
       <c r="M27" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="N27" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="O27" s="45" t="s">
         <v>176</v>
-      </c>
-      <c r="N27" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="O27" s="45" t="s">
-        <v>178</v>
       </c>
       <c r="P27" s="45">
         <v>18</v>
@@ -19550,7 +19558,7 @@
         <v>500</v>
       </c>
       <c r="S27" s="45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T27" s="45">
         <v>16</v>
@@ -19566,25 +19574,25 @@
         <v>0.8</v>
       </c>
       <c r="Y27" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z27" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA27" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB27" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC27" s="45" t="s">
         <v>180</v>
-      </c>
-      <c r="Z27" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA27" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB27" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC27" s="45" t="s">
-        <v>182</v>
       </c>
       <c r="AD27" s="45">
         <v>281886</v>
       </c>
       <c r="AE27" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF27" s="45">
         <v>281763</v>
@@ -19593,10 +19601,10 @@
         <v>1.5</v>
       </c>
       <c r="AH27" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI27" s="45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AJ27" s="45"/>
       <c r="AK27" s="45"/>
@@ -20602,7 +20610,7 @@
         <v>1012</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28" s="24">
         <v>2</v>
@@ -20611,7 +20619,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="26">
@@ -20625,19 +20633,19 @@
         <v>392764</v>
       </c>
       <c r="K28" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="L28" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="L28" s="27" t="s">
-        <v>126</v>
-      </c>
       <c r="M28" s="31" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="N28" s="31" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="O28" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="P28" s="26">
         <v>20</v>
@@ -20663,25 +20671,25 @@
         <v>1</v>
       </c>
       <c r="Y28" s="27" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="Z28" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA28" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="AA28" s="27" t="s">
-        <v>129</v>
-      </c>
       <c r="AB28" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AC28" s="27" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="AD28" s="27">
         <v>144183</v>
       </c>
       <c r="AE28" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF28" s="27">
         <v>279686</v>
@@ -20690,7 +20698,7 @@
         <v>2.5</v>
       </c>
       <c r="AH28" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI28" s="27"/>
       <c r="AJ28" s="27"/>
@@ -21697,7 +21705,7 @@
         <v>1013</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C29" s="34">
         <v>2</v>
@@ -21706,7 +21714,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F29" s="40"/>
       <c r="G29" s="40">
@@ -21720,19 +21728,19 @@
         <v>392695</v>
       </c>
       <c r="K29" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="L29" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="M29" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="N29" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="L29" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="M29" s="39" t="s">
+      <c r="O29" s="40" t="s">
         <v>190</v>
-      </c>
-      <c r="N29" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="O29" s="40" t="s">
-        <v>192</v>
       </c>
       <c r="P29" s="40"/>
       <c r="Q29" s="40"/>
@@ -21748,19 +21756,19 @@
         <v>1</v>
       </c>
       <c r="Y29" s="40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Z29" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AA29" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB29" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC29" s="40" t="s">
-        <v>195</v>
+        <v>393</v>
       </c>
       <c r="AD29" s="40">
         <v>285237</v>
@@ -21771,10 +21779,10 @@
       </c>
       <c r="AG29" s="40"/>
       <c r="AH29" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI29" s="39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AJ29" s="40"/>
       <c r="AK29" s="40"/>
@@ -22780,7 +22788,7 @@
         <v>1014</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C30" s="34">
         <v>2</v>
@@ -22789,7 +22797,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="40" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F30" s="40"/>
       <c r="G30" s="40">
@@ -22803,19 +22811,19 @@
         <v>392753</v>
       </c>
       <c r="K30" s="51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L30" s="40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M30" s="39" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N30" s="39" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="O30" s="40" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="P30" s="40"/>
       <c r="Q30" s="40"/>
@@ -22831,19 +22839,19 @@
         <v>1</v>
       </c>
       <c r="Y30" s="40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="Z30" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AA30" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB30" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC30" s="40" t="s">
-        <v>203</v>
+        <v>394</v>
       </c>
       <c r="AD30" s="40">
         <v>285459</v>
@@ -22854,10 +22862,10 @@
       </c>
       <c r="AG30" s="40"/>
       <c r="AH30" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI30" s="39" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="AJ30" s="40"/>
       <c r="AK30" s="40"/>
@@ -23863,7 +23871,7 @@
         <v>1015</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C31" s="45">
         <v>3</v>
@@ -23872,7 +23880,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="45" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F31" s="45">
         <v>9</v>
@@ -23888,19 +23896,19 @@
         <v>392699</v>
       </c>
       <c r="K31" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="L31" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="45" t="s">
-        <v>83</v>
-      </c>
       <c r="M31" s="45" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="N31" s="45" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="O31" s="45" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="P31" s="45">
         <v>22</v>
@@ -23912,14 +23920,14 @@
         <v>300</v>
       </c>
       <c r="S31" s="45" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="T31" s="45">
         <v>16</v>
       </c>
       <c r="U31" s="45"/>
       <c r="V31" s="45" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="W31" s="45">
         <v>151576</v>
@@ -23928,37 +23936,37 @@
         <v>1</v>
       </c>
       <c r="Y31" s="45" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="Z31" s="45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AA31" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB31" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC31" s="45" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="AD31" s="45">
         <v>281788</v>
       </c>
       <c r="AE31" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF31" s="45" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="AG31" s="45">
         <v>0.4</v>
       </c>
       <c r="AH31" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI31" s="45" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="AJ31" s="45"/>
       <c r="AK31" s="45"/>
@@ -24964,7 +24972,7 @@
         <v>1016</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C32" s="45">
         <v>3</v>
@@ -24973,7 +24981,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="45" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F32" s="45">
         <v>7</v>
@@ -24989,19 +24997,19 @@
         <v>392704</v>
       </c>
       <c r="K32" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="L32" s="45" t="s">
-        <v>83</v>
-      </c>
       <c r="M32" s="45" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="N32" s="45" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O32" s="45" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="P32" s="45">
         <v>22</v>
@@ -25013,14 +25021,14 @@
         <v>200</v>
       </c>
       <c r="S32" s="45" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="T32" s="45">
         <v>16</v>
       </c>
       <c r="U32" s="45"/>
       <c r="V32" s="45" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="W32" s="45">
         <v>168944</v>
@@ -25029,37 +25037,37 @@
         <v>0.3</v>
       </c>
       <c r="Y32" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z32" s="45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AA32" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB32" s="45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AC32" s="45" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AD32" s="45">
         <v>285400</v>
       </c>
       <c r="AE32" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF32" s="45" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="AG32" s="45">
         <v>0.4</v>
       </c>
       <c r="AH32" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI32" s="45" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="AJ32" s="45"/>
       <c r="AK32" s="45"/>
@@ -26065,7 +26073,7 @@
         <v>1017</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C33" s="45">
         <v>3</v>
@@ -26074,7 +26082,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="45" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F33" s="45">
         <v>2</v>
@@ -26092,19 +26100,19 @@
         <v>392693</v>
       </c>
       <c r="K33" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="L33" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="L33" s="45" t="s">
-        <v>83</v>
-      </c>
       <c r="M33" s="45" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="N33" s="45" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="O33" s="45" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="P33" s="45">
         <v>22</v>
@@ -26116,7 +26124,7 @@
         <v>100</v>
       </c>
       <c r="S33" s="45" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="T33" s="45">
         <v>16</v>
@@ -26132,25 +26140,25 @@
         <v>1.2</v>
       </c>
       <c r="Y33" s="45" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="Z33" s="45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AA33" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB33" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC33" s="45" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AD33" s="45">
         <v>281710</v>
       </c>
       <c r="AE33" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF33" s="45">
         <v>80483</v>
@@ -26159,7 +26167,7 @@
         <v>0.4</v>
       </c>
       <c r="AH33" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI33" s="45"/>
       <c r="AJ33" s="45"/>
@@ -27166,7 +27174,7 @@
         <v>1018</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C34" s="45">
         <v>3</v>
@@ -27175,7 +27183,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="45" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F34" s="45">
         <v>4</v>
@@ -27191,19 +27199,19 @@
         <v>392692</v>
       </c>
       <c r="K34" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L34" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M34" s="45" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="N34" s="45" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="O34" s="45" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="P34" s="45">
         <v>22</v>
@@ -27212,17 +27220,17 @@
         <v>23</v>
       </c>
       <c r="R34" s="45" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="S34" s="45" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="T34" s="45">
         <v>16</v>
       </c>
       <c r="U34" s="45"/>
       <c r="V34" s="45" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="W34" s="45">
         <v>288335</v>
@@ -27231,37 +27239,37 @@
         <v>0.5</v>
       </c>
       <c r="Y34" s="45" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="Z34" s="45" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="AA34" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB34" s="45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AC34" s="45" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="AD34" s="45">
         <v>299561</v>
       </c>
       <c r="AE34" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF34" s="45" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="AG34" s="45">
         <v>2</v>
       </c>
       <c r="AH34" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI34" s="45" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="AJ34" s="45"/>
       <c r="AK34" s="45"/>
@@ -28267,7 +28275,7 @@
         <v>1019</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C35" s="45">
         <v>3</v>
@@ -28276,7 +28284,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="45" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F35" s="45"/>
       <c r="G35" s="45">
@@ -28290,19 +28298,19 @@
         <v>392697</v>
       </c>
       <c r="K35" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L35" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M35" s="45" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="N35" s="45" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="O35" s="45" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="P35" s="45">
         <v>22</v>
@@ -28311,17 +28319,17 @@
         <v>23</v>
       </c>
       <c r="R35" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S35" s="45" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="T35" s="45">
         <v>16</v>
       </c>
       <c r="U35" s="45"/>
       <c r="V35" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W35" s="45">
         <v>130642</v>
@@ -28330,34 +28338,34 @@
         <v>0.8</v>
       </c>
       <c r="Y35" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z35" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA35" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB35" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC35" s="45" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="AD35" s="45">
         <v>285356</v>
       </c>
       <c r="AE35" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF35" s="45" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="AG35" s="45">
         <v>2</v>
       </c>
       <c r="AH35" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI35" s="45"/>
       <c r="AJ35" s="45"/>
@@ -29364,7 +29372,7 @@
         <v>1020</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C36" s="45">
         <v>3</v>
@@ -29373,7 +29381,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="45" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F36" s="45">
         <v>2</v>
@@ -29391,19 +29399,19 @@
         <v>392694</v>
       </c>
       <c r="K36" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L36" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M36" s="45" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="N36" s="45" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="O36" s="45" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="P36" s="45">
         <v>22</v>
@@ -29412,17 +29420,17 @@
         <v>23</v>
       </c>
       <c r="R36" s="45" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="S36" s="45" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="T36" s="45">
         <v>16</v>
       </c>
       <c r="U36" s="45"/>
       <c r="V36" s="45" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="W36" s="45">
         <v>254276</v>
@@ -29431,34 +29439,34 @@
         <v>1</v>
       </c>
       <c r="Y36" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z36" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA36" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="AA36" s="45" t="s">
-        <v>89</v>
-      </c>
       <c r="AB36" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC36" s="45" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="AD36" s="45">
         <v>20301</v>
       </c>
       <c r="AE36" s="45" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AF36" s="45" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AG36" s="45">
         <v>3</v>
       </c>
       <c r="AH36" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI36" s="45"/>
       <c r="AJ36" s="45"/>
@@ -30465,7 +30473,7 @@
         <v>1021</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C37" s="45">
         <v>4</v>
@@ -30474,7 +30482,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="45" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F37" s="45">
         <v>8</v>
@@ -30492,19 +30500,19 @@
         <v>392706</v>
       </c>
       <c r="K37" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="L37" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="45" t="s">
-        <v>83</v>
-      </c>
       <c r="M37" s="45" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="N37" s="45" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="O37" s="45" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="P37" s="45">
         <v>24</v>
@@ -30516,7 +30524,7 @@
         <v>100</v>
       </c>
       <c r="S37" s="45" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="T37" s="45">
         <v>16</v>
@@ -30532,25 +30540,25 @@
         <v>1</v>
       </c>
       <c r="Y37" s="45" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="Z37" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA37" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="AA37" s="45" t="s">
-        <v>89</v>
-      </c>
       <c r="AB37" s="45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC37" s="45" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="AD37" s="45">
         <v>281710</v>
       </c>
       <c r="AE37" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF37" s="45">
         <v>80483</v>
@@ -30559,10 +30567,10 @@
         <v>0.4</v>
       </c>
       <c r="AH37" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI37" s="52" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AJ37" s="45"/>
       <c r="AK37" s="45"/>
@@ -31568,7 +31576,7 @@
         <v>1022</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C38" s="45">
         <v>4</v>
@@ -31577,7 +31585,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="45" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F38" s="45">
         <v>4</v>
@@ -31593,19 +31601,19 @@
         <v>392700</v>
       </c>
       <c r="K38" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="L38" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="L38" s="45" t="s">
-        <v>83</v>
-      </c>
       <c r="M38" s="45" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="N38" s="45" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="O38" s="45" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="P38" s="45">
         <v>24</v>
@@ -31617,14 +31625,14 @@
         <v>200</v>
       </c>
       <c r="S38" s="45" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="T38" s="45">
         <v>16</v>
       </c>
       <c r="U38" s="45"/>
       <c r="V38" s="45" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="W38" s="45">
         <v>271321</v>
@@ -31633,37 +31641,37 @@
         <v>0.8</v>
       </c>
       <c r="Y38" s="45" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Z38" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA38" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="AA38" s="45" t="s">
-        <v>89</v>
-      </c>
       <c r="AB38" s="45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AC38" s="45" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="AD38" s="45">
         <v>281871</v>
       </c>
       <c r="AE38" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF38" s="45" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="AG38" s="45">
         <v>1</v>
       </c>
       <c r="AH38" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI38" s="45" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="AJ38" s="45"/>
       <c r="AK38" s="45"/>
@@ -32669,7 +32677,7 @@
         <v>1023</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C39" s="45">
         <v>4</v>
@@ -32678,7 +32686,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="45" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F39" s="45">
         <v>10</v>
@@ -32696,19 +32704,19 @@
         <v>392696</v>
       </c>
       <c r="K39" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L39" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M39" s="45" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="N39" s="45" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="O39" s="45" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="P39" s="45">
         <v>24</v>
@@ -32720,7 +32728,7 @@
         <v>200</v>
       </c>
       <c r="S39" s="45" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="T39" s="45">
         <v>16</v>
@@ -32736,25 +32744,25 @@
         <v>1.5</v>
       </c>
       <c r="Y39" s="45" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="Z39" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA39" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="AA39" s="45" t="s">
-        <v>89</v>
-      </c>
       <c r="AB39" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC39" s="45" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="AD39" s="45">
         <v>300932</v>
       </c>
       <c r="AE39" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF39" s="45">
         <v>285208</v>
@@ -32763,10 +32771,10 @@
         <v>2</v>
       </c>
       <c r="AH39" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI39" s="45" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="AJ39" s="45"/>
       <c r="AK39" s="45"/>
@@ -33772,7 +33780,7 @@
         <v>1024</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C40" s="45">
         <v>4</v>
@@ -33781,7 +33789,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="45" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F40" s="45"/>
       <c r="G40" s="45">
@@ -33795,19 +33803,19 @@
         <v>392703</v>
       </c>
       <c r="K40" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L40" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M40" s="45" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="N40" s="45" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="O40" s="45" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="P40" s="45">
         <v>24</v>
@@ -33819,7 +33827,7 @@
         <v>300</v>
       </c>
       <c r="S40" s="45" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="T40" s="45">
         <v>16</v>
@@ -33835,25 +33843,25 @@
         <v>1.5</v>
       </c>
       <c r="Y40" s="45" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="Z40" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA40" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="AA40" s="45" t="s">
-        <v>89</v>
-      </c>
       <c r="AB40" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC40" s="45" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="AD40" s="45">
         <v>117391</v>
       </c>
       <c r="AE40" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF40" s="45">
         <v>269275</v>
@@ -33862,7 +33870,7 @@
         <v>2</v>
       </c>
       <c r="AH40" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI40" s="45"/>
       <c r="AJ40" s="45"/>
@@ -34869,7 +34877,7 @@
         <v>1025</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C41" s="45">
         <v>4</v>
@@ -34878,7 +34886,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="45" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F41" s="45">
         <v>6</v>
@@ -34894,19 +34902,19 @@
         <v>392698</v>
       </c>
       <c r="K41" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L41" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M41" s="45" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="N41" s="45" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="O41" s="45" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="P41" s="45">
         <v>24</v>
@@ -34918,7 +34926,7 @@
         <v>100</v>
       </c>
       <c r="S41" s="45" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="T41" s="45">
         <v>16</v>
@@ -34934,25 +34942,25 @@
         <v>1.5</v>
       </c>
       <c r="Y41" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z41" s="45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA41" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB41" s="45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AC41" s="45" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="AD41" s="45">
         <v>285445</v>
       </c>
       <c r="AE41" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF41" s="53">
         <v>269223</v>
@@ -34961,10 +34969,10 @@
         <v>0.5</v>
       </c>
       <c r="AH41" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI41" s="45" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="AJ41" s="45"/>
       <c r="AK41" s="45"/>
@@ -35970,7 +35978,7 @@
         <v>1026</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C42" s="40">
         <v>4</v>
@@ -35979,7 +35987,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="40" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F42" s="40"/>
       <c r="G42" s="40">
@@ -35993,19 +36001,19 @@
         <v>392705</v>
       </c>
       <c r="K42" s="51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L42" s="40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M42" s="39" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="N42" s="39" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="O42" s="40" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P42" s="40">
         <v>24</v>
@@ -36025,19 +36033,19 @@
         <v>1</v>
       </c>
       <c r="Y42" s="40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Z42" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AA42" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB42" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC42" s="40" t="s">
-        <v>195</v>
+        <v>395</v>
       </c>
       <c r="AD42" s="40">
         <v>94268</v>
@@ -36048,10 +36056,10 @@
       </c>
       <c r="AG42" s="40"/>
       <c r="AH42" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI42" s="39" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ42" s="40"/>
       <c r="AK42" s="40"/>
@@ -37057,7 +37065,7 @@
         <v>1027</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C43" s="15">
         <v>5</v>
@@ -37066,7 +37074,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F43" s="15"/>
       <c r="G43" s="15">
@@ -37080,19 +37088,19 @@
         <v>392701</v>
       </c>
       <c r="K43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L43" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="L43" s="15" t="s">
-        <v>83</v>
-      </c>
       <c r="M43" s="15" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="N43" s="15" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="O43" s="15" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P43" s="15">
         <v>26</v>
@@ -37104,7 +37112,7 @@
         <v>100</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="T43" s="15">
         <v>16</v>
@@ -37118,25 +37126,25 @@
         <v>0.6</v>
       </c>
       <c r="Y43" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z43" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Z43" s="15" t="s">
+      <c r="AA43" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA43" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="AB43" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC43" s="15" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="AD43" s="15">
         <v>279765</v>
       </c>
       <c r="AE43" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF43" s="15">
         <v>303167</v>
@@ -37145,10 +37153,10 @@
         <v>0.5</v>
       </c>
       <c r="AH43" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI43" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AJ43" s="15"/>
       <c r="AK43" s="15"/>
@@ -38154,7 +38162,7 @@
         <v>1028</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C44" s="15">
         <v>5</v>
@@ -38163,7 +38171,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F44" s="15"/>
       <c r="G44" s="15">
@@ -38177,19 +38185,19 @@
         <v>392708</v>
       </c>
       <c r="K44" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L44" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M44" s="15" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="N44" s="15" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="O44" s="15" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="P44" s="15">
         <v>44</v>
@@ -38201,7 +38209,7 @@
         <v>100</v>
       </c>
       <c r="S44" s="15" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="T44" s="15">
         <v>16</v>
@@ -38217,25 +38225,25 @@
         <v>1.4</v>
       </c>
       <c r="Y44" s="15" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="Z44" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA44" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA44" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="AB44" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC44" s="15" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="AD44" s="15">
         <v>85944</v>
       </c>
       <c r="AE44" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF44" s="23">
         <v>29747</v>
@@ -38244,7 +38252,7 @@
         <v>0.5</v>
       </c>
       <c r="AH44" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI44" s="15"/>
       <c r="AJ44" s="15"/>
@@ -39251,7 +39259,7 @@
         <v>1029</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C45" s="15">
         <v>5</v>
@@ -39260,7 +39268,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F45" s="15">
         <v>3</v>
@@ -39276,19 +39284,19 @@
         <v>392716</v>
       </c>
       <c r="K45" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L45" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M45" s="15" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="N45" s="15" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="O45" s="15" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="P45" s="15">
         <v>46</v>
@@ -39300,7 +39308,7 @@
         <v>400</v>
       </c>
       <c r="S45" s="15" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="T45" s="15">
         <v>16</v>
@@ -39316,25 +39324,25 @@
         <v>1</v>
       </c>
       <c r="Y45" s="15" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="Z45" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AA45" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB45" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC45" s="15" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="AD45" s="15">
         <v>326802</v>
       </c>
       <c r="AE45" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF45" s="15">
         <v>279685</v>
@@ -39343,10 +39351,10 @@
         <v>0.8</v>
       </c>
       <c r="AH45" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI45" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AJ45" s="15"/>
       <c r="AK45" s="15"/>
@@ -40352,7 +40360,7 @@
         <v>1030</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C46" s="15">
         <v>5</v>
@@ -40361,7 +40369,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F46" s="15">
         <v>6</v>
@@ -40377,19 +40385,19 @@
         <v>392717</v>
       </c>
       <c r="K46" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L46" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M46" s="15" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="O46" s="15" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="P46" s="15">
         <v>48</v>
@@ -40399,7 +40407,7 @@
       </c>
       <c r="R46" s="15"/>
       <c r="S46" s="15" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="T46" s="15">
         <v>16</v>
@@ -40415,25 +40423,25 @@
         <v>1</v>
       </c>
       <c r="Y46" s="15" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="Z46" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA46" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB46" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC46" s="15" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="AD46" s="15">
         <v>281871</v>
       </c>
       <c r="AE46" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF46" s="15">
         <v>268572</v>
@@ -40442,10 +40450,10 @@
         <v>0.7</v>
       </c>
       <c r="AH46" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI46" s="45" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="AJ46" s="15"/>
       <c r="AK46" s="15"/>
@@ -41451,7 +41459,7 @@
         <v>1031</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C47" s="27">
         <v>5</v>
@@ -41460,7 +41468,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F47" s="27"/>
       <c r="G47" s="27">
@@ -41474,19 +41482,19 @@
         <v>392712</v>
       </c>
       <c r="K47" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="L47" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="L47" s="27" t="s">
-        <v>126</v>
-      </c>
       <c r="M47" s="27" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="N47" s="27" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="O47" s="27" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="P47" s="27">
         <v>40</v>
@@ -41498,7 +41506,7 @@
         <v>1000</v>
       </c>
       <c r="S47" s="27" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="T47" s="27">
         <v>16</v>
@@ -41512,25 +41520,25 @@
         <v>0.6</v>
       </c>
       <c r="Y47" s="27" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="Z47" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA47" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="AA47" s="27" t="s">
-        <v>89</v>
-      </c>
       <c r="AB47" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC47" s="27" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="AD47" s="27">
         <v>285673</v>
       </c>
       <c r="AE47" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF47" s="27">
         <v>268686</v>
@@ -41539,7 +41547,7 @@
         <v>1</v>
       </c>
       <c r="AH47" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI47" s="27"/>
       <c r="AJ47" s="27"/>
@@ -42546,7 +42554,7 @@
         <v>1032</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C48" s="24">
         <v>5</v>
@@ -42555,7 +42563,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F48" s="27"/>
       <c r="G48" s="26">
@@ -42569,19 +42577,19 @@
         <v>392711</v>
       </c>
       <c r="K48" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="L48" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="L48" s="27" t="s">
-        <v>126</v>
-      </c>
       <c r="M48" s="27" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="N48" s="27" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="O48" s="27" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="P48" s="26">
         <v>42</v>
@@ -42605,25 +42613,25 @@
         <v>1</v>
       </c>
       <c r="Y48" s="27" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="Z48" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA48" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="AA48" s="27" t="s">
-        <v>89</v>
-      </c>
       <c r="AB48" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC48" s="27" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AD48" s="27">
         <v>144183</v>
       </c>
       <c r="AE48" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF48" s="27">
         <v>20270</v>
@@ -42632,7 +42640,7 @@
         <v>1.8</v>
       </c>
       <c r="AH48" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI48" s="27"/>
       <c r="AJ48" s="27"/>
@@ -43639,7 +43647,7 @@
         <v>1033</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C49" s="15">
         <v>6</v>
@@ -43648,7 +43656,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F49" s="15">
         <v>5</v>
@@ -43664,19 +43672,19 @@
         <v>392710</v>
       </c>
       <c r="K49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L49" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="L49" s="15" t="s">
-        <v>83</v>
-      </c>
       <c r="M49" s="15" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="N49" s="15" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="O49" s="15" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="P49" s="15">
         <v>28</v>
@@ -43688,7 +43696,7 @@
         <v>350</v>
       </c>
       <c r="S49" s="15" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="T49" s="15">
         <v>16</v>
@@ -43704,25 +43712,25 @@
         <v>1.5</v>
       </c>
       <c r="Y49" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Z49" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AA49" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB49" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC49" s="15" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="AD49" s="15">
         <v>303259</v>
       </c>
       <c r="AE49" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF49" s="15">
         <v>303247</v>
@@ -43731,10 +43739,10 @@
         <v>1.5</v>
       </c>
       <c r="AH49" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI49" s="15" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="AJ49" s="15"/>
       <c r="AK49" s="15"/>
@@ -44740,7 +44748,7 @@
         <v>1034</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C50" s="15">
         <v>6</v>
@@ -44749,7 +44757,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F50" s="15"/>
       <c r="G50" s="15">
@@ -44763,19 +44771,19 @@
         <v>392713</v>
       </c>
       <c r="K50" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L50" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M50" s="15" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="N50" s="15" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="O50" s="15" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="P50" s="15">
         <v>30</v>
@@ -44787,7 +44795,7 @@
         <v>650</v>
       </c>
       <c r="S50" s="15" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="T50" s="15">
         <v>16</v>
@@ -44803,25 +44811,25 @@
         <v>1</v>
       </c>
       <c r="Y50" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Z50" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA50" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB50" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC50" s="15" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="AD50" s="15">
         <v>305224</v>
       </c>
       <c r="AE50" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF50" s="15">
         <v>284893</v>
@@ -44830,7 +44838,7 @@
         <v>1.3</v>
       </c>
       <c r="AH50" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI50" s="15"/>
       <c r="AJ50" s="15"/>
@@ -45837,7 +45845,7 @@
         <v>1035</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C51" s="15">
         <v>6</v>
@@ -45846,7 +45854,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F51" s="15">
         <v>3</v>
@@ -45862,19 +45870,19 @@
         <v>392707</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L51" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M51" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="N51" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="O51" s="15" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="P51" s="15">
         <v>32</v>
@@ -45886,7 +45894,7 @@
         <v>1000</v>
       </c>
       <c r="S51" s="15" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="T51" s="15">
         <v>16</v>
@@ -45902,25 +45910,25 @@
         <v>1</v>
       </c>
       <c r="Y51" s="15" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="Z51" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA51" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA51" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="AB51" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC51" s="15" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="AD51" s="15">
         <v>269209</v>
       </c>
       <c r="AE51" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF51" s="15">
         <v>268704</v>
@@ -45929,10 +45937,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AH51" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI51" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AJ51" s="15"/>
       <c r="AK51" s="15"/>
@@ -46938,7 +46946,7 @@
         <v>1036</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C52" s="15">
         <v>6</v>
@@ -46947,7 +46955,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F52" s="15">
         <v>6</v>
@@ -46959,25 +46967,25 @@
         <v>1</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="J52" s="15">
         <v>392709</v>
       </c>
       <c r="K52" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L52" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="L52" s="15" t="s">
-        <v>83</v>
-      </c>
       <c r="M52" s="15" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="N52" s="15" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="O52" s="15" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="P52" s="15">
         <v>38</v>
@@ -46989,7 +46997,7 @@
         <v>500</v>
       </c>
       <c r="S52" s="15" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="T52" s="15">
         <v>16</v>
@@ -47005,25 +47013,25 @@
         <v>1</v>
       </c>
       <c r="Y52" s="15" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="Z52" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA52" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB52" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC52" s="15" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="AD52" s="15">
         <v>144183</v>
       </c>
       <c r="AE52" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF52" s="15">
         <v>279726</v>
@@ -47032,10 +47040,10 @@
         <v>1</v>
       </c>
       <c r="AH52" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI52" s="15" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="AJ52" s="15"/>
       <c r="AK52" s="15"/>
@@ -48041,7 +48049,7 @@
         <v>1037</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C53" s="15">
         <v>6</v>
@@ -48050,7 +48058,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F53" s="15"/>
       <c r="G53" s="15">
@@ -48060,25 +48068,25 @@
         <v>1</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="J53" s="15">
         <v>392714</v>
       </c>
       <c r="K53" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L53" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M53" s="15" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="N53" s="15" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="O53" s="15" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="P53" s="15">
         <v>34</v>
@@ -48088,7 +48096,7 @@
       </c>
       <c r="R53" s="15"/>
       <c r="S53" s="15" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="T53" s="15">
         <v>16</v>
@@ -48102,25 +48110,25 @@
         <v>2</v>
       </c>
       <c r="Y53" s="15" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="Z53" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA53" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB53" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC53" s="15" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="AD53" s="15">
         <v>281795</v>
       </c>
       <c r="AE53" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF53" s="15">
         <v>81687</v>
@@ -48129,7 +48137,7 @@
         <v>1</v>
       </c>
       <c r="AH53" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI53" s="17"/>
       <c r="AJ53" s="15"/>
@@ -49136,7 +49144,7 @@
         <v>1038</v>
       </c>
       <c r="B54" s="33" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C54" s="40">
         <v>6</v>
@@ -49145,7 +49153,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="40" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F54" s="40"/>
       <c r="G54" s="35">
@@ -49155,25 +49163,25 @@
         <v>2</v>
       </c>
       <c r="I54" s="40" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="J54" s="40">
         <v>392715</v>
       </c>
       <c r="K54" s="51" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="L54" s="40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M54" s="39" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="N54" s="39" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="O54" s="40" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="P54" s="40">
         <v>36</v>
@@ -49195,16 +49203,16 @@
         <v>1</v>
       </c>
       <c r="Y54" s="40" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="Z54" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA54" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="AA54" s="40" t="s">
-        <v>129</v>
-      </c>
       <c r="AB54" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AC54" s="40" t="s">
         <v>396</v>
@@ -49213,7 +49221,7 @@
         <v>144183</v>
       </c>
       <c r="AE54" s="40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF54" s="40">
         <v>20270</v>
@@ -49222,10 +49230,10 @@
         <v>1</v>
       </c>
       <c r="AH54" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI54" s="39" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AJ54" s="40"/>
       <c r="AK54" s="40"/>

</xml_diff>

<commit_message>
feat: update StageConfig and Tower
更新关卡配置和塔配置
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6209477C-7355-4C7B-B3F8-B19CBFA95E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53BB673-D432-491A-815C-A849BFFD0ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="421">
   <si>
     <t>int</t>
   </si>
@@ -317,9 +317,6 @@
     <t>0|0|0</t>
   </si>
   <si>
-    <t>58|108|128</t>
-  </si>
-  <si>
     <t>FF9C6CFF|65AAFFFF|FF45FEFF</t>
   </si>
   <si>
@@ -378,9 +375,6 @@
   </si>
   <si>
     <t>2|2|2.5</t>
-  </si>
-  <si>
-    <t>280|350|350</t>
   </si>
   <si>
     <t>20275|281753</t>
@@ -784,9 +778,6 @@
     <t>0.8|0.8|0.7</t>
   </si>
   <si>
-    <t>58|88|128</t>
-  </si>
-  <si>
     <t>268572|284907</t>
   </si>
   <si>
@@ -1111,9 +1102,6 @@
     <t>C2B668554B1057C2E3EA788780B7592D</t>
   </si>
   <si>
-    <t>0.4|0.4|0.4</t>
-  </si>
-  <si>
     <t>30|60|90</t>
   </si>
   <si>
@@ -1432,6 +1420,30 @@
   </si>
   <si>
     <t>72|98|124</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6|0.6|0.6</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>50|88|128</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>60|100|140</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>280|350|420</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>80|140|240</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.45|0.45|0.45</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1919,10 +1931,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="AC33" sqref="AC33"/>
+      <selection pane="topRight" activeCell="AI64" sqref="AH64:AI87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -8500,7 +8512,7 @@
         <v>84</v>
       </c>
       <c r="N17" s="14" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="O17" s="13" t="s">
         <v>85</v>
@@ -8529,7 +8541,7 @@
         <v>0.3</v>
       </c>
       <c r="Y17" s="13" t="s">
-        <v>87</v>
+        <v>415</v>
       </c>
       <c r="Z17" s="13" t="s">
         <v>88</v>
@@ -8541,13 +8553,13 @@
         <v>88</v>
       </c>
       <c r="AC17" s="13" t="s">
-        <v>90</v>
+        <v>416</v>
       </c>
       <c r="AD17" s="13">
         <v>144183</v>
       </c>
       <c r="AE17" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF17" s="13">
         <v>279719</v>
@@ -8556,7 +8568,7 @@
         <v>0.5</v>
       </c>
       <c r="AH17" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AI17" s="13"/>
       <c r="AJ17" s="13"/>
@@ -9553,7 +9565,7 @@
         <v>1002</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
@@ -9562,7 +9574,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="11">
@@ -9582,13 +9594,13 @@
         <v>83</v>
       </c>
       <c r="M18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="O18" s="13" t="s">
         <v>95</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="O18" s="13" t="s">
-        <v>96</v>
       </c>
       <c r="P18" s="13">
         <v>4</v>
@@ -9600,7 +9612,7 @@
         <v>300</v>
       </c>
       <c r="S18" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T18" s="13">
         <v>16</v>
@@ -9616,7 +9628,7 @@
         <v>1.5</v>
       </c>
       <c r="Y18" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Z18" s="13" t="s">
         <v>88</v>
@@ -9625,16 +9637,16 @@
         <v>89</v>
       </c>
       <c r="AB18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC18" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="AC18" s="13" t="s">
-        <v>100</v>
       </c>
       <c r="AD18" s="13">
         <v>284848</v>
       </c>
       <c r="AE18" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF18" s="13">
         <v>121794</v>
@@ -9643,7 +9655,7 @@
         <v>2.5</v>
       </c>
       <c r="AH18" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI18" s="13"/>
       <c r="AJ18" s="13"/>
@@ -10640,7 +10652,7 @@
         <v>1003</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
@@ -10649,7 +10661,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="9">
         <v>8</v>
@@ -10673,32 +10685,32 @@
         <v>83</v>
       </c>
       <c r="M19" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="O19" s="13" t="s">
         <v>104</v>
-      </c>
-      <c r="N19" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="O19" s="13" t="s">
-        <v>105</v>
       </c>
       <c r="P19" s="13">
         <v>6</v>
       </c>
       <c r="Q19" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="R19" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="R19" s="13" t="s">
+      <c r="S19" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="S19" s="13" t="s">
-        <v>108</v>
       </c>
       <c r="T19" s="13">
         <v>16</v>
       </c>
       <c r="U19" s="13"/>
       <c r="V19" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W19" s="13">
         <v>151551</v>
@@ -10707,34 +10719,34 @@
         <v>1</v>
       </c>
       <c r="Y19" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z19" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA19" s="13" t="s">
         <v>89</v>
       </c>
       <c r="AB19" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AC19" s="13" t="s">
-        <v>111</v>
+        <v>418</v>
       </c>
       <c r="AD19" s="13">
         <v>144183</v>
       </c>
       <c r="AE19" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF19" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AG19" s="13">
         <v>3</v>
       </c>
       <c r="AH19" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI19" s="13">
         <v>4008</v>
@@ -11733,7 +11745,7 @@
         <v>1004</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C20" s="9">
         <v>1</v>
@@ -11742,7 +11754,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F20" s="9">
         <v>7</v>
@@ -11764,13 +11776,13 @@
         <v>83</v>
       </c>
       <c r="M20" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="O20" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P20" s="13">
         <v>8</v>
@@ -11779,17 +11791,17 @@
         <v>9</v>
       </c>
       <c r="R20" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S20" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T20" s="13">
         <v>16</v>
       </c>
       <c r="U20" s="13"/>
       <c r="V20" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="W20" s="13">
         <v>200133</v>
@@ -11798,7 +11810,7 @@
         <v>1</v>
       </c>
       <c r="Y20" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z20" s="13" t="s">
         <v>88</v>
@@ -11807,25 +11819,25 @@
         <v>89</v>
       </c>
       <c r="AB20" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AC20" s="13" t="s">
-        <v>115</v>
+        <v>419</v>
       </c>
       <c r="AD20" s="13">
         <v>144183</v>
       </c>
       <c r="AE20" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AF20" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AG20" s="13">
         <v>1.8</v>
       </c>
       <c r="AH20" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI20" s="13">
         <v>4002</v>
@@ -12824,7 +12836,7 @@
         <v>1005</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C21" s="22">
         <v>1</v>
@@ -12833,7 +12845,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="24">
@@ -12847,19 +12859,19 @@
         <v>392758</v>
       </c>
       <c r="K21" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="M21" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="L21" s="27" t="s">
+      <c r="N21" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="O21" s="25" t="s">
         <v>126</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="N21" s="28" t="s">
-        <v>382</v>
-      </c>
-      <c r="O21" s="25" t="s">
-        <v>128</v>
       </c>
       <c r="P21" s="25">
         <v>10</v>
@@ -12883,25 +12895,25 @@
         <v>1</v>
       </c>
       <c r="Y21" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z21" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA21" s="25" t="s">
         <v>129</v>
-      </c>
-      <c r="Z21" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="AA21" s="25" t="s">
-        <v>131</v>
       </c>
       <c r="AB21" s="25" t="s">
         <v>89</v>
       </c>
       <c r="AC21" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AD21" s="25">
         <v>279748</v>
       </c>
       <c r="AE21" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF21" s="25">
         <v>281056</v>
@@ -12910,7 +12922,7 @@
         <v>1.8</v>
       </c>
       <c r="AH21" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI21" s="25"/>
       <c r="AJ21" s="25"/>
@@ -13907,7 +13919,7 @@
         <v>1006</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
@@ -13916,7 +13928,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F22" s="9">
         <v>1</v>
@@ -13932,19 +13944,19 @@
         <v>392754</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L22" s="20" t="s">
         <v>83</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="O22" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P22" s="13">
         <v>12</v>
@@ -13954,7 +13966,7 @@
       </c>
       <c r="R22" s="13"/>
       <c r="S22" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="T22" s="13">
         <v>16</v>
@@ -13970,7 +13982,7 @@
         <v>1</v>
       </c>
       <c r="Y22" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="Z22" s="13" t="s">
         <v>88</v>
@@ -13979,16 +13991,16 @@
         <v>89</v>
       </c>
       <c r="AB22" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC22" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AD22" s="13">
         <v>122546</v>
       </c>
       <c r="AE22" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AF22" s="13">
         <v>135369</v>
@@ -13997,7 +14009,7 @@
         <v>2</v>
       </c>
       <c r="AH22" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI22" s="13">
         <v>4009</v>
@@ -14996,7 +15008,7 @@
         <v>1007</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C23" s="33">
         <v>1</v>
@@ -15005,7 +15017,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="34">
@@ -15019,19 +15031,19 @@
         <v>392759</v>
       </c>
       <c r="K23" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="L23" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="M23" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="N23" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="O23" s="39" t="s">
         <v>143</v>
-      </c>
-      <c r="M23" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="N23" s="38" t="s">
-        <v>384</v>
-      </c>
-      <c r="O23" s="39" t="s">
-        <v>145</v>
       </c>
       <c r="P23" s="39">
         <v>14</v>
@@ -15053,19 +15065,19 @@
         <v>1</v>
       </c>
       <c r="Y23" s="39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="Z23" s="39" t="s">
         <v>88</v>
       </c>
       <c r="AA23" s="39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AB23" s="39" t="s">
         <v>88</v>
       </c>
       <c r="AC23" s="39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AD23" s="39">
         <v>279748</v>
@@ -15076,10 +15088,10 @@
       </c>
       <c r="AG23" s="39"/>
       <c r="AH23" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI23" s="38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AJ23" s="39"/>
       <c r="AK23" s="39"/>
@@ -16075,7 +16087,7 @@
         <v>1008</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C24" s="9">
         <v>2</v>
@@ -16084,7 +16096,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="13">
@@ -16098,19 +16110,19 @@
         <v>392702</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L24" s="20" t="s">
         <v>83</v>
       </c>
       <c r="M24" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N24" s="14" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="P24" s="13">
         <v>16</v>
@@ -16119,17 +16131,17 @@
         <v>17</v>
       </c>
       <c r="R24" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="S24" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="T24" s="13">
         <v>16</v>
       </c>
       <c r="U24" s="13"/>
       <c r="V24" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="W24" s="13">
         <v>254300</v>
@@ -16138,7 +16150,7 @@
         <v>1</v>
       </c>
       <c r="Y24" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Z24" s="13" t="s">
         <v>88</v>
@@ -16147,25 +16159,25 @@
         <v>89</v>
       </c>
       <c r="AB24" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AC24" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AD24" s="11">
         <v>285370</v>
       </c>
       <c r="AE24" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF24" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AG24" s="13">
         <v>1.5</v>
       </c>
       <c r="AH24" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI24" s="13"/>
       <c r="AJ24" s="13"/>
@@ -17162,7 +17174,7 @@
         <v>1009</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C25" s="9">
         <v>2</v>
@@ -17171,7 +17183,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F25" s="9">
         <v>7</v>
@@ -17193,13 +17205,13 @@
         <v>83</v>
       </c>
       <c r="M25" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="O25" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="P25" s="13">
         <v>18</v>
@@ -17211,7 +17223,7 @@
         <v>400</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="T25" s="13">
         <v>16</v>
@@ -17227,25 +17239,25 @@
         <v>1.3</v>
       </c>
       <c r="Y25" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Z25" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AA25" s="13" t="s">
         <v>89</v>
       </c>
       <c r="AB25" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AC25" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AD25" s="13">
         <v>146119</v>
       </c>
       <c r="AE25" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF25" s="13">
         <v>279672</v>
@@ -17254,10 +17266,10 @@
         <v>1.5</v>
       </c>
       <c r="AH25" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI25" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AJ25" s="13"/>
       <c r="AK25" s="13"/>
@@ -18253,7 +18265,7 @@
         <v>1010</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C26" s="9">
         <v>2</v>
@@ -18262,7 +18274,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="13">
@@ -18278,19 +18290,19 @@
         <v>392763</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L26" s="13" t="s">
         <v>83</v>
       </c>
       <c r="M26" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="O26" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P26" s="13">
         <v>18</v>
@@ -18302,7 +18314,7 @@
         <v>600</v>
       </c>
       <c r="S26" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="T26" s="13">
         <v>16</v>
@@ -18318,7 +18330,7 @@
         <v>1.5</v>
       </c>
       <c r="Y26" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Z26" s="13" t="s">
         <v>88</v>
@@ -18327,16 +18339,16 @@
         <v>89</v>
       </c>
       <c r="AB26" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AC26" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AD26" s="11">
         <v>144198</v>
       </c>
       <c r="AE26" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF26" s="13">
         <v>285283</v>
@@ -18345,7 +18357,7 @@
         <v>0.4</v>
       </c>
       <c r="AH26" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI26" s="13"/>
       <c r="AJ26" s="13"/>
@@ -19342,7 +19354,7 @@
         <v>1011</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C27" s="42">
         <v>2</v>
@@ -19351,7 +19363,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F27" s="42">
         <v>3</v>
@@ -19373,13 +19385,13 @@
         <v>83</v>
       </c>
       <c r="M27" s="46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N27" s="46" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="O27" s="44" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="P27" s="44">
         <v>18</v>
@@ -19391,7 +19403,7 @@
         <v>500</v>
       </c>
       <c r="S27" s="44" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T27" s="44">
         <v>16</v>
@@ -19407,10 +19419,10 @@
         <v>0.8</v>
       </c>
       <c r="Y27" s="44" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Z27" s="44" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AA27" s="44" t="s">
         <v>89</v>
@@ -19419,13 +19431,13 @@
         <v>88</v>
       </c>
       <c r="AC27" s="44" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AD27" s="44">
         <v>281886</v>
       </c>
       <c r="AE27" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF27" s="44">
         <v>281763</v>
@@ -19434,10 +19446,10 @@
         <v>1.5</v>
       </c>
       <c r="AH27" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI27" s="44" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AJ27" s="44"/>
       <c r="AK27" s="44"/>
@@ -20433,7 +20445,7 @@
         <v>1012</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28" s="22">
         <v>2</v>
@@ -20442,7 +20454,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="24">
@@ -20456,19 +20468,19 @@
         <v>392764</v>
       </c>
       <c r="K28" s="49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M28" s="30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N28" s="30" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="P28" s="24">
         <v>20</v>
@@ -20494,25 +20506,25 @@
         <v>1</v>
       </c>
       <c r="Y28" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Z28" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AA28" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AB28" s="25" t="s">
         <v>89</v>
       </c>
       <c r="AC28" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AD28" s="25">
         <v>144183</v>
       </c>
       <c r="AE28" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF28" s="25">
         <v>279686</v>
@@ -20521,7 +20533,7 @@
         <v>2.5</v>
       </c>
       <c r="AH28" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI28" s="25"/>
       <c r="AJ28" s="25"/>
@@ -21518,7 +21530,7 @@
         <v>1013</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C29" s="33">
         <v>2</v>
@@ -21527,7 +21539,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F29" s="39"/>
       <c r="G29" s="39">
@@ -21541,19 +21553,19 @@
         <v>392695</v>
       </c>
       <c r="K29" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="L29" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="M29" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="N29" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="O29" s="39" t="s">
         <v>192</v>
-      </c>
-      <c r="L29" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="M29" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="N29" s="38" t="s">
-        <v>390</v>
-      </c>
-      <c r="O29" s="39" t="s">
-        <v>194</v>
       </c>
       <c r="P29" s="39"/>
       <c r="Q29" s="39"/>
@@ -21569,19 +21581,19 @@
         <v>1</v>
       </c>
       <c r="Y29" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z29" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA29" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB29" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC29" s="39" t="s">
         <v>195</v>
-      </c>
-      <c r="Z29" s="39" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA29" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB29" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC29" s="39" t="s">
-        <v>197</v>
       </c>
       <c r="AD29" s="39">
         <v>285237</v>
@@ -21592,10 +21604,10 @@
       </c>
       <c r="AG29" s="39"/>
       <c r="AH29" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI29" s="38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AJ29" s="39"/>
       <c r="AK29" s="39"/>
@@ -22591,7 +22603,7 @@
         <v>1014</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C30" s="33">
         <v>2</v>
@@ -22600,7 +22612,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F30" s="39"/>
       <c r="G30" s="39">
@@ -22614,19 +22626,19 @@
         <v>392753</v>
       </c>
       <c r="K30" s="50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L30" s="39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M30" s="38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N30" s="38" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="O30" s="39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="P30" s="39"/>
       <c r="Q30" s="39"/>
@@ -22642,19 +22654,19 @@
         <v>1</v>
       </c>
       <c r="Y30" s="39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="Z30" s="39" t="s">
         <v>88</v>
       </c>
       <c r="AA30" s="39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AB30" s="39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AC30" s="39" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AD30" s="39">
         <v>285459</v>
@@ -22665,10 +22677,10 @@
       </c>
       <c r="AG30" s="39"/>
       <c r="AH30" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI30" s="38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AJ30" s="39"/>
       <c r="AK30" s="39"/>
@@ -23664,7 +23676,7 @@
         <v>1015</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C31" s="44">
         <v>3</v>
@@ -23673,7 +23685,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="44" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F31" s="44">
         <v>9</v>
@@ -23695,13 +23707,13 @@
         <v>83</v>
       </c>
       <c r="M31" s="44" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N31" s="44" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="O31" s="44" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P31" s="44">
         <v>22</v>
@@ -23713,14 +23725,14 @@
         <v>300</v>
       </c>
       <c r="S31" s="44" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="T31" s="44">
         <v>16</v>
       </c>
       <c r="U31" s="44"/>
       <c r="V31" s="44" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="W31" s="44">
         <v>151576</v>
@@ -23729,37 +23741,37 @@
         <v>1</v>
       </c>
       <c r="Y31" s="44" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Z31" s="44" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AA31" s="44" t="s">
         <v>89</v>
       </c>
       <c r="AB31" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC31" s="44" t="s">
-        <v>213</v>
+        <v>417</v>
       </c>
       <c r="AD31" s="44">
         <v>281788</v>
       </c>
       <c r="AE31" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF31" s="44" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AG31" s="44">
         <v>0.4</v>
       </c>
       <c r="AH31" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI31" s="44" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AJ31" s="44"/>
       <c r="AK31" s="44"/>
@@ -24755,7 +24767,7 @@
         <v>1016</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C32" s="44">
         <v>3</v>
@@ -24764,7 +24776,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="44" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F32" s="44">
         <v>7</v>
@@ -24786,13 +24798,13 @@
         <v>83</v>
       </c>
       <c r="M32" s="44" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="N32" s="44" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="O32" s="44" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="P32" s="44">
         <v>22</v>
@@ -24804,14 +24816,14 @@
         <v>200</v>
       </c>
       <c r="S32" s="44" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="T32" s="44">
         <v>16</v>
       </c>
       <c r="U32" s="44"/>
       <c r="V32" s="44" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="W32" s="44">
         <v>168944</v>
@@ -24820,37 +24832,37 @@
         <v>0.3</v>
       </c>
       <c r="Y32" s="44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z32" s="44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA32" s="44" t="s">
         <v>89</v>
       </c>
       <c r="AB32" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AC32" s="44" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AD32" s="44">
         <v>285400</v>
       </c>
       <c r="AE32" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF32" s="44" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AG32" s="44">
         <v>0.4</v>
       </c>
       <c r="AH32" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI32" s="44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AJ32" s="44"/>
       <c r="AK32" s="44"/>
@@ -25846,7 +25858,7 @@
         <v>1017</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C33" s="44">
         <v>3</v>
@@ -25855,7 +25867,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="44" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F33" s="44">
         <v>2</v>
@@ -25879,13 +25891,13 @@
         <v>83</v>
       </c>
       <c r="M33" s="44" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="N33" s="44" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="O33" s="44" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="P33" s="44">
         <v>22</v>
@@ -25897,7 +25909,7 @@
         <v>100</v>
       </c>
       <c r="S33" s="44" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="T33" s="44">
         <v>16</v>
@@ -25913,25 +25925,25 @@
         <v>1.2</v>
       </c>
       <c r="Y33" s="44" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="Z33" s="44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AA33" s="44" t="s">
         <v>89</v>
       </c>
       <c r="AB33" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC33" s="44" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="AD33" s="44">
         <v>281710</v>
       </c>
       <c r="AE33" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF33" s="44">
         <v>80483</v>
@@ -25940,7 +25952,7 @@
         <v>0.4</v>
       </c>
       <c r="AH33" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI33" s="44"/>
       <c r="AJ33" s="44"/>
@@ -26937,7 +26949,7 @@
         <v>1018</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C34" s="44">
         <v>3</v>
@@ -26946,7 +26958,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="44" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F34" s="44">
         <v>4</v>
@@ -26962,19 +26974,19 @@
         <v>392692</v>
       </c>
       <c r="K34" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L34" s="44" t="s">
         <v>83</v>
       </c>
       <c r="M34" s="44" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="N34" s="44" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="O34" s="44" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="P34" s="44">
         <v>22</v>
@@ -26983,17 +26995,17 @@
         <v>23</v>
       </c>
       <c r="R34" s="44" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="S34" s="44" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="T34" s="44">
         <v>16</v>
       </c>
       <c r="U34" s="44"/>
       <c r="V34" s="44" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="W34" s="44">
         <v>288335</v>
@@ -27002,37 +27014,37 @@
         <v>0.5</v>
       </c>
       <c r="Y34" s="44" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Z34" s="44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AA34" s="44" t="s">
         <v>89</v>
       </c>
       <c r="AB34" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AC34" s="44" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="AD34" s="44">
         <v>299561</v>
       </c>
       <c r="AE34" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF34" s="44" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="AG34" s="44">
         <v>2</v>
       </c>
       <c r="AH34" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI34" s="44" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="AJ34" s="44"/>
       <c r="AK34" s="44"/>
@@ -28028,7 +28040,7 @@
         <v>1019</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C35" s="44">
         <v>3</v>
@@ -28037,7 +28049,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="44" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F35" s="44"/>
       <c r="G35" s="44">
@@ -28051,19 +28063,19 @@
         <v>392697</v>
       </c>
       <c r="K35" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L35" s="44" t="s">
         <v>83</v>
       </c>
       <c r="M35" s="44" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="N35" s="44" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="O35" s="44" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="P35" s="44">
         <v>22</v>
@@ -28072,17 +28084,17 @@
         <v>23</v>
       </c>
       <c r="R35" s="44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S35" s="44" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="T35" s="44">
         <v>16</v>
       </c>
       <c r="U35" s="44"/>
       <c r="V35" s="44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="W35" s="44">
         <v>130642</v>
@@ -28091,34 +28103,34 @@
         <v>0.8</v>
       </c>
       <c r="Y35" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z35" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA35" s="44" t="s">
         <v>89</v>
       </c>
       <c r="AB35" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC35" s="44" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AD35" s="44">
         <v>285356</v>
       </c>
       <c r="AE35" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF35" s="44" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="AG35" s="44">
         <v>2</v>
       </c>
       <c r="AH35" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI35" s="44"/>
       <c r="AJ35" s="44"/>
@@ -29115,7 +29127,7 @@
         <v>1020</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C36" s="44">
         <v>3</v>
@@ -29124,7 +29136,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="44" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F36" s="44">
         <v>2</v>
@@ -29142,19 +29154,19 @@
         <v>392694</v>
       </c>
       <c r="K36" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L36" s="44" t="s">
         <v>83</v>
       </c>
       <c r="M36" s="44" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="N36" s="44" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="O36" s="44" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="P36" s="44">
         <v>22</v>
@@ -29163,17 +29175,17 @@
         <v>23</v>
       </c>
       <c r="R36" s="44" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="S36" s="44" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="T36" s="44">
         <v>16</v>
       </c>
       <c r="U36" s="44"/>
       <c r="V36" s="44" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="W36" s="44">
         <v>254276</v>
@@ -29182,7 +29194,7 @@
         <v>1</v>
       </c>
       <c r="Y36" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z36" s="44" t="s">
         <v>88</v>
@@ -29191,25 +29203,25 @@
         <v>89</v>
       </c>
       <c r="AB36" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC36" s="44" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AD36" s="44">
         <v>20301</v>
       </c>
       <c r="AE36" s="44" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="AF36" s="44" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AG36" s="44">
         <v>3</v>
       </c>
       <c r="AH36" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI36" s="44"/>
       <c r="AJ36" s="44"/>
@@ -30206,7 +30218,7 @@
         <v>1021</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C37" s="44">
         <v>4</v>
@@ -30215,7 +30227,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="44" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F37" s="44">
         <v>8</v>
@@ -30239,13 +30251,13 @@
         <v>83</v>
       </c>
       <c r="M37" s="44" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="N37" s="44" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="O37" s="44" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="P37" s="44">
         <v>24</v>
@@ -30257,7 +30269,7 @@
         <v>100</v>
       </c>
       <c r="S37" s="44" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="T37" s="44">
         <v>16</v>
@@ -30273,7 +30285,7 @@
         <v>1</v>
       </c>
       <c r="Y37" s="44" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="Z37" s="44" t="s">
         <v>88</v>
@@ -30282,16 +30294,16 @@
         <v>89</v>
       </c>
       <c r="AB37" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC37" s="44" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="AD37" s="44">
         <v>281710</v>
       </c>
       <c r="AE37" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF37" s="44">
         <v>80483</v>
@@ -30300,10 +30312,10 @@
         <v>0.4</v>
       </c>
       <c r="AH37" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI37" s="51" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="AJ37" s="44"/>
       <c r="AK37" s="44"/>
@@ -31299,7 +31311,7 @@
         <v>1022</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C38" s="44">
         <v>4</v>
@@ -31308,7 +31320,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="44" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F38" s="44">
         <v>4</v>
@@ -31330,13 +31342,13 @@
         <v>83</v>
       </c>
       <c r="M38" s="44" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="N38" s="44" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="O38" s="44" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="P38" s="44">
         <v>24</v>
@@ -31348,14 +31360,14 @@
         <v>200</v>
       </c>
       <c r="S38" s="44" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="T38" s="44">
         <v>16</v>
       </c>
       <c r="U38" s="44"/>
       <c r="V38" s="44" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="W38" s="44">
         <v>271321</v>
@@ -31364,7 +31376,7 @@
         <v>0.8</v>
       </c>
       <c r="Y38" s="44" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="Z38" s="44" t="s">
         <v>88</v>
@@ -31373,28 +31385,28 @@
         <v>89</v>
       </c>
       <c r="AB38" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AC38" s="44" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="AD38" s="44">
         <v>281871</v>
       </c>
       <c r="AE38" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF38" s="44" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="AG38" s="44">
         <v>1</v>
       </c>
       <c r="AH38" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI38" s="44" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AJ38" s="44"/>
       <c r="AK38" s="44"/>
@@ -32390,7 +32402,7 @@
         <v>1023</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C39" s="44">
         <v>4</v>
@@ -32399,7 +32411,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="44" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F39" s="44">
         <v>10</v>
@@ -32417,19 +32429,19 @@
         <v>392696</v>
       </c>
       <c r="K39" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L39" s="44" t="s">
         <v>83</v>
       </c>
       <c r="M39" s="44" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="N39" s="44" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="O39" s="44" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="P39" s="44">
         <v>24</v>
@@ -32441,7 +32453,7 @@
         <v>200</v>
       </c>
       <c r="S39" s="44" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="T39" s="44">
         <v>16</v>
@@ -32457,7 +32469,7 @@
         <v>1.5</v>
       </c>
       <c r="Y39" s="44" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="Z39" s="44" t="s">
         <v>88</v>
@@ -32466,16 +32478,16 @@
         <v>89</v>
       </c>
       <c r="AB39" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC39" s="44" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AD39" s="44">
         <v>300932</v>
       </c>
       <c r="AE39" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF39" s="44">
         <v>285208</v>
@@ -32484,10 +32496,10 @@
         <v>2</v>
       </c>
       <c r="AH39" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI39" s="44" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AJ39" s="44"/>
       <c r="AK39" s="44"/>
@@ -33483,7 +33495,7 @@
         <v>1024</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C40" s="44">
         <v>4</v>
@@ -33492,7 +33504,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="44" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F40" s="44"/>
       <c r="G40" s="44">
@@ -33506,19 +33518,19 @@
         <v>392703</v>
       </c>
       <c r="K40" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L40" s="44" t="s">
         <v>83</v>
       </c>
       <c r="M40" s="44" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="N40" s="44" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="O40" s="44" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="P40" s="44">
         <v>24</v>
@@ -33530,7 +33542,7 @@
         <v>300</v>
       </c>
       <c r="S40" s="44" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="T40" s="44">
         <v>16</v>
@@ -33546,7 +33558,7 @@
         <v>1.5</v>
       </c>
       <c r="Y40" s="44" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="Z40" s="44" t="s">
         <v>88</v>
@@ -33555,16 +33567,16 @@
         <v>89</v>
       </c>
       <c r="AB40" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC40" s="44" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="AD40" s="44">
         <v>117391</v>
       </c>
       <c r="AE40" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF40" s="44">
         <v>269275</v>
@@ -33573,7 +33585,7 @@
         <v>2</v>
       </c>
       <c r="AH40" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI40" s="44"/>
       <c r="AJ40" s="44"/>
@@ -34570,7 +34582,7 @@
         <v>1025</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C41" s="44">
         <v>4</v>
@@ -34579,7 +34591,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="44" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F41" s="44">
         <v>6</v>
@@ -34595,19 +34607,19 @@
         <v>392698</v>
       </c>
       <c r="K41" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L41" s="44" t="s">
         <v>83</v>
       </c>
       <c r="M41" s="44" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N41" s="44" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="O41" s="44" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="P41" s="44">
         <v>24</v>
@@ -34619,7 +34631,7 @@
         <v>100</v>
       </c>
       <c r="S41" s="44" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="T41" s="44">
         <v>16</v>
@@ -34638,22 +34650,22 @@
         <v>87</v>
       </c>
       <c r="Z41" s="44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AA41" s="44" t="s">
         <v>89</v>
       </c>
       <c r="AB41" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AC41" s="44" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="AD41" s="44">
         <v>285445</v>
       </c>
       <c r="AE41" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF41" s="52">
         <v>269223</v>
@@ -34662,10 +34674,10 @@
         <v>0.5</v>
       </c>
       <c r="AH41" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI41" s="44" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AJ41" s="44"/>
       <c r="AK41" s="44"/>
@@ -35661,7 +35673,7 @@
         <v>1026</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C42" s="39">
         <v>4</v>
@@ -35670,7 +35682,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F42" s="39"/>
       <c r="G42" s="39">
@@ -35684,19 +35696,19 @@
         <v>392705</v>
       </c>
       <c r="K42" s="50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L42" s="39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M42" s="38" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="N42" s="38" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="O42" s="39" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="P42" s="39">
         <v>24</v>
@@ -35716,19 +35728,19 @@
         <v>1</v>
       </c>
       <c r="Y42" s="39" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="Z42" s="39" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AA42" s="39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AB42" s="39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AC42" s="39" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="AD42" s="39">
         <v>94268</v>
@@ -35739,10 +35751,10 @@
       </c>
       <c r="AG42" s="39"/>
       <c r="AH42" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI42" s="38" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AJ42" s="39"/>
       <c r="AK42" s="39"/>
@@ -36738,7 +36750,7 @@
         <v>1027</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C43" s="13">
         <v>5</v>
@@ -36747,7 +36759,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F43" s="13"/>
       <c r="G43" s="13">
@@ -36767,13 +36779,13 @@
         <v>83</v>
       </c>
       <c r="M43" s="13" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="N43" s="13" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="O43" s="13" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="P43" s="13">
         <v>26</v>
@@ -36785,7 +36797,7 @@
         <v>100</v>
       </c>
       <c r="S43" s="13" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="T43" s="13">
         <v>16</v>
@@ -36808,16 +36820,16 @@
         <v>89</v>
       </c>
       <c r="AB43" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC43" s="13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="AD43" s="13">
         <v>279765</v>
       </c>
       <c r="AE43" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF43" s="13">
         <v>303167</v>
@@ -36826,10 +36838,10 @@
         <v>0.5</v>
       </c>
       <c r="AH43" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI43" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AJ43" s="13"/>
       <c r="AK43" s="13"/>
@@ -37825,7 +37837,7 @@
         <v>1028</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C44" s="13">
         <v>5</v>
@@ -37834,7 +37846,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F44" s="13"/>
       <c r="G44" s="13">
@@ -37848,19 +37860,19 @@
         <v>392708</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L44" s="13" t="s">
         <v>83</v>
       </c>
       <c r="M44" s="13" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="N44" s="13" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="O44" s="13" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="P44" s="13">
         <v>44</v>
@@ -37872,7 +37884,7 @@
         <v>100</v>
       </c>
       <c r="S44" s="13" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="T44" s="13">
         <v>16</v>
@@ -37888,7 +37900,7 @@
         <v>1.4</v>
       </c>
       <c r="Y44" s="13" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="Z44" s="13" t="s">
         <v>88</v>
@@ -37897,16 +37909,16 @@
         <v>89</v>
       </c>
       <c r="AB44" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC44" s="13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AD44" s="13">
         <v>85944</v>
       </c>
       <c r="AE44" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF44" s="21">
         <v>29747</v>
@@ -37915,7 +37927,7 @@
         <v>0.5</v>
       </c>
       <c r="AH44" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI44" s="13"/>
       <c r="AJ44" s="13"/>
@@ -38912,7 +38924,7 @@
         <v>1029</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C45" s="13">
         <v>5</v>
@@ -38921,7 +38933,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F45" s="13">
         <v>3</v>
@@ -38937,19 +38949,19 @@
         <v>392716</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L45" s="13" t="s">
         <v>83</v>
       </c>
       <c r="M45" s="13" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="N45" s="13" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="O45" s="13" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="P45" s="13">
         <v>46</v>
@@ -38961,7 +38973,7 @@
         <v>400</v>
       </c>
       <c r="S45" s="13" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="T45" s="13">
         <v>16</v>
@@ -38977,25 +38989,25 @@
         <v>1</v>
       </c>
       <c r="Y45" s="13" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="Z45" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AA45" s="13" t="s">
         <v>89</v>
       </c>
       <c r="AB45" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC45" s="13" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="AD45" s="13">
         <v>326802</v>
       </c>
       <c r="AE45" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF45" s="13">
         <v>279685</v>
@@ -39004,10 +39016,10 @@
         <v>0.8</v>
       </c>
       <c r="AH45" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI45" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AJ45" s="13"/>
       <c r="AK45" s="13"/>
@@ -40003,7 +40015,7 @@
         <v>1030</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C46" s="13">
         <v>5</v>
@@ -40012,7 +40024,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F46" s="13">
         <v>6</v>
@@ -40028,19 +40040,19 @@
         <v>392717</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L46" s="13" t="s">
         <v>83</v>
       </c>
       <c r="M46" s="13" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N46" s="13" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="O46" s="13" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="P46" s="13">
         <v>48</v>
@@ -40050,7 +40062,7 @@
       </c>
       <c r="R46" s="13"/>
       <c r="S46" s="13" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="T46" s="13">
         <v>16</v>
@@ -40066,10 +40078,10 @@
         <v>1</v>
       </c>
       <c r="Y46" s="13" t="s">
-        <v>322</v>
+        <v>420</v>
       </c>
       <c r="Z46" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA46" s="13" t="s">
         <v>89</v>
@@ -40078,13 +40090,13 @@
         <v>88</v>
       </c>
       <c r="AC46" s="13" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="AD46" s="13">
         <v>281871</v>
       </c>
       <c r="AE46" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF46" s="13">
         <v>268572</v>
@@ -40093,10 +40105,10 @@
         <v>0.7</v>
       </c>
       <c r="AH46" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI46" s="44" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AJ46" s="13"/>
       <c r="AK46" s="13"/>
@@ -41092,7 +41104,7 @@
         <v>1031</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C47" s="25">
         <v>5</v>
@@ -41101,7 +41113,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F47" s="25"/>
       <c r="G47" s="25">
@@ -41115,19 +41127,19 @@
         <v>392712</v>
       </c>
       <c r="K47" s="49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L47" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M47" s="25" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="O47" s="25" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="P47" s="25">
         <v>40</v>
@@ -41139,7 +41151,7 @@
         <v>1000</v>
       </c>
       <c r="S47" s="25" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="T47" s="25">
         <v>16</v>
@@ -41165,13 +41177,13 @@
         <v>88</v>
       </c>
       <c r="AC47" s="25" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="AD47" s="25">
         <v>285673</v>
       </c>
       <c r="AE47" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF47" s="25">
         <v>268686</v>
@@ -41180,7 +41192,7 @@
         <v>1</v>
       </c>
       <c r="AH47" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI47" s="25"/>
       <c r="AJ47" s="25"/>
@@ -42177,7 +42189,7 @@
         <v>1032</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C48" s="22">
         <v>5</v>
@@ -42186,7 +42198,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="24">
@@ -42200,19 +42212,19 @@
         <v>392711</v>
       </c>
       <c r="K48" s="49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L48" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M48" s="25" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="N48" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="O48" s="25" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="P48" s="24">
         <v>42</v>
@@ -42236,7 +42248,7 @@
         <v>1</v>
       </c>
       <c r="Y48" s="25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Z48" s="25" t="s">
         <v>88</v>
@@ -42248,13 +42260,13 @@
         <v>88</v>
       </c>
       <c r="AC48" s="25" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AD48" s="25">
         <v>144183</v>
       </c>
       <c r="AE48" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF48" s="25">
         <v>20270</v>
@@ -42263,7 +42275,7 @@
         <v>1.8</v>
       </c>
       <c r="AH48" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI48" s="25"/>
       <c r="AJ48" s="25"/>
@@ -43260,7 +43272,7 @@
         <v>1033</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C49" s="13">
         <v>6</v>
@@ -43269,7 +43281,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F49" s="13">
         <v>5</v>
@@ -43291,13 +43303,13 @@
         <v>83</v>
       </c>
       <c r="M49" s="13" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="N49" s="13" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="P49" s="13">
         <v>28</v>
@@ -43309,7 +43321,7 @@
         <v>350</v>
       </c>
       <c r="S49" s="13" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="T49" s="13">
         <v>16</v>
@@ -43325,25 +43337,25 @@
         <v>1.5</v>
       </c>
       <c r="Y49" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Z49" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AA49" s="13" t="s">
         <v>89</v>
       </c>
       <c r="AB49" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC49" s="13" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="AD49" s="13">
         <v>303259</v>
       </c>
       <c r="AE49" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF49" s="13">
         <v>303247</v>
@@ -43352,10 +43364,10 @@
         <v>1.5</v>
       </c>
       <c r="AH49" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI49" s="13" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="AJ49" s="13"/>
       <c r="AK49" s="13"/>
@@ -44351,7 +44363,7 @@
         <v>1034</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C50" s="13">
         <v>6</v>
@@ -44360,7 +44372,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="13">
@@ -44374,19 +44386,19 @@
         <v>392713</v>
       </c>
       <c r="K50" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L50" s="13" t="s">
         <v>83</v>
       </c>
       <c r="M50" s="13" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="N50" s="13" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="O50" s="13" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="P50" s="13">
         <v>30</v>
@@ -44398,7 +44410,7 @@
         <v>650</v>
       </c>
       <c r="S50" s="13" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="T50" s="13">
         <v>16</v>
@@ -44414,10 +44426,10 @@
         <v>1</v>
       </c>
       <c r="Y50" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Z50" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AA50" s="13" t="s">
         <v>89</v>
@@ -44426,13 +44438,13 @@
         <v>88</v>
       </c>
       <c r="AC50" s="13" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="AD50" s="13">
         <v>305224</v>
       </c>
       <c r="AE50" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF50" s="13">
         <v>284893</v>
@@ -44441,7 +44453,7 @@
         <v>1.3</v>
       </c>
       <c r="AH50" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI50" s="13"/>
       <c r="AJ50" s="13"/>
@@ -45438,7 +45450,7 @@
         <v>1035</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C51" s="13">
         <v>6</v>
@@ -45447,7 +45459,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F51" s="13">
         <v>3</v>
@@ -45463,19 +45475,19 @@
         <v>392707</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L51" s="13" t="s">
         <v>83</v>
       </c>
       <c r="M51" s="13" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="N51" s="13" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="O51" s="13" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="P51" s="13">
         <v>32</v>
@@ -45487,7 +45499,7 @@
         <v>1000</v>
       </c>
       <c r="S51" s="13" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="T51" s="13">
         <v>16</v>
@@ -45503,7 +45515,7 @@
         <v>1</v>
       </c>
       <c r="Y51" s="13" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Z51" s="13" t="s">
         <v>88</v>
@@ -45512,16 +45524,16 @@
         <v>89</v>
       </c>
       <c r="AB51" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC51" s="13" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="AD51" s="13">
         <v>269209</v>
       </c>
       <c r="AE51" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF51" s="13">
         <v>268704</v>
@@ -45530,10 +45542,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AH51" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI51" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AJ51" s="13"/>
       <c r="AK51" s="13"/>
@@ -46529,7 +46541,7 @@
         <v>1036</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C52" s="13">
         <v>6</v>
@@ -46538,7 +46550,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F52" s="13">
         <v>6</v>
@@ -46560,13 +46572,13 @@
         <v>83</v>
       </c>
       <c r="M52" s="13" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="N52" s="13" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="O52" s="13" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="P52" s="13">
         <v>38</v>
@@ -46578,7 +46590,7 @@
         <v>500</v>
       </c>
       <c r="S52" s="13" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="T52" s="13">
         <v>16</v>
@@ -46594,25 +46606,25 @@
         <v>1</v>
       </c>
       <c r="Y52" s="13" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="Z52" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA52" s="13" t="s">
         <v>89</v>
       </c>
       <c r="AB52" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC52" s="13" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="AD52" s="13">
         <v>144183</v>
       </c>
       <c r="AE52" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF52" s="13">
         <v>279726</v>
@@ -46621,10 +46633,10 @@
         <v>1</v>
       </c>
       <c r="AH52" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI52" s="13" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AJ52" s="13"/>
       <c r="AK52" s="13"/>
@@ -47620,7 +47632,7 @@
         <v>1037</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C53" s="13">
         <v>6</v>
@@ -47629,7 +47641,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F53" s="13"/>
       <c r="G53" s="13">
@@ -47639,25 +47651,25 @@
         <v>1</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J53" s="13">
         <v>392714</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L53" s="13" t="s">
         <v>83</v>
       </c>
       <c r="M53" s="13" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="N53" s="13" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="O53" s="13" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="P53" s="13">
         <v>34</v>
@@ -47667,7 +47679,7 @@
       </c>
       <c r="R53" s="13"/>
       <c r="S53" s="13" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="T53" s="13">
         <v>16</v>
@@ -47681,25 +47693,25 @@
         <v>2</v>
       </c>
       <c r="Y53" s="13" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="Z53" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA53" s="13" t="s">
         <v>89</v>
       </c>
       <c r="AB53" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC53" s="13" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="AD53" s="13">
         <v>281795</v>
       </c>
       <c r="AE53" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF53" s="13">
         <v>81687</v>
@@ -47708,7 +47720,7 @@
         <v>1</v>
       </c>
       <c r="AH53" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI53" s="15"/>
       <c r="AJ53" s="13"/>
@@ -48705,7 +48717,7 @@
         <v>1038</v>
       </c>
       <c r="B54" s="54" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C54" s="55">
         <v>6</v>
@@ -48714,7 +48726,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="55" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F54" s="55"/>
       <c r="G54" s="56">
@@ -48724,25 +48736,25 @@
         <v>3</v>
       </c>
       <c r="I54" s="55" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J54" s="55">
         <v>392715</v>
       </c>
       <c r="K54" s="57" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="L54" s="55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M54" s="58" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="N54" s="58" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="O54" s="55" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="P54" s="55">
         <v>36</v>
@@ -48764,25 +48776,25 @@
         <v>1</v>
       </c>
       <c r="Y54" s="55" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="Z54" s="55" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AA54" s="55" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AB54" s="55" t="s">
         <v>89</v>
       </c>
       <c r="AC54" s="55" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AD54" s="55">
         <v>144183</v>
       </c>
       <c r="AE54" s="55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF54" s="55">
         <v>20270</v>
@@ -48791,10 +48803,10 @@
         <v>1</v>
       </c>
       <c r="AH54" s="55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI54" s="58" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AJ54" s="55"/>
       <c r="AK54" s="55"/>

</xml_diff>

<commit_message>
feat: update Tower & StageCoing
调整百分比攻击塔配置和世界3 5关卡配置
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E8E1F0-54B9-4697-9A62-6C5BE4DE3B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1097C548-377C-46C4-82CB-B03BFB108462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -700,16 +700,10 @@
     <t>Tower_attackTags_9|Tower_attackTags_10</t>
   </si>
   <si>
-    <t>200|400|600</t>
-  </si>
-  <si>
     <t>2413BE794DFD89225C6BB1984BF3B39A|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
   </si>
   <si>
     <t>2|2|2</t>
-  </si>
-  <si>
-    <t>30|40|50</t>
   </si>
   <si>
     <t>4026||4027||4028</t>
@@ -719,9 +713,6 @@
   </si>
   <si>
     <t>黑曜</t>
-  </si>
-  <si>
-    <t>250|400|550</t>
   </si>
   <si>
     <t>4E3FA2424F946AAFD47668983B3506B9|E718B09E4408CE5534779780E5365B64|E456238842ACC53D8C01EAABD11B256C</t>
@@ -1272,9 +1263,6 @@
     <t>112|272|496</t>
   </si>
   <si>
-    <t>160|480|960</t>
-  </si>
-  <si>
     <t>200|520|960</t>
   </si>
   <si>
@@ -1455,6 +1443,22 @@
     Stealth = 1,
     Flying = 2,
 Armored = 3</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>40|50|60</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>250|400|550</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>140|35|35</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>112|140|168</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1952,10 +1956,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="L49" sqref="L49"/>
+      <selection pane="topRight" activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -2273,7 +2277,7 @@
         <v>50</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>51</v>
@@ -8533,7 +8537,7 @@
         <v>83</v>
       </c>
       <c r="N17" s="44" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="O17" s="43" t="s">
         <v>84</v>
@@ -8562,7 +8566,7 @@
         <v>0.3</v>
       </c>
       <c r="Y17" s="43" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="Z17" s="43" t="s">
         <v>87</v>
@@ -8574,7 +8578,7 @@
         <v>87</v>
       </c>
       <c r="AC17" s="43" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="AD17" s="43">
         <v>144183</v>
@@ -9618,7 +9622,7 @@
         <v>93</v>
       </c>
       <c r="N18" s="45" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="O18" s="43" t="s">
         <v>94</v>
@@ -10709,7 +10713,7 @@
         <v>102</v>
       </c>
       <c r="N19" s="45" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="O19" s="43" t="s">
         <v>103</v>
@@ -10752,7 +10756,7 @@
         <v>108</v>
       </c>
       <c r="AC19" s="43" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AD19" s="43">
         <v>144183</v>
@@ -11800,7 +11804,7 @@
         <v>112</v>
       </c>
       <c r="N20" s="45" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="O20" s="43" t="s">
         <v>113</v>
@@ -11843,7 +11847,7 @@
         <v>117</v>
       </c>
       <c r="AC20" s="43" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="AD20" s="43">
         <v>144183</v>
@@ -12886,10 +12890,10 @@
         <v>123</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>124</v>
@@ -13974,7 +13978,7 @@
         <v>132</v>
       </c>
       <c r="N22" s="45" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="O22" s="43" t="s">
         <v>133</v>
@@ -15058,10 +15062,10 @@
         <v>139</v>
       </c>
       <c r="M23" s="34" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="N23" s="35" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="O23" s="36" t="s">
         <v>140</v>
@@ -15086,7 +15090,7 @@
         <v>1</v>
       </c>
       <c r="Y23" s="36" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="Z23" s="36" t="s">
         <v>87</v>
@@ -15098,7 +15102,7 @@
         <v>87</v>
       </c>
       <c r="AC23" s="36" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AD23" s="36">
         <v>279748</v>
@@ -16140,7 +16144,7 @@
         <v>145</v>
       </c>
       <c r="N24" s="44" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="O24" s="43" t="s">
         <v>146</v>
@@ -17229,7 +17233,7 @@
         <v>154</v>
       </c>
       <c r="N25" s="45" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="O25" s="43" t="s">
         <v>155</v>
@@ -18320,7 +18324,7 @@
         <v>164</v>
       </c>
       <c r="N26" s="45" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="O26" s="43" t="s">
         <v>165</v>
@@ -19409,7 +19413,7 @@
         <v>171</v>
       </c>
       <c r="N27" s="57" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="O27" s="55" t="s">
         <v>172</v>
@@ -20495,10 +20499,10 @@
         <v>123</v>
       </c>
       <c r="M28" s="17" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="O28" s="12" t="s">
         <v>180</v>
@@ -21580,13 +21584,13 @@
         <v>139</v>
       </c>
       <c r="M29" s="35" t="s">
+        <v>416</v>
+      </c>
+      <c r="N29" s="35" t="s">
+        <v>417</v>
+      </c>
+      <c r="O29" s="36" t="s">
         <v>186</v>
-      </c>
-      <c r="N29" s="35" t="s">
-        <v>367</v>
-      </c>
-      <c r="O29" s="36" t="s">
-        <v>187</v>
       </c>
       <c r="P29" s="36"/>
       <c r="Q29" s="36"/>
@@ -21602,10 +21606,10 @@
         <v>1</v>
       </c>
       <c r="Y29" s="36" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="Z29" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA29" s="36" t="s">
         <v>127</v>
@@ -21614,7 +21618,7 @@
         <v>87</v>
       </c>
       <c r="AC29" s="36" t="s">
-        <v>189</v>
+        <v>414</v>
       </c>
       <c r="AD29" s="36">
         <v>285237</v>
@@ -21628,7 +21632,7 @@
         <v>99</v>
       </c>
       <c r="AI29" s="35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AJ29" s="36"/>
       <c r="AK29" s="36"/>
@@ -22624,7 +22628,7 @@
         <v>1014</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C30" s="29">
         <v>2</v>
@@ -22633,7 +22637,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F30" s="36"/>
       <c r="G30" s="36">
@@ -22653,13 +22657,13 @@
         <v>139</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>193</v>
+        <v>415</v>
       </c>
       <c r="N30" s="35" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O30" s="36" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="P30" s="36"/>
       <c r="Q30" s="36"/>
@@ -22675,7 +22679,7 @@
         <v>1</v>
       </c>
       <c r="Y30" s="36" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="Z30" s="36" t="s">
         <v>87</v>
@@ -22687,7 +22691,7 @@
         <v>87</v>
       </c>
       <c r="AC30" s="36" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AD30" s="36">
         <v>285459</v>
@@ -22701,7 +22705,7 @@
         <v>99</v>
       </c>
       <c r="AI30" s="35" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AJ30" s="36"/>
       <c r="AK30" s="36"/>
@@ -23697,7 +23701,7 @@
         <v>1015</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C31" s="55">
         <v>3</v>
@@ -23706,7 +23710,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F31" s="55">
         <v>9</v>
@@ -23728,13 +23732,13 @@
         <v>82</v>
       </c>
       <c r="M31" s="55" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N31" s="55" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="O31" s="55" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="P31" s="55">
         <v>22</v>
@@ -23746,14 +23750,14 @@
         <v>300</v>
       </c>
       <c r="S31" s="55" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="T31" s="55">
         <v>16</v>
       </c>
       <c r="U31" s="55"/>
       <c r="V31" s="55" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="W31" s="55">
         <v>151576</v>
@@ -23762,10 +23766,10 @@
         <v>1</v>
       </c>
       <c r="Y31" s="55" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="Z31" s="55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA31" s="55" t="s">
         <v>88</v>
@@ -23774,7 +23778,7 @@
         <v>97</v>
       </c>
       <c r="AC31" s="55" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="AD31" s="55">
         <v>281788</v>
@@ -23783,7 +23787,7 @@
         <v>89</v>
       </c>
       <c r="AF31" s="55" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AG31" s="55">
         <v>0.4</v>
@@ -23792,7 +23796,7 @@
         <v>99</v>
       </c>
       <c r="AI31" s="55" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AJ31" s="55"/>
       <c r="AK31" s="55"/>
@@ -24788,7 +24792,7 @@
         <v>1016</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C32" s="55">
         <v>3</v>
@@ -24797,7 +24801,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="55" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F32" s="55">
         <v>7</v>
@@ -24819,13 +24823,13 @@
         <v>82</v>
       </c>
       <c r="M32" s="55" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="N32" s="55" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="O32" s="55" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="P32" s="55">
         <v>22</v>
@@ -24837,14 +24841,14 @@
         <v>200</v>
       </c>
       <c r="S32" s="55" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="T32" s="55">
         <v>16</v>
       </c>
       <c r="U32" s="55"/>
       <c r="V32" s="55" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="W32" s="55">
         <v>168944</v>
@@ -24865,7 +24869,7 @@
         <v>157</v>
       </c>
       <c r="AC32" s="55" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AD32" s="55">
         <v>285400</v>
@@ -24874,7 +24878,7 @@
         <v>89</v>
       </c>
       <c r="AF32" s="55" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AG32" s="55">
         <v>0.4</v>
@@ -25879,7 +25883,7 @@
         <v>1017</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C33" s="55">
         <v>3</v>
@@ -25888,7 +25892,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="55" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F33" s="55">
         <v>2</v>
@@ -25912,13 +25916,13 @@
         <v>82</v>
       </c>
       <c r="M33" s="55" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="N33" s="55" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="O33" s="55" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P33" s="55">
         <v>22</v>
@@ -25930,7 +25934,7 @@
         <v>100</v>
       </c>
       <c r="S33" s="55" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="T33" s="55">
         <v>16</v>
@@ -25946,7 +25950,7 @@
         <v>1.2</v>
       </c>
       <c r="Y33" s="55" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="Z33" s="55" t="s">
         <v>141</v>
@@ -25958,7 +25962,7 @@
         <v>97</v>
       </c>
       <c r="AC33" s="55" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="AD33" s="55">
         <v>281710</v>
@@ -26970,7 +26974,7 @@
         <v>1018</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C34" s="55">
         <v>3</v>
@@ -26979,7 +26983,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="55" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F34" s="55">
         <v>4</v>
@@ -27001,13 +27005,13 @@
         <v>82</v>
       </c>
       <c r="M34" s="55" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="N34" s="55" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="O34" s="55" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P34" s="55">
         <v>22</v>
@@ -27016,17 +27020,17 @@
         <v>23</v>
       </c>
       <c r="R34" s="55" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S34" s="55" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="T34" s="55">
         <v>16</v>
       </c>
       <c r="U34" s="55"/>
       <c r="V34" s="55" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W34" s="55">
         <v>288335</v>
@@ -27035,7 +27039,7 @@
         <v>0.5</v>
       </c>
       <c r="Y34" s="55" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Z34" s="55" t="s">
         <v>125</v>
@@ -27047,7 +27051,7 @@
         <v>157</v>
       </c>
       <c r="AC34" s="55" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AD34" s="55">
         <v>299561</v>
@@ -27056,7 +27060,7 @@
         <v>89</v>
       </c>
       <c r="AF34" s="55" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AG34" s="55">
         <v>2</v>
@@ -27065,7 +27069,7 @@
         <v>99</v>
       </c>
       <c r="AI34" s="55" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="AJ34" s="55"/>
       <c r="AK34" s="55"/>
@@ -28061,7 +28065,7 @@
         <v>1019</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C35" s="55">
         <v>3</v>
@@ -28070,7 +28074,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="55" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F35" s="55"/>
       <c r="G35" s="55">
@@ -28090,13 +28094,13 @@
         <v>82</v>
       </c>
       <c r="M35" s="55" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="N35" s="55" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="O35" s="55" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="P35" s="55">
         <v>22</v>
@@ -28108,7 +28112,7 @@
         <v>114</v>
       </c>
       <c r="S35" s="55" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="T35" s="55">
         <v>16</v>
@@ -28136,7 +28140,7 @@
         <v>97</v>
       </c>
       <c r="AC35" s="55" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="AD35" s="55">
         <v>285356</v>
@@ -28145,7 +28149,7 @@
         <v>89</v>
       </c>
       <c r="AF35" s="55" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="AG35" s="55">
         <v>2</v>
@@ -29148,7 +29152,7 @@
         <v>1020</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C36" s="55">
         <v>3</v>
@@ -29157,7 +29161,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="55" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F36" s="55">
         <v>2</v>
@@ -29181,13 +29185,13 @@
         <v>82</v>
       </c>
       <c r="M36" s="55" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N36" s="55" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="O36" s="55" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="P36" s="55">
         <v>22</v>
@@ -29196,17 +29200,17 @@
         <v>23</v>
       </c>
       <c r="R36" s="55" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="S36" s="55" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="T36" s="55">
         <v>16</v>
       </c>
       <c r="U36" s="55"/>
       <c r="V36" s="55" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="W36" s="55">
         <v>254276</v>
@@ -29227,16 +29231,16 @@
         <v>97</v>
       </c>
       <c r="AC36" s="55" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="AD36" s="55">
         <v>20301</v>
       </c>
       <c r="AE36" s="55" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="AF36" s="55" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AG36" s="55">
         <v>3</v>
@@ -30239,7 +30243,7 @@
         <v>1021</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C37" s="55">
         <v>4</v>
@@ -30248,7 +30252,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F37" s="55">
         <v>8</v>
@@ -30272,13 +30276,13 @@
         <v>82</v>
       </c>
       <c r="M37" s="55" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N37" s="55" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="O37" s="55" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="P37" s="55">
         <v>24</v>
@@ -30290,7 +30294,7 @@
         <v>100</v>
       </c>
       <c r="S37" s="55" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="T37" s="55">
         <v>16</v>
@@ -30306,7 +30310,7 @@
         <v>1</v>
       </c>
       <c r="Y37" s="55" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="Z37" s="55" t="s">
         <v>87</v>
@@ -30318,7 +30322,7 @@
         <v>107</v>
       </c>
       <c r="AC37" s="55" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AD37" s="55">
         <v>281710</v>
@@ -30336,7 +30340,7 @@
         <v>99</v>
       </c>
       <c r="AI37" s="60" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="AJ37" s="55"/>
       <c r="AK37" s="55"/>
@@ -31332,7 +31336,7 @@
         <v>1022</v>
       </c>
       <c r="B38" s="52" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C38" s="55">
         <v>4</v>
@@ -31341,7 +31345,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F38" s="55">
         <v>4</v>
@@ -31363,13 +31367,13 @@
         <v>82</v>
       </c>
       <c r="M38" s="55" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="N38" s="55" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="O38" s="55" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P38" s="55">
         <v>24</v>
@@ -31381,14 +31385,14 @@
         <v>200</v>
       </c>
       <c r="S38" s="55" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="T38" s="55">
         <v>16</v>
       </c>
       <c r="U38" s="55"/>
       <c r="V38" s="55" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="W38" s="55">
         <v>271321</v>
@@ -31397,7 +31401,7 @@
         <v>0.8</v>
       </c>
       <c r="Y38" s="55" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Z38" s="55" t="s">
         <v>87</v>
@@ -31409,7 +31413,7 @@
         <v>157</v>
       </c>
       <c r="AC38" s="55" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="AD38" s="55">
         <v>281871</v>
@@ -31418,7 +31422,7 @@
         <v>89</v>
       </c>
       <c r="AF38" s="55" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="AG38" s="55">
         <v>1</v>
@@ -31427,7 +31431,7 @@
         <v>99</v>
       </c>
       <c r="AI38" s="55" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="AJ38" s="55"/>
       <c r="AK38" s="55"/>
@@ -32423,7 +32427,7 @@
         <v>1023</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C39" s="55">
         <v>4</v>
@@ -32432,7 +32436,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F39" s="55">
         <v>10</v>
@@ -32456,13 +32460,13 @@
         <v>82</v>
       </c>
       <c r="M39" s="55" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="N39" s="55" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="O39" s="55" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="P39" s="55">
         <v>24</v>
@@ -32474,7 +32478,7 @@
         <v>200</v>
       </c>
       <c r="S39" s="55" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="T39" s="55">
         <v>16</v>
@@ -32490,7 +32494,7 @@
         <v>1.5</v>
       </c>
       <c r="Y39" s="55" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="Z39" s="55" t="s">
         <v>87</v>
@@ -32502,7 +32506,7 @@
         <v>97</v>
       </c>
       <c r="AC39" s="55" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="AD39" s="55">
         <v>300932</v>
@@ -32520,7 +32524,7 @@
         <v>99</v>
       </c>
       <c r="AI39" s="55" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="AJ39" s="55"/>
       <c r="AK39" s="55"/>
@@ -33516,7 +33520,7 @@
         <v>1024</v>
       </c>
       <c r="B40" s="52" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C40" s="55">
         <v>4</v>
@@ -33525,7 +33529,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F40" s="55"/>
       <c r="G40" s="55">
@@ -33545,13 +33549,13 @@
         <v>82</v>
       </c>
       <c r="M40" s="55" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="N40" s="55" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="O40" s="55" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="P40" s="55">
         <v>24</v>
@@ -33563,7 +33567,7 @@
         <v>300</v>
       </c>
       <c r="S40" s="55" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="T40" s="55">
         <v>16</v>
@@ -33579,7 +33583,7 @@
         <v>1.5</v>
       </c>
       <c r="Y40" s="55" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="Z40" s="55" t="s">
         <v>87</v>
@@ -33591,7 +33595,7 @@
         <v>97</v>
       </c>
       <c r="AC40" s="55" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="AD40" s="55">
         <v>117391</v>
@@ -34603,7 +34607,7 @@
         <v>1025</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C41" s="55">
         <v>4</v>
@@ -34612,7 +34616,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="55" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F41" s="55">
         <v>6</v>
@@ -34634,13 +34638,13 @@
         <v>82</v>
       </c>
       <c r="M41" s="55" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N41" s="55" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="O41" s="55" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="P41" s="55">
         <v>24</v>
@@ -34652,7 +34656,7 @@
         <v>100</v>
       </c>
       <c r="S41" s="55" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="T41" s="55">
         <v>16</v>
@@ -34680,7 +34684,7 @@
         <v>157</v>
       </c>
       <c r="AC41" s="55" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="AD41" s="55">
         <v>285445</v>
@@ -34698,7 +34702,7 @@
         <v>99</v>
       </c>
       <c r="AI41" s="55" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AJ41" s="55"/>
       <c r="AK41" s="55"/>
@@ -35694,7 +35698,7 @@
         <v>1026</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C42" s="36">
         <v>4</v>
@@ -35703,7 +35707,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F42" s="36"/>
       <c r="G42" s="36">
@@ -35723,13 +35727,13 @@
         <v>139</v>
       </c>
       <c r="M42" s="35" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="N42" s="35" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="O42" s="36" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="P42" s="36">
         <v>24</v>
@@ -35749,10 +35753,10 @@
         <v>1</v>
       </c>
       <c r="Y42" s="36" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="Z42" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA42" s="36" t="s">
         <v>127</v>
@@ -35761,7 +35765,7 @@
         <v>87</v>
       </c>
       <c r="AC42" s="36" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AD42" s="36">
         <v>94268</v>
@@ -35775,7 +35779,7 @@
         <v>99</v>
       </c>
       <c r="AI42" s="35" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="AJ42" s="36"/>
       <c r="AK42" s="36"/>
@@ -36771,7 +36775,7 @@
         <v>1027</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C43" s="43">
         <v>5</v>
@@ -36780,7 +36784,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="43" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F43" s="43"/>
       <c r="G43" s="43">
@@ -36800,13 +36804,13 @@
         <v>82</v>
       </c>
       <c r="M43" s="43" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N43" s="43" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="O43" s="43" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="P43" s="43">
         <v>26</v>
@@ -36818,7 +36822,7 @@
         <v>100</v>
       </c>
       <c r="S43" s="43" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="T43" s="43">
         <v>16</v>
@@ -36844,7 +36848,7 @@
         <v>107</v>
       </c>
       <c r="AC43" s="43" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="AD43" s="43">
         <v>279765</v>
@@ -37858,7 +37862,7 @@
         <v>1028</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C44" s="43">
         <v>5</v>
@@ -37867,7 +37871,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="43" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F44" s="43"/>
       <c r="G44" s="43">
@@ -37887,13 +37891,13 @@
         <v>82</v>
       </c>
       <c r="M44" s="43" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="N44" s="43" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="O44" s="43" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="P44" s="43">
         <v>44</v>
@@ -37905,7 +37909,7 @@
         <v>100</v>
       </c>
       <c r="S44" s="43" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="T44" s="43">
         <v>16</v>
@@ -37921,7 +37925,7 @@
         <v>1.4</v>
       </c>
       <c r="Y44" s="43" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="Z44" s="43" t="s">
         <v>87</v>
@@ -38945,7 +38949,7 @@
         <v>1029</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C45" s="43">
         <v>5</v>
@@ -38954,7 +38958,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="43" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F45" s="43">
         <v>3</v>
@@ -38976,13 +38980,13 @@
         <v>82</v>
       </c>
       <c r="M45" s="43" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="N45" s="43" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="O45" s="43" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="P45" s="43">
         <v>46</v>
@@ -38994,7 +38998,7 @@
         <v>400</v>
       </c>
       <c r="S45" s="43" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="T45" s="43">
         <v>16</v>
@@ -39010,10 +39014,10 @@
         <v>1</v>
       </c>
       <c r="Y45" s="43" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="Z45" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA45" s="43" t="s">
         <v>88</v>
@@ -39022,7 +39026,7 @@
         <v>97</v>
       </c>
       <c r="AC45" s="43" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="AD45" s="43">
         <v>326802</v>
@@ -40036,7 +40040,7 @@
         <v>1030</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C46" s="43">
         <v>5</v>
@@ -40045,7 +40049,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="43" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F46" s="43">
         <v>6</v>
@@ -40067,13 +40071,13 @@
         <v>82</v>
       </c>
       <c r="M46" s="43" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="N46" s="43" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="O46" s="43" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="P46" s="43">
         <v>48</v>
@@ -40083,7 +40087,7 @@
       </c>
       <c r="R46" s="43"/>
       <c r="S46" s="43" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="T46" s="43">
         <v>16</v>
@@ -40099,7 +40103,7 @@
         <v>1</v>
       </c>
       <c r="Y46" s="43" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="Z46" s="43" t="s">
         <v>107</v>
@@ -40111,7 +40115,7 @@
         <v>87</v>
       </c>
       <c r="AC46" s="43" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="AD46" s="43">
         <v>281871</v>
@@ -40129,7 +40133,7 @@
         <v>99</v>
       </c>
       <c r="AI46" s="55" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AJ46" s="43"/>
       <c r="AK46" s="43"/>
@@ -41125,7 +41129,7 @@
         <v>1031</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C47" s="12">
         <v>5</v>
@@ -41134,7 +41138,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12">
@@ -41154,13 +41158,13 @@
         <v>123</v>
       </c>
       <c r="M47" s="12" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="O47" s="12" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="P47" s="12">
         <v>40</v>
@@ -41172,7 +41176,7 @@
         <v>1000</v>
       </c>
       <c r="S47" s="12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="T47" s="12">
         <v>16</v>
@@ -41198,7 +41202,7 @@
         <v>87</v>
       </c>
       <c r="AC47" s="12" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="AD47" s="12">
         <v>285673</v>
@@ -42210,7 +42214,7 @@
         <v>1032</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C48" s="9">
         <v>5</v>
@@ -42219,7 +42223,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="11">
@@ -42239,13 +42243,13 @@
         <v>123</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="N48" s="12" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="O48" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="P48" s="11">
         <v>42</v>
@@ -42281,7 +42285,7 @@
         <v>87</v>
       </c>
       <c r="AC48" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="AD48" s="12">
         <v>144183</v>
@@ -43293,7 +43297,7 @@
         <v>1033</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C49" s="43">
         <v>6</v>
@@ -43302,7 +43306,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="43" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F49" s="43">
         <v>5</v>
@@ -43324,13 +43328,13 @@
         <v>82</v>
       </c>
       <c r="M49" s="43" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="N49" s="43" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="O49" s="43" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="P49" s="43">
         <v>28</v>
@@ -43342,7 +43346,7 @@
         <v>350</v>
       </c>
       <c r="S49" s="43" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="T49" s="43">
         <v>16</v>
@@ -43358,10 +43362,10 @@
         <v>1.5</v>
       </c>
       <c r="Y49" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Z49" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA49" s="43" t="s">
         <v>88</v>
@@ -43370,7 +43374,7 @@
         <v>97</v>
       </c>
       <c r="AC49" s="43" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AD49" s="43">
         <v>303259</v>
@@ -43388,7 +43392,7 @@
         <v>99</v>
       </c>
       <c r="AI49" s="43" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="AJ49" s="43"/>
       <c r="AK49" s="43"/>
@@ -44384,7 +44388,7 @@
         <v>1034</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C50" s="43">
         <v>6</v>
@@ -44393,7 +44397,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F50" s="43"/>
       <c r="G50" s="43">
@@ -44413,13 +44417,13 @@
         <v>82</v>
       </c>
       <c r="M50" s="43" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="N50" s="43" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="O50" s="43" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P50" s="43">
         <v>30</v>
@@ -44431,7 +44435,7 @@
         <v>650</v>
       </c>
       <c r="S50" s="43" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="T50" s="43">
         <v>16</v>
@@ -44447,7 +44451,7 @@
         <v>1</v>
       </c>
       <c r="Y50" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Z50" s="43" t="s">
         <v>158</v>
@@ -44459,7 +44463,7 @@
         <v>87</v>
       </c>
       <c r="AC50" s="43" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="AD50" s="43">
         <v>305224</v>
@@ -45471,7 +45475,7 @@
         <v>1035</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C51" s="43">
         <v>6</v>
@@ -45480,7 +45484,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F51" s="43">
         <v>3</v>
@@ -45502,13 +45506,13 @@
         <v>82</v>
       </c>
       <c r="M51" s="43" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="N51" s="43" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="O51" s="43" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="P51" s="43">
         <v>32</v>
@@ -45520,7 +45524,7 @@
         <v>1000</v>
       </c>
       <c r="S51" s="43" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="T51" s="43">
         <v>16</v>
@@ -45536,7 +45540,7 @@
         <v>1</v>
       </c>
       <c r="Y51" s="43" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="Z51" s="43" t="s">
         <v>87</v>
@@ -45548,7 +45552,7 @@
         <v>107</v>
       </c>
       <c r="AC51" s="43" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="AD51" s="43">
         <v>269209</v>
@@ -46562,7 +46566,7 @@
         <v>1036</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C52" s="43">
         <v>6</v>
@@ -46571,7 +46575,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="43" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F52" s="43">
         <v>6</v>
@@ -46593,13 +46597,13 @@
         <v>82</v>
       </c>
       <c r="M52" s="43" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="N52" s="43" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="O52" s="43" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="P52" s="43">
         <v>38</v>
@@ -46611,7 +46615,7 @@
         <v>500</v>
       </c>
       <c r="S52" s="43" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="T52" s="43">
         <v>16</v>
@@ -46627,7 +46631,7 @@
         <v>1</v>
       </c>
       <c r="Y52" s="43" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="Z52" s="43" t="s">
         <v>107</v>
@@ -46639,7 +46643,7 @@
         <v>97</v>
       </c>
       <c r="AC52" s="43" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="AD52" s="43">
         <v>144183</v>
@@ -46657,7 +46661,7 @@
         <v>99</v>
       </c>
       <c r="AI52" s="43" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AJ52" s="43"/>
       <c r="AK52" s="43"/>
@@ -47653,7 +47657,7 @@
         <v>1037</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C53" s="43">
         <v>6</v>
@@ -47662,7 +47666,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F53" s="43"/>
       <c r="G53" s="43">
@@ -47684,13 +47688,13 @@
         <v>82</v>
       </c>
       <c r="M53" s="43" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N53" s="43" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="O53" s="43" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="P53" s="43">
         <v>34</v>
@@ -47700,7 +47704,7 @@
       </c>
       <c r="R53" s="43"/>
       <c r="S53" s="43" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="T53" s="43">
         <v>16</v>
@@ -47714,7 +47718,7 @@
         <v>2</v>
       </c>
       <c r="Y53" s="43" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="Z53" s="43" t="s">
         <v>97</v>
@@ -47726,7 +47730,7 @@
         <v>97</v>
       </c>
       <c r="AC53" s="43" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="AD53" s="43">
         <v>281795</v>
@@ -48738,7 +48742,7 @@
         <v>1038</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C54" s="22">
         <v>6</v>
@@ -48747,7 +48751,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="23">
@@ -48761,19 +48765,19 @@
         <v>392715</v>
       </c>
       <c r="K54" s="24" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="L54" s="22" t="s">
         <v>123</v>
       </c>
       <c r="M54" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="N54" s="25" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="O54" s="22" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="P54" s="22">
         <v>36</v>
@@ -48795,7 +48799,7 @@
         <v>1</v>
       </c>
       <c r="Y54" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="Z54" s="22" t="s">
         <v>126</v>
@@ -48807,7 +48811,7 @@
         <v>88</v>
       </c>
       <c r="AC54" s="22" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="AD54" s="22">
         <v>144183</v>

</xml_diff>

<commit_message>
feat: update 041branch diff
同步041分支改动
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Tower_塔表.xlsx
+++ b/nevergiveup/Excel/Tower_塔表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\editor_v0.40.0.2.20241015185135\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA1ED73-4F9A-4767-A382-95D115D20462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90729BFC-0260-4223-82D8-D519860CCCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2008,9 +2008,9 @@
   <dimension ref="A1:AMJ54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="AJ26" sqref="AJ26"/>
+      <selection pane="topRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -8586,7 +8586,9 @@
       <c r="E17" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="39"/>
+      <c r="F17" s="39">
+        <v>4</v>
+      </c>
       <c r="G17" s="41">
         <v>1000</v>
       </c>

</xml_diff>